<commit_message>
Update dqc_0001 and dqc_0015 xlsx files
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="277">
   <si>
     <t>Rule element ID</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Limited</t>
   </si>
   <si>
-    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member</t>
-  </si>
-  <si>
     <t>DQC_0001.52</t>
   </si>
   <si>
@@ -907,6 +904,12 @@
   </si>
   <si>
     <t>NotDesignatedAsHedgingInstrumentEconomicHedgesMember, NotDesignatedAsHedgingInstrumentTradingMember</t>
+  </si>
+  <si>
+    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, InvestmentsNetAssetValueMember</t>
+  </si>
+  <si>
+    <t>InvestmentsNetAssetValueMember</t>
   </si>
 </sst>
 </file>
@@ -1335,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1420,22 +1423,22 @@
         <v>14</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>15</v>
+        <v>275</v>
       </c>
       <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>13</v>
@@ -1443,26 +1446,26 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -1474,25 +1477,25 @@
     </row>
     <row r="5" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>13</v>
@@ -1502,19 +1505,19 @@
     </row>
     <row r="6" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -1526,19 +1529,19 @@
     </row>
     <row r="7" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1551,23 +1554,23 @@
     </row>
     <row r="8" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>13</v>
@@ -1587,19 +1590,19 @@
     </row>
     <row r="9" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -1612,19 +1615,19 @@
     </row>
     <row r="10" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="E10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -1637,16 +1640,16 @@
     </row>
     <row r="11" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>13</v>
@@ -1657,23 +1660,23 @@
         <v>14</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>13</v>
@@ -1684,23 +1687,23 @@
         <v>14</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>13</v>
@@ -1708,7 +1711,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -1716,16 +1719,16 @@
     </row>
     <row r="14" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>13</v>
@@ -1733,24 +1736,26 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>276</v>
+      </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>13</v>
@@ -1761,32 +1766,32 @@
         <v>14</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>13</v>
@@ -1797,16 +1802,16 @@
     </row>
     <row r="17" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>13</v>
@@ -1817,29 +1822,29 @@
         <v>14</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6" t="s">
@@ -1851,19 +1856,19 @@
     </row>
     <row r="19" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="E19" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -1876,16 +1881,16 @@
     </row>
     <row r="20" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>13</v>
@@ -1893,7 +1898,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
@@ -1901,23 +1906,23 @@
     </row>
     <row r="21" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>13</v>
@@ -1928,16 +1933,16 @@
     </row>
     <row r="22" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>13</v>
@@ -1953,16 +1958,16 @@
     </row>
     <row r="23" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>13</v>
@@ -1970,7 +1975,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
@@ -2037,7 +2042,7 @@
     </row>
     <row r="28" spans="1:29" s="7" customFormat="1" ht="16.5">
       <c r="A28" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -2070,7 +2075,7 @@
     </row>
     <row r="29" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10" t="s">
@@ -2080,228 +2085,228 @@
         <v>1</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A30" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A43" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="45" spans="1:5" s="7" customFormat="1" ht="16.5">
       <c r="A45" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A46" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10" t="s">
@@ -2311,137 +2316,137 @@
         <v>1</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>141</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A49" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B49" s="15"/>
       <c r="C49" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A50" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A51" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="D51" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A52" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="D52" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A53" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="D53" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A54" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="D54" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E54" s="8" t="s">
         <v>162</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A55" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="D55" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E55" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="7" customFormat="1" ht="16.5">
@@ -2449,12 +2454,12 @@
     </row>
     <row r="57" spans="1:5" s="7" customFormat="1" ht="16.5">
       <c r="A57" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A58" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
@@ -2464,405 +2469,405 @@
         <v>1</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A60" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A61" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A62" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A63" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A64" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A65" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A66" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B66" s="6"/>
       <c r="C66" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A67" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B67" s="6"/>
       <c r="C67" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A68" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A69" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="6" t="s">
         <v>199</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A70" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B70" s="6"/>
       <c r="C70" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A71" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B71" s="6"/>
       <c r="C71" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A72" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B72" s="6"/>
       <c r="C72" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>208</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A73" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A74" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A75" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B75" s="6"/>
       <c r="C75" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A76" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B76" s="6"/>
       <c r="C76" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A77" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B77" s="6"/>
       <c r="C77" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A78" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B78" s="6"/>
       <c r="C78" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="6" t="s">
         <v>226</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A79" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B79" s="6"/>
       <c r="C79" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>229</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A80" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B80" s="6"/>
       <c r="C80" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="6" t="s">
         <v>232</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="81" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A81" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B81" s="6"/>
       <c r="C81" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="82" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A82" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="D82" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="8" t="s">
         <v>238</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="83" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A83" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="D83" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="8" t="s">
         <v>241</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A84" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="D84" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" s="8" t="s">
         <v>244</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="85" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="86" spans="1:29" s="7" customFormat="1" ht="16.5">
       <c r="A86" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A87" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B87" s="10"/>
       <c r="C87" s="10" t="s">
@@ -2872,7 +2877,7 @@
         <v>1</v>
       </c>
       <c r="E87" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
@@ -2901,17 +2906,17 @@
     </row>
     <row r="88" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A88" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B88" s="6"/>
       <c r="C88" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E88" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>249</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
@@ -2940,17 +2945,17 @@
     </row>
     <row r="89" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A89" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E89" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>252</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
@@ -2979,17 +2984,17 @@
     </row>
     <row r="90" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A90" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E90" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>255</v>
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
@@ -3018,17 +3023,17 @@
     </row>
     <row r="91" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A91" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B91" s="6"/>
       <c r="C91" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E91" s="6" t="s">
         <v>257</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>258</v>
       </c>
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
@@ -3057,17 +3062,17 @@
     </row>
     <row r="92" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A92" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E92" s="6" t="s">
         <v>260</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>261</v>
       </c>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
@@ -3127,7 +3132,7 @@
     </row>
     <row r="94" spans="1:29" s="7" customFormat="1" ht="16.5">
       <c r="A94" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -3160,7 +3165,7 @@
     </row>
     <row r="95" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A95" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" s="10"/>
       <c r="C95" s="10" t="s">
@@ -3170,7 +3175,7 @@
         <v>1</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
@@ -3199,64 +3204,65 @@
     </row>
     <row r="96" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A96" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="C96" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="C96" s="6" t="s">
+      <c r="D96" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E96" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="97" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A97" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C97" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="D97" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E97" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A98" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C98" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="D98" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E98" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A99" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="C99" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="D99" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="8" t="s">
         <v>273</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A1:K99"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update dqc_0011 list of axes.xlsx
add automobile member
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7320" windowWidth="23340" windowHeight="9405"/>
+    <workbookView xWindow="3180" yWindow="0" windowWidth="12600" windowHeight="22350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$100</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="280">
   <si>
     <t>Rule element ID</t>
   </si>
@@ -910,13 +910,22 @@
   </si>
   <si>
     <t>InvestmentsNetAssetValueMember</t>
+  </si>
+  <si>
+    <t>AutomobilesMember</t>
+  </si>
+  <si>
+    <t>Automobiles [Member]</t>
+  </si>
+  <si>
+    <t>Vehicles that are used primarily for transporting people.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -968,6 +977,15 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1025,7 +1043,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1042,6 +1060,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1336,10 +1357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC100"/>
+  <dimension ref="A1:AC101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2859,64 +2880,39 @@
         <v>244</v>
       </c>
     </row>
-    <row r="85" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="86" spans="1:29" s="7" customFormat="1" ht="16.5">
-      <c r="A86" s="9" t="s">
+    <row r="85" spans="1:29" s="17" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A85" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="87" spans="1:29" s="7" customFormat="1" ht="16.5">
+      <c r="A87" s="9" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="87" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A87" s="10" t="s">
+    <row r="88" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A88" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B87" s="10"/>
-      <c r="C87" s="10" t="s">
+      <c r="B88" s="10"/>
+      <c r="C88" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D87" s="10" t="s">
+      <c r="D88" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E87" s="10" t="s">
+      <c r="E88" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="F87" s="6"/>
-      <c r="G87" s="6"/>
-      <c r="H87" s="6"/>
-      <c r="I87" s="6"/>
-      <c r="J87" s="6"/>
-      <c r="K87" s="6"/>
-      <c r="L87" s="6"/>
-      <c r="M87" s="6"/>
-      <c r="N87" s="6"/>
-      <c r="O87" s="6"/>
-      <c r="P87" s="6"/>
-      <c r="Q87" s="6"/>
-      <c r="R87" s="6"/>
-      <c r="S87" s="6"/>
-      <c r="T87" s="6"/>
-      <c r="U87" s="6"/>
-      <c r="V87" s="6"/>
-      <c r="W87" s="6"/>
-      <c r="X87" s="6"/>
-      <c r="Y87" s="6"/>
-      <c r="Z87" s="6"/>
-      <c r="AA87" s="6"/>
-      <c r="AB87" s="6"/>
-      <c r="AC87" s="6"/>
-    </row>
-    <row r="88" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A88" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B88" s="6"/>
-      <c r="C88" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
@@ -2945,17 +2941,17 @@
     </row>
     <row r="89" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A89" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="6" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>140</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
@@ -2984,17 +2980,17 @@
     </row>
     <row r="90" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A90" s="6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>140</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
@@ -3023,17 +3019,17 @@
     </row>
     <row r="91" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A91" s="6" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B91" s="6"/>
       <c r="C91" s="6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>140</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
@@ -3062,17 +3058,17 @@
     </row>
     <row r="92" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A92" s="6" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>140</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
@@ -3100,11 +3096,19 @@
       <c r="AC92" s="6"/>
     </row>
     <row r="93" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A93" s="6"/>
+      <c r="A93" s="6" t="s">
+        <v>258</v>
+      </c>
       <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
+      <c r="C93" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>260</v>
+      </c>
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
       <c r="H93" s="6"/>
@@ -3130,10 +3134,8 @@
       <c r="AB93" s="6"/>
       <c r="AC93" s="6"/>
     </row>
-    <row r="94" spans="1:29" s="7" customFormat="1" ht="16.5">
-      <c r="A94" s="9" t="s">
-        <v>261</v>
-      </c>
+    <row r="94" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
@@ -3163,20 +3165,14 @@
       <c r="AB94" s="6"/>
       <c r="AC94" s="6"/>
     </row>
-    <row r="95" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A95" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B95" s="10"/>
-      <c r="C95" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D95" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>94</v>
-      </c>
+    <row r="95" spans="1:29" s="7" customFormat="1" ht="16.5">
+      <c r="A95" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
       <c r="H95" s="6"/>
@@ -3203,64 +3199,103 @@
       <c r="AC95" s="6"/>
     </row>
     <row r="96" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A96" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>264</v>
-      </c>
+      <c r="A96" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
+      <c r="O96" s="6"/>
+      <c r="P96" s="6"/>
+      <c r="Q96" s="6"/>
+      <c r="R96" s="6"/>
+      <c r="S96" s="6"/>
+      <c r="T96" s="6"/>
+      <c r="U96" s="6"/>
+      <c r="V96" s="6"/>
+      <c r="W96" s="6"/>
+      <c r="X96" s="6"/>
+      <c r="Y96" s="6"/>
+      <c r="Z96" s="6"/>
+      <c r="AA96" s="6"/>
+      <c r="AB96" s="6"/>
+      <c r="AC96" s="6"/>
     </row>
     <row r="97" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A97" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A98" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A99" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A100" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="C100" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="D99" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" s="8" t="s">
+      <c r="D100" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="101" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:K99"/>
+  <autoFilter ref="A1:K100"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Update master with DQC-approved code and documentation for version 4   (#272)
Changes to v.4.0.0 from public exposure (#270)
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7320" windowWidth="23340" windowHeight="9405"/>
+    <workbookView xWindow="3180" yWindow="0" windowWidth="12600" windowHeight="22350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$100</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="280">
   <si>
     <t>Rule element ID</t>
   </si>
@@ -910,13 +910,22 @@
   </si>
   <si>
     <t>InvestmentsNetAssetValueMember</t>
+  </si>
+  <si>
+    <t>AutomobilesMember</t>
+  </si>
+  <si>
+    <t>Automobiles [Member]</t>
+  </si>
+  <si>
+    <t>Vehicles that are used primarily for transporting people.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -968,6 +977,15 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1025,7 +1043,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1042,6 +1060,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1336,10 +1357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC100"/>
+  <dimension ref="A1:AC101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2859,64 +2880,39 @@
         <v>244</v>
       </c>
     </row>
-    <row r="85" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="86" spans="1:29" s="7" customFormat="1" ht="16.5">
-      <c r="A86" s="9" t="s">
+    <row r="85" spans="1:29" s="17" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A85" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="87" spans="1:29" s="7" customFormat="1" ht="16.5">
+      <c r="A87" s="9" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="87" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A87" s="10" t="s">
+    <row r="88" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A88" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B87" s="10"/>
-      <c r="C87" s="10" t="s">
+      <c r="B88" s="10"/>
+      <c r="C88" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D87" s="10" t="s">
+      <c r="D88" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E87" s="10" t="s">
+      <c r="E88" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="F87" s="6"/>
-      <c r="G87" s="6"/>
-      <c r="H87" s="6"/>
-      <c r="I87" s="6"/>
-      <c r="J87" s="6"/>
-      <c r="K87" s="6"/>
-      <c r="L87" s="6"/>
-      <c r="M87" s="6"/>
-      <c r="N87" s="6"/>
-      <c r="O87" s="6"/>
-      <c r="P87" s="6"/>
-      <c r="Q87" s="6"/>
-      <c r="R87" s="6"/>
-      <c r="S87" s="6"/>
-      <c r="T87" s="6"/>
-      <c r="U87" s="6"/>
-      <c r="V87" s="6"/>
-      <c r="W87" s="6"/>
-      <c r="X87" s="6"/>
-      <c r="Y87" s="6"/>
-      <c r="Z87" s="6"/>
-      <c r="AA87" s="6"/>
-      <c r="AB87" s="6"/>
-      <c r="AC87" s="6"/>
-    </row>
-    <row r="88" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A88" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B88" s="6"/>
-      <c r="C88" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
@@ -2945,17 +2941,17 @@
     </row>
     <row r="89" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A89" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="6" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>140</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
@@ -2984,17 +2980,17 @@
     </row>
     <row r="90" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A90" s="6" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>140</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
@@ -3023,17 +3019,17 @@
     </row>
     <row r="91" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A91" s="6" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B91" s="6"/>
       <c r="C91" s="6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>140</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
@@ -3062,17 +3058,17 @@
     </row>
     <row r="92" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A92" s="6" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>140</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
@@ -3100,11 +3096,19 @@
       <c r="AC92" s="6"/>
     </row>
     <row r="93" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A93" s="6"/>
+      <c r="A93" s="6" t="s">
+        <v>258</v>
+      </c>
       <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
+      <c r="C93" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>260</v>
+      </c>
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
       <c r="H93" s="6"/>
@@ -3130,10 +3134,8 @@
       <c r="AB93" s="6"/>
       <c r="AC93" s="6"/>
     </row>
-    <row r="94" spans="1:29" s="7" customFormat="1" ht="16.5">
-      <c r="A94" s="9" t="s">
-        <v>261</v>
-      </c>
+    <row r="94" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
@@ -3163,20 +3165,14 @@
       <c r="AB94" s="6"/>
       <c r="AC94" s="6"/>
     </row>
-    <row r="95" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A95" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B95" s="10"/>
-      <c r="C95" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D95" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>94</v>
-      </c>
+    <row r="95" spans="1:29" s="7" customFormat="1" ht="16.5">
+      <c r="A95" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
       <c r="H95" s="6"/>
@@ -3203,64 +3199,103 @@
       <c r="AC95" s="6"/>
     </row>
     <row r="96" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A96" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>264</v>
-      </c>
+      <c r="A96" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
+      <c r="O96" s="6"/>
+      <c r="P96" s="6"/>
+      <c r="Q96" s="6"/>
+      <c r="R96" s="6"/>
+      <c r="S96" s="6"/>
+      <c r="T96" s="6"/>
+      <c r="U96" s="6"/>
+      <c r="V96" s="6"/>
+      <c r="W96" s="6"/>
+      <c r="X96" s="6"/>
+      <c r="Y96" s="6"/>
+      <c r="Z96" s="6"/>
+      <c r="AA96" s="6"/>
+      <c r="AB96" s="6"/>
+      <c r="AC96" s="6"/>
     </row>
     <row r="97" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A97" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A98" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A99" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="8" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A100" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="C100" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="D99" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" s="8" t="s">
+      <c r="D100" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="101" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:K99"/>
+  <autoFilter ref="A1:K100"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
update DQC_0001 List of Axes .xlsx
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -306,9 +306,6 @@
     <t>Defined Benefit Plan, Asset Categories [Axis]</t>
   </si>
   <si>
-    <t>All - except members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis</t>
-  </si>
-  <si>
     <t>DQC_0001.72</t>
   </si>
   <si>
@@ -906,9 +903,6 @@
     <t>NotDesignatedAsHedgingInstrumentEconomicHedgesMember, NotDesignatedAsHedgingInstrumentTradingMember</t>
   </si>
   <si>
-    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, InvestmentsNetAssetValueMember</t>
-  </si>
-  <si>
     <t>InvestmentsNetAssetValueMember</t>
   </si>
   <si>
@@ -919,6 +913,12 @@
   </si>
   <si>
     <t>Vehicles that are used primarily for transporting people.</t>
+  </si>
+  <si>
+    <t>ALL but no members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis</t>
+  </si>
+  <si>
+    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3, MemberFairValueMeasuredAtNetAssetValuePerShareMember</t>
   </si>
 </sst>
 </file>
@@ -1359,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1444,7 +1444,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="J2" s="6"/>
     </row>
@@ -1757,10 +1757,10 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -1787,7 +1787,7 @@
         <v>14</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -1865,7 +1865,7 @@
         <v>13</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>75</v>
+        <v>278</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6" t="s">
@@ -1877,16 +1877,16 @@
     </row>
     <row r="19" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>22</v>
@@ -1902,16 +1902,16 @@
     </row>
     <row r="20" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>13</v>
@@ -1927,23 +1927,23 @@
     </row>
     <row r="21" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>13</v>
@@ -1954,16 +1954,16 @@
     </row>
     <row r="22" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>13</v>
@@ -1979,16 +1979,16 @@
     </row>
     <row r="23" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>13</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="28" spans="1:29" s="7" customFormat="1" ht="16.5">
       <c r="A28" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -2096,7 +2096,7 @@
     </row>
     <row r="29" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10" t="s">
@@ -2106,228 +2106,228 @@
         <v>1</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A30" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A43" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="45" spans="1:5" s="7" customFormat="1" ht="16.5">
       <c r="A45" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A46" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10" t="s">
@@ -2337,137 +2337,137 @@
         <v>1</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A49" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B49" s="15"/>
       <c r="C49" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A50" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A51" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="D51" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A52" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="D52" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A53" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="D53" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E53" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A54" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="D54" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E54" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A55" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="D55" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E55" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="7" customFormat="1" ht="16.5">
@@ -2475,12 +2475,12 @@
     </row>
     <row r="57" spans="1:5" s="7" customFormat="1" ht="16.5">
       <c r="A57" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A58" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
@@ -2490,419 +2490,419 @@
         <v>1</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A60" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A61" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A62" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A63" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A64" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A65" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A66" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B66" s="6"/>
       <c r="C66" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A67" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B67" s="6"/>
       <c r="C67" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A68" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A69" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A70" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B70" s="6"/>
       <c r="C70" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A71" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B71" s="6"/>
       <c r="C71" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>204</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A72" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B72" s="6"/>
       <c r="C72" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A73" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A74" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="6" t="s">
         <v>213</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A75" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B75" s="6"/>
       <c r="C75" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="6" t="s">
         <v>216</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A76" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B76" s="6"/>
       <c r="C76" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A77" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B77" s="6"/>
       <c r="C77" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A78" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B78" s="6"/>
       <c r="C78" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A79" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B79" s="6"/>
       <c r="C79" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>228</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A80" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B80" s="6"/>
       <c r="C80" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="81" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A81" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B81" s="6"/>
       <c r="C81" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="6" t="s">
         <v>234</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="82" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A82" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="D82" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="8" t="s">
         <v>237</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="83" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A83" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="D83" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A84" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="D84" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:29" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A85" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="18" t="s">
         <v>277</v>
-      </c>
-      <c r="C85" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="D85" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E85" s="18" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="86" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="87" spans="1:29" s="7" customFormat="1" ht="16.5">
       <c r="A87" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A88" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B88" s="10"/>
       <c r="C88" s="10" t="s">
@@ -2912,7 +2912,7 @@
         <v>1</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
@@ -2941,17 +2941,17 @@
     </row>
     <row r="89" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A89" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E89" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
@@ -2980,17 +2980,17 @@
     </row>
     <row r="90" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A90" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E90" s="6" t="s">
         <v>250</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>251</v>
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
@@ -3019,17 +3019,17 @@
     </row>
     <row r="91" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A91" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B91" s="6"/>
       <c r="C91" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E91" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>254</v>
       </c>
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
@@ -3058,17 +3058,17 @@
     </row>
     <row r="92" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A92" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E92" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>257</v>
       </c>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
@@ -3097,17 +3097,17 @@
     </row>
     <row r="93" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A93" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B93" s="6"/>
       <c r="C93" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E93" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>260</v>
       </c>
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
@@ -3167,7 +3167,7 @@
     </row>
     <row r="95" spans="1:29" s="7" customFormat="1" ht="16.5">
       <c r="A95" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="96" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A96" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="10" t="s">
@@ -3210,7 +3210,7 @@
         <v>1</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
@@ -3239,58 +3239,58 @@
     </row>
     <row r="97" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A97" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C97" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="D97" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E97" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A98" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C98" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="D98" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E98" s="8" t="s">
         <v>266</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A99" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="C99" s="6" t="s">
+      <c r="D99" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="8" t="s">
         <v>269</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A100" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C100" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="D100" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>272</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update test suite and rule documentation (#298)
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="0" windowWidth="12600" windowHeight="22350"/>
+    <workbookView xWindow="2730" yWindow="870" windowWidth="23280" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -306,9 +306,6 @@
     <t>Defined Benefit Plan, Asset Categories [Axis]</t>
   </si>
   <si>
-    <t>All - except members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis</t>
-  </si>
-  <si>
     <t>DQC_0001.72</t>
   </si>
   <si>
@@ -906,9 +903,6 @@
     <t>NotDesignatedAsHedgingInstrumentEconomicHedgesMember, NotDesignatedAsHedgingInstrumentTradingMember</t>
   </si>
   <si>
-    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, InvestmentsNetAssetValueMember</t>
-  </si>
-  <si>
     <t>InvestmentsNetAssetValueMember</t>
   </si>
   <si>
@@ -919,6 +913,12 @@
   </si>
   <si>
     <t>Vehicles that are used primarily for transporting people.</t>
+  </si>
+  <si>
+    <t>ALL but no members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis</t>
+  </si>
+  <si>
+    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, FairValueMeasuredAtNetAssetValuePerShareMember</t>
   </si>
 </sst>
 </file>
@@ -1359,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1444,7 +1444,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="J2" s="6"/>
     </row>
@@ -1757,10 +1757,10 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -1787,7 +1787,7 @@
         <v>14</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -1865,7 +1865,7 @@
         <v>13</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>75</v>
+        <v>278</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6" t="s">
@@ -1877,16 +1877,16 @@
     </row>
     <row r="19" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>22</v>
@@ -1902,16 +1902,16 @@
     </row>
     <row r="20" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>13</v>
@@ -1927,23 +1927,23 @@
     </row>
     <row r="21" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>13</v>
@@ -1954,16 +1954,16 @@
     </row>
     <row r="22" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>13</v>
@@ -1979,16 +1979,16 @@
     </row>
     <row r="23" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>13</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="28" spans="1:29" s="7" customFormat="1" ht="16.5">
       <c r="A28" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -2096,7 +2096,7 @@
     </row>
     <row r="29" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10" t="s">
@@ -2106,228 +2106,228 @@
         <v>1</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A30" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A43" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="45" spans="1:5" s="7" customFormat="1" ht="16.5">
       <c r="A45" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A46" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10" t="s">
@@ -2337,137 +2337,137 @@
         <v>1</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A49" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B49" s="15"/>
       <c r="C49" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A50" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A51" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="D51" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A52" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="D52" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A53" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="D53" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E53" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A54" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="D54" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E54" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A55" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="D55" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E55" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="7" customFormat="1" ht="16.5">
@@ -2475,12 +2475,12 @@
     </row>
     <row r="57" spans="1:5" s="7" customFormat="1" ht="16.5">
       <c r="A57" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A58" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
@@ -2490,419 +2490,419 @@
         <v>1</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A60" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A61" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A62" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A63" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A64" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A65" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A66" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B66" s="6"/>
       <c r="C66" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A67" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B67" s="6"/>
       <c r="C67" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A68" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A69" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A70" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B70" s="6"/>
       <c r="C70" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A71" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B71" s="6"/>
       <c r="C71" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>204</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A72" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B72" s="6"/>
       <c r="C72" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A73" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A74" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="6" t="s">
         <v>213</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A75" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B75" s="6"/>
       <c r="C75" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="6" t="s">
         <v>216</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A76" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B76" s="6"/>
       <c r="C76" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A77" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B77" s="6"/>
       <c r="C77" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A78" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B78" s="6"/>
       <c r="C78" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A79" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B79" s="6"/>
       <c r="C79" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>228</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A80" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B80" s="6"/>
       <c r="C80" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="81" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A81" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B81" s="6"/>
       <c r="C81" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="6" t="s">
         <v>234</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="82" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A82" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="D82" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="8" t="s">
         <v>237</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="83" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A83" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="D83" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A84" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="D84" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:29" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A85" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="18" t="s">
         <v>277</v>
-      </c>
-      <c r="C85" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="D85" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E85" s="18" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="86" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="87" spans="1:29" s="7" customFormat="1" ht="16.5">
       <c r="A87" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A88" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B88" s="10"/>
       <c r="C88" s="10" t="s">
@@ -2912,7 +2912,7 @@
         <v>1</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
@@ -2941,17 +2941,17 @@
     </row>
     <row r="89" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A89" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E89" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
@@ -2980,17 +2980,17 @@
     </row>
     <row r="90" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A90" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E90" s="6" t="s">
         <v>250</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>251</v>
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
@@ -3019,17 +3019,17 @@
     </row>
     <row r="91" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A91" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B91" s="6"/>
       <c r="C91" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E91" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>254</v>
       </c>
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
@@ -3058,17 +3058,17 @@
     </row>
     <row r="92" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A92" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E92" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>257</v>
       </c>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
@@ -3097,17 +3097,17 @@
     </row>
     <row r="93" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A93" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B93" s="6"/>
       <c r="C93" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E93" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>260</v>
       </c>
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
@@ -3167,7 +3167,7 @@
     </row>
     <row r="95" spans="1:29" s="7" customFormat="1" ht="16.5">
       <c r="A95" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="96" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A96" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="10" t="s">
@@ -3210,7 +3210,7 @@
         <v>1</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
@@ -3239,58 +3239,58 @@
     </row>
     <row r="97" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A97" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C97" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="D97" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E97" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A98" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C98" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="D98" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E98" s="8" t="s">
         <v>266</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A99" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="C99" s="6" t="s">
+      <c r="D99" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="8" t="s">
         <v>269</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A100" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C100" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="D100" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>272</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update xule processor, integrate Travis CI, update documentation (#299)
* Add test suite (#297)

* Update test suite and rule documentation (#298)
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="0" windowWidth="12600" windowHeight="22350"/>
+    <workbookView xWindow="2730" yWindow="870" windowWidth="23280" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -306,9 +306,6 @@
     <t>Defined Benefit Plan, Asset Categories [Axis]</t>
   </si>
   <si>
-    <t>All - except members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis</t>
-  </si>
-  <si>
     <t>DQC_0001.72</t>
   </si>
   <si>
@@ -906,9 +903,6 @@
     <t>NotDesignatedAsHedgingInstrumentEconomicHedgesMember, NotDesignatedAsHedgingInstrumentTradingMember</t>
   </si>
   <si>
-    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, InvestmentsNetAssetValueMember</t>
-  </si>
-  <si>
     <t>InvestmentsNetAssetValueMember</t>
   </si>
   <si>
@@ -919,6 +913,12 @@
   </si>
   <si>
     <t>Vehicles that are used primarily for transporting people.</t>
+  </si>
+  <si>
+    <t>ALL but no members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis</t>
+  </si>
+  <si>
+    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, FairValueMeasuredAtNetAssetValuePerShareMember</t>
   </si>
 </sst>
 </file>
@@ -1359,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1444,7 +1444,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="J2" s="6"/>
     </row>
@@ -1757,10 +1757,10 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -1787,7 +1787,7 @@
         <v>14</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -1865,7 +1865,7 @@
         <v>13</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>75</v>
+        <v>278</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6" t="s">
@@ -1877,16 +1877,16 @@
     </row>
     <row r="19" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>22</v>
@@ -1902,16 +1902,16 @@
     </row>
     <row r="20" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>81</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>13</v>
@@ -1927,23 +1927,23 @@
     </row>
     <row r="21" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>13</v>
@@ -1954,16 +1954,16 @@
     </row>
     <row r="22" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>13</v>
@@ -1979,16 +1979,16 @@
     </row>
     <row r="23" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>13</v>
@@ -2063,7 +2063,7 @@
     </row>
     <row r="28" spans="1:29" s="7" customFormat="1" ht="16.5">
       <c r="A28" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -2096,7 +2096,7 @@
     </row>
     <row r="29" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10" t="s">
@@ -2106,228 +2106,228 @@
         <v>1</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A30" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A37" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>117</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>126</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B42" s="6"/>
       <c r="C42" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>132</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A43" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>135</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="45" spans="1:5" s="7" customFormat="1" ht="16.5">
       <c r="A45" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A46" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10" t="s">
@@ -2337,137 +2337,137 @@
         <v>1</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A49" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B49" s="15"/>
       <c r="C49" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A50" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A51" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="D51" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>152</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A52" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="D52" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A53" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="D53" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E53" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A54" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="D54" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E54" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A55" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="D55" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E55" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="7" customFormat="1" ht="16.5">
@@ -2475,12 +2475,12 @@
     </row>
     <row r="57" spans="1:5" s="7" customFormat="1" ht="16.5">
       <c r="A57" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A58" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10" t="s">
@@ -2490,419 +2490,419 @@
         <v>1</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A59" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B59" s="6"/>
       <c r="C59" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A60" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A61" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B61" s="6"/>
       <c r="C61" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A62" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A63" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A64" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B64" s="6"/>
       <c r="C64" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A65" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A66" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B66" s="6"/>
       <c r="C66" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A67" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B67" s="6"/>
       <c r="C67" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A68" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A69" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A70" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B70" s="6"/>
       <c r="C70" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A71" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B71" s="6"/>
       <c r="C71" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>204</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A72" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B72" s="6"/>
       <c r="C72" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A73" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A74" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="6" t="s">
         <v>213</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A75" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B75" s="6"/>
       <c r="C75" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="6" t="s">
         <v>216</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A76" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B76" s="6"/>
       <c r="C76" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A77" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B77" s="6"/>
       <c r="C77" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A78" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B78" s="6"/>
       <c r="C78" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A79" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B79" s="6"/>
       <c r="C79" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>228</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A80" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B80" s="6"/>
       <c r="C80" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="6" t="s">
         <v>231</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="81" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A81" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B81" s="6"/>
       <c r="C81" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="6" t="s">
         <v>234</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="82" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A82" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="D82" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="8" t="s">
         <v>237</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="83" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A83" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="D83" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A84" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="D84" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="85" spans="1:29" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A85" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="18" t="s">
         <v>277</v>
-      </c>
-      <c r="C85" s="18" t="s">
-        <v>278</v>
-      </c>
-      <c r="D85" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E85" s="18" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="86" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="87" spans="1:29" s="7" customFormat="1" ht="16.5">
       <c r="A87" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A88" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B88" s="10"/>
       <c r="C88" s="10" t="s">
@@ -2912,7 +2912,7 @@
         <v>1</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
@@ -2941,17 +2941,17 @@
     </row>
     <row r="89" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A89" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E89" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
@@ -2980,17 +2980,17 @@
     </row>
     <row r="90" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A90" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E90" s="6" t="s">
         <v>250</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>251</v>
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
@@ -3019,17 +3019,17 @@
     </row>
     <row r="91" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A91" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B91" s="6"/>
       <c r="C91" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E91" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>254</v>
       </c>
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
@@ -3058,17 +3058,17 @@
     </row>
     <row r="92" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A92" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E92" s="6" t="s">
         <v>256</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>257</v>
       </c>
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
@@ -3097,17 +3097,17 @@
     </row>
     <row r="93" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A93" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B93" s="6"/>
       <c r="C93" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E93" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>260</v>
       </c>
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
@@ -3167,7 +3167,7 @@
     </row>
     <row r="95" spans="1:29" s="7" customFormat="1" ht="16.5">
       <c r="A95" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="96" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A96" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="10" t="s">
@@ -3210,7 +3210,7 @@
         <v>1</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
@@ -3239,58 +3239,58 @@
     </row>
     <row r="97" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A97" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C97" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="D97" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E97" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="98" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A98" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C98" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="D98" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E98" s="8" t="s">
         <v>266</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A99" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="C99" s="6" t="s">
+      <c r="D99" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="8" t="s">
         <v>269</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="100" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A100" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C100" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="D100" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E100" s="8" t="s">
         <v>272</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="101" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update documentation and resource files for v6
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="870" windowWidth="23280" windowHeight="9660"/>
+    <workbookView xWindow="3180" yWindow="0" windowWidth="12600" windowHeight="22350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -294,9 +294,6 @@
     <t>Consolidation Items [Axis]</t>
   </si>
   <si>
-    <t>CorporateReconcilingItemsAndEliminationsMember, CorporateAndReconcilingItemsMember, CorporateAndEliminationsMember, EliminationsAndReconcilingItemsMember, OperatingSegmentsAndCorporateNonSegmentMember</t>
-  </si>
-  <si>
     <t>DQC_0001.71</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
     <t>Defined Benefit Plan, Asset Categories [Axis]</t>
   </si>
   <si>
+    <t>All - except members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis</t>
+  </si>
+  <si>
     <t>DQC_0001.72</t>
   </si>
   <si>
@@ -903,6 +903,9 @@
     <t>NotDesignatedAsHedgingInstrumentEconomicHedgesMember, NotDesignatedAsHedgingInstrumentTradingMember</t>
   </si>
   <si>
+    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, InvestmentsNetAssetValueMember</t>
+  </si>
+  <si>
     <t>InvestmentsNetAssetValueMember</t>
   </si>
   <si>
@@ -915,10 +918,7 @@
     <t>Vehicles that are used primarily for transporting people.</t>
   </si>
   <si>
-    <t>ALL but no members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis</t>
-  </si>
-  <si>
-    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, FairValueMeasuredAtNetAssetValuePerShareMember</t>
+    <t>CorporateReconcilingItemsAndEliminationsMember, CorporateAndReconcilingItemsMember, CorporateAndEliminationsMember, EliminationsAndReconcilingItemsMember, OperatingSegmentsAndCorporateNonSegmentMember, OperatingSegmentsExcludingIntersegmentEliminationMember</t>
   </si>
 </sst>
 </file>
@@ -1359,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1444,7 +1444,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="J2" s="6"/>
     </row>
@@ -1760,7 +1760,7 @@
         <v>14</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -1843,29 +1843,29 @@
         <v>14</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>71</v>
+        <v>279</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>278</v>
+        <v>74</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6" t="s">
@@ -2882,16 +2882,16 @@
     </row>
     <row r="85" spans="1:29" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A85" s="16" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C85" s="18" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D85" s="18" t="s">
         <v>10</v>
       </c>
       <c r="E85" s="18" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="86" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Revert "Update documentation and resource files for v6"
This reverts commit 364f7f14b6b8e158db454dca6360f0246f327561.
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="0" windowWidth="12600" windowHeight="22350"/>
+    <workbookView xWindow="2730" yWindow="870" windowWidth="23280" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -294,6 +294,9 @@
     <t>Consolidation Items [Axis]</t>
   </si>
   <si>
+    <t>CorporateReconcilingItemsAndEliminationsMember, CorporateAndReconcilingItemsMember, CorporateAndEliminationsMember, EliminationsAndReconcilingItemsMember, OperatingSegmentsAndCorporateNonSegmentMember</t>
+  </si>
+  <si>
     <t>DQC_0001.71</t>
   </si>
   <si>
@@ -303,9 +306,6 @@
     <t>Defined Benefit Plan, Asset Categories [Axis]</t>
   </si>
   <si>
-    <t>All - except members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis</t>
-  </si>
-  <si>
     <t>DQC_0001.72</t>
   </si>
   <si>
@@ -903,9 +903,6 @@
     <t>NotDesignatedAsHedgingInstrumentEconomicHedgesMember, NotDesignatedAsHedgingInstrumentTradingMember</t>
   </si>
   <si>
-    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, InvestmentsNetAssetValueMember</t>
-  </si>
-  <si>
     <t>InvestmentsNetAssetValueMember</t>
   </si>
   <si>
@@ -918,7 +915,10 @@
     <t>Vehicles that are used primarily for transporting people.</t>
   </si>
   <si>
-    <t>CorporateReconcilingItemsAndEliminationsMember, CorporateAndReconcilingItemsMember, CorporateAndEliminationsMember, EliminationsAndReconcilingItemsMember, OperatingSegmentsAndCorporateNonSegmentMember, OperatingSegmentsExcludingIntersegmentEliminationMember</t>
+    <t>ALL but no members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis</t>
+  </si>
+  <si>
+    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, FairValueMeasuredAtNetAssetValuePerShareMember</t>
   </si>
 </sst>
 </file>
@@ -1359,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1444,7 +1444,7 @@
         <v>14</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="J2" s="6"/>
     </row>
@@ -1760,7 +1760,7 @@
         <v>14</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
@@ -1843,29 +1843,29 @@
         <v>14</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>279</v>
+        <v>71</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>74</v>
+        <v>278</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6" t="s">
@@ -2882,16 +2882,16 @@
     </row>
     <row r="85" spans="1:29" s="17" customFormat="1" ht="15.75" customHeight="1">
       <c r="A85" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="C85" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="C85" s="18" t="s">
+      <c r="D85" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="18" t="s">
         <v>277</v>
-      </c>
-      <c r="D85" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E85" s="18" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="86" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update DQC_0001 List of Axes and DQC_0070 for public exposure
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$100</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -22,7 +22,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="G8" authorId="0">
+    <comment ref="H8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -35,7 +35,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0">
+    <comment ref="J11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0">
+    <comment ref="H16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0">
+    <comment ref="J17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="283">
   <si>
     <t>Rule element ID</t>
   </si>
@@ -303,9 +303,6 @@
     <t>Defined Benefit Plan, Asset Categories [Axis]</t>
   </si>
   <si>
-    <t>All - except members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis</t>
-  </si>
-  <si>
     <t>DQC_0001.72</t>
   </si>
   <si>
@@ -900,9 +897,6 @@
     <t>Trust created by the entity that exists for the benefit of its employees, such as pension and profit-sharing trusts that are managed by or under the trusteeship of the entity's management.</t>
   </si>
   <si>
-    <t>NotDesignatedAsHedgingInstrumentEconomicHedgesMember, NotDesignatedAsHedgingInstrumentTradingMember</t>
-  </si>
-  <si>
     <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, InvestmentsNetAssetValueMember</t>
   </si>
   <si>
@@ -919,6 +913,21 @@
   </si>
   <si>
     <t>CorporateReconcilingItemsAndEliminationsMember, CorporateAndReconcilingItemsMember, CorporateAndEliminationsMember, EliminationsAndReconcilingItemsMember, OperatingSegmentsAndCorporateNonSegmentMember, OperatingSegmentsExcludingIntersegmentEliminationMember</t>
+  </si>
+  <si>
+    <t>All Taxonomies</t>
+  </si>
+  <si>
+    <t>All to 2016</t>
+  </si>
+  <si>
+    <t>Rule Applies to:</t>
+  </si>
+  <si>
+    <t>NotDesignatedAsHedgingInstrumentEconomicHedgesMember, NotDesignatedAsHedgingInstrumentTradingMember (PRIOR TO 2017)</t>
+  </si>
+  <si>
+    <t>All - except members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis (Not applicable after 2016);  All - except members on: RetirementPlanTypeAxis, RetirementPlanSponsorLocationAxis, RetirementPlanTaxStatusAxis, RetirementPlanFundingStatusAxis, RetirementPlanNameAxis (After 2016)</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1063,6 +1072,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1357,52 +1367,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC101"/>
+  <dimension ref="A1:AD101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="54" customWidth="1"/>
-    <col min="4" max="4" width="47" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="46.85546875" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
-    <col min="9" max="9" width="54.85546875" customWidth="1"/>
+    <col min="1" max="2" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="54" customWidth="1"/>
+    <col min="5" max="5" width="47" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="46.85546875" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" customWidth="1"/>
+    <col min="10" max="10" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" customHeight="1">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -1421,182 +1431,203 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
-    </row>
-    <row r="2" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AC1" s="3"/>
+    </row>
+    <row r="2" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>10</v>
+      <c r="B2" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="12"/>
       <c r="G2" s="12"/>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="J2" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>10</v>
+      <c r="B3" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
+      <c r="B4" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>10</v>
+      <c r="B6" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>10</v>
+      <c r="B7" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>10</v>
+      <c r="B8" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -1608,401 +1639,447 @@
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
-    </row>
-    <row r="9" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="U8" s="6"/>
+    </row>
+    <row r="9" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
+      <c r="B9" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="6"/>
+      <c r="I9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>10</v>
+      <c r="B10" s="19" t="s">
+        <v>279</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="6"/>
+      <c r="I10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="6"/>
+      <c r="I11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="6"/>
       <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>10</v>
+      <c r="B12" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="6"/>
+      <c r="I12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="J12" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>10</v>
+      <c r="B13" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="6"/>
+      <c r="I13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>10</v>
+      <c r="B14" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="6"/>
+      <c r="I14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="J14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>273</v>
+      </c>
       <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>10</v>
+      <c r="B15" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="6"/>
+      <c r="I15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="J15" s="6"/>
+      <c r="J15" s="6" t="s">
+        <v>281</v>
+      </c>
       <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>10</v>
+      <c r="B16" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="G16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="H16" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="I16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>10</v>
+      <c r="B17" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="6"/>
+      <c r="I17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="J17" s="6"/>
+      <c r="J17" s="6" t="s">
+        <v>277</v>
+      </c>
       <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>10</v>
+      <c r="B18" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6" t="s">
+      <c r="G18" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="6"/>
+      <c r="I19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="6"/>
+      <c r="I20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="F21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="I21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="6"/>
+      <c r="I22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="6"/>
+      <c r="I23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -2014,8 +2091,9 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:29" ht="15.75" customHeight="1">
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:30" ht="15.75" customHeight="1">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2045,9 +2123,9 @@
       <c r="AA25" s="4"/>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
-    </row>
-    <row r="27" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="G27" s="6"/>
+      <c r="AD25" s="4"/>
+    </row>
+    <row r="27" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
@@ -2060,12 +2138,13 @@
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
       <c r="S27" s="6"/>
-    </row>
-    <row r="28" spans="1:29" s="7" customFormat="1" ht="16.5">
+      <c r="T27" s="6"/>
+    </row>
+    <row r="28" spans="1:30" s="7" customFormat="1" ht="16.5">
       <c r="A28" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="13"/>
+        <v>90</v>
+      </c>
+      <c r="B28" s="9"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
@@ -2093,828 +2172,886 @@
       <c r="AA28" s="13"/>
       <c r="AB28" s="13"/>
       <c r="AC28" s="13"/>
-    </row>
-    <row r="29" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD28" s="13"/>
+    </row>
+    <row r="29" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10" t="s">
+    </row>
+    <row r="30" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A30" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A31" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A32" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A33" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A34" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A35" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A36" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A37" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A38" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A39" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A40" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A41" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A42" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A43" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:6" s="7" customFormat="1" ht="16.5">
+      <c r="A45" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="9"/>
+    </row>
+    <row r="46" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A46" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="E46" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A31" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A32" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A33" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A34" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A35" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A36" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A37" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A38" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A39" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A40" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A41" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A42" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A43" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="45" spans="1:5" s="7" customFormat="1" ht="16.5">
-      <c r="A45" s="9" t="s">
+      <c r="F46" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A47" s="6" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A46" s="10" t="s">
+      <c r="B47" s="6"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A48" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" s="6"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A49" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A50" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A51" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="D51" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A52" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="D52" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A53" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="D53" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A54" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="D54" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A55" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="D55" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="7" customFormat="1" ht="16.5">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+    </row>
+    <row r="57" spans="1:6" s="7" customFormat="1" ht="16.5">
+      <c r="A57" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B57" s="9"/>
+    </row>
+    <row r="58" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A58" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10" t="s">
+    </row>
+    <row r="59" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A59" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A60" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A61" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A62" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A63" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A64" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A65" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A66" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A67" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A68" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A69" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A70" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A71" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A72" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A73" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A74" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A75" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A76" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A77" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A78" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A79" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A80" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="81" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A81" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="82" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A82" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="D82" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="83" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A83" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B83" s="8"/>
+      <c r="D83" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="84" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A84" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B84" s="8"/>
+      <c r="D84" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="85" spans="1:30" s="17" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A85" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="B85" s="16"/>
+      <c r="D85" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" s="18" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="86" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="87" spans="1:30" s="7" customFormat="1" ht="16.5">
+      <c r="A87" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B87" s="9"/>
+    </row>
+    <row r="88" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A88" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="E88" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E46" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A47" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B47" s="15"/>
-      <c r="C47" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A48" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B48" s="15"/>
-      <c r="C48" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A49" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A50" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A51" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A52" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A53" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A54" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A55" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="7" customFormat="1" ht="16.5">
-      <c r="A56" s="9"/>
-    </row>
-    <row r="57" spans="1:5" s="7" customFormat="1" ht="16.5">
-      <c r="A57" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A58" s="10" t="s">
+      <c r="F88" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A59" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A60" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A61" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A62" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A63" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B63" s="6"/>
-      <c r="C63" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A64" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B64" s="6"/>
-      <c r="C64" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A65" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B65" s="6"/>
-      <c r="C65" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A66" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B66" s="6"/>
-      <c r="C66" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A67" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A68" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A69" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A70" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A71" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A72" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B72" s="6"/>
-      <c r="C72" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A73" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A74" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A75" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="B75" s="6"/>
-      <c r="C75" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A76" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="B76" s="6"/>
-      <c r="C76" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A77" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="B77" s="6"/>
-      <c r="C77" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A78" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="B78" s="6"/>
-      <c r="C78" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A79" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="B79" s="6"/>
-      <c r="C79" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A80" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="B80" s="6"/>
-      <c r="C80" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="81" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A81" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B81" s="6"/>
-      <c r="C81" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="82" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A82" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="83" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A83" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="84" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A84" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="85" spans="1:29" s="17" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A85" s="16" t="s">
-        <v>276</v>
-      </c>
-      <c r="C85" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="D85" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E85" s="18" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="86" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="87" spans="1:29" s="7" customFormat="1" ht="16.5">
-      <c r="A87" s="9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="88" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A88" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B88" s="10"/>
-      <c r="C88" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D88" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E88" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F88" s="6"/>
       <c r="G88" s="6"/>
       <c r="H88" s="6"/>
       <c r="I88" s="6"/>
@@ -2938,22 +3075,23 @@
       <c r="AA88" s="6"/>
       <c r="AB88" s="6"/>
       <c r="AC88" s="6"/>
-    </row>
-    <row r="89" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD88" s="6"/>
+    </row>
+    <row r="89" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A89" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="B89" s="6"/>
-      <c r="C89" s="6" t="s">
+      <c r="E89" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F89" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="D89" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="F89" s="6"/>
       <c r="G89" s="6"/>
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
@@ -2977,22 +3115,23 @@
       <c r="AA89" s="6"/>
       <c r="AB89" s="6"/>
       <c r="AC89" s="6"/>
-    </row>
-    <row r="90" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD89" s="6"/>
+    </row>
+    <row r="90" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A90" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B90" s="6"/>
-      <c r="C90" s="6" t="s">
+      <c r="E90" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F90" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="D90" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="F90" s="6"/>
       <c r="G90" s="6"/>
       <c r="H90" s="6"/>
       <c r="I90" s="6"/>
@@ -3016,22 +3155,23 @@
       <c r="AA90" s="6"/>
       <c r="AB90" s="6"/>
       <c r="AC90" s="6"/>
-    </row>
-    <row r="91" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD90" s="6"/>
+    </row>
+    <row r="91" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A91" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B91" s="6"/>
-      <c r="C91" s="6" t="s">
+      <c r="E91" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F91" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="D91" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="F91" s="6"/>
       <c r="G91" s="6"/>
       <c r="H91" s="6"/>
       <c r="I91" s="6"/>
@@ -3055,22 +3195,23 @@
       <c r="AA91" s="6"/>
       <c r="AB91" s="6"/>
       <c r="AC91" s="6"/>
-    </row>
-    <row r="92" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD91" s="6"/>
+    </row>
+    <row r="92" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A92" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B92" s="6"/>
-      <c r="C92" s="6" t="s">
+      <c r="E92" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F92" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="D92" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="F92" s="6"/>
       <c r="G92" s="6"/>
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
@@ -3094,22 +3235,23 @@
       <c r="AA92" s="6"/>
       <c r="AB92" s="6"/>
       <c r="AC92" s="6"/>
-    </row>
-    <row r="93" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD92" s="6"/>
+    </row>
+    <row r="93" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A93" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="B93" s="6"/>
-      <c r="C93" s="6" t="s">
+      <c r="E93" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F93" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="D93" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="F93" s="6"/>
       <c r="G93" s="6"/>
       <c r="H93" s="6"/>
       <c r="I93" s="6"/>
@@ -3133,8 +3275,9 @@
       <c r="AA93" s="6"/>
       <c r="AB93" s="6"/>
       <c r="AC93" s="6"/>
-    </row>
-    <row r="94" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD93" s="6"/>
+    </row>
+    <row r="94" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -3164,12 +3307,13 @@
       <c r="AA94" s="6"/>
       <c r="AB94" s="6"/>
       <c r="AC94" s="6"/>
-    </row>
-    <row r="95" spans="1:29" s="7" customFormat="1" ht="16.5">
+      <c r="AD94" s="6"/>
+    </row>
+    <row r="95" spans="1:30" s="7" customFormat="1" ht="16.5">
       <c r="A95" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="B95" s="6"/>
+        <v>259</v>
+      </c>
+      <c r="B95" s="9"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
       <c r="E95" s="6"/>
@@ -3197,22 +3341,23 @@
       <c r="AA95" s="6"/>
       <c r="AB95" s="6"/>
       <c r="AC95" s="6"/>
-    </row>
-    <row r="96" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD95" s="6"/>
+    </row>
+    <row r="96" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A96" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F96" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D96" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E96" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F96" s="6"/>
       <c r="G96" s="6"/>
       <c r="H96" s="6"/>
       <c r="I96" s="6"/>
@@ -3236,66 +3381,73 @@
       <c r="AA96" s="6"/>
       <c r="AB96" s="6"/>
       <c r="AC96" s="6"/>
-    </row>
-    <row r="97" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD96" s="6"/>
+    </row>
+    <row r="97" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A97" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B97" s="8"/>
+      <c r="D97" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="E97" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="D97" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E97" s="8" t="s">
+    </row>
+    <row r="98" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A98" s="8" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A98" s="8" t="s">
+      <c r="B98" s="8"/>
+      <c r="D98" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="E98" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F98" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="D98" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E98" s="8" t="s">
+    </row>
+    <row r="99" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A99" s="8" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A99" s="8" t="s">
+      <c r="B99" s="8"/>
+      <c r="D99" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="C99" s="6" t="s">
+      <c r="E99" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F99" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="D99" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" s="8" t="s">
+    </row>
+    <row r="100" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A100" s="8" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A100" s="8" t="s">
+      <c r="B100" s="8"/>
+      <c r="D100" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="E100" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F100" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="D100" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="101" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:K100"/>
+  <autoFilter ref="A1:L100">
+    <filterColumn colId="1"/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Merge for v7 Public Exposure (#331)
* Commit Version 7

* Updates for version 7 of the rules

* Updated and Created Version 7 rules for 2017 Taxonomy

* Updated rules for Resource files and fix to DQC 1

* Updated Rules for bugs identified during testing

* Updated functions for rule 43 2018 & 2016

* Updated Rule 43 to address when there are multiple cash flow statements with contradicting weights.

* Updated rule 70 for 2016 and 2018 taxonomies

* Updated DQC 15 so would be more efficient. Regenerated test cases for 13 and 15.

* Updated DQC0001 for deprecated items.

* Changed DQC.US.0001.71 for deprecated axis and updated 66 for extension elements that are now in the taxonomy and removed rule 60 which has DefinedContributionPlanNameAxis.

* Updated rule 47 to clean up error message which was misleading

* Split plugin into xule and dqc.

* Remove test cases

* update rulesetMap
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$100</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -22,7 +22,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="G8" authorId="0">
+    <comment ref="H8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -35,7 +35,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0">
+    <comment ref="J11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0">
+    <comment ref="H16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0">
+    <comment ref="J17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="283">
   <si>
     <t>Rule element ID</t>
   </si>
@@ -303,9 +303,6 @@
     <t>Defined Benefit Plan, Asset Categories [Axis]</t>
   </si>
   <si>
-    <t>All - except members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis</t>
-  </si>
-  <si>
     <t>DQC_0001.72</t>
   </si>
   <si>
@@ -900,9 +897,6 @@
     <t>Trust created by the entity that exists for the benefit of its employees, such as pension and profit-sharing trusts that are managed by or under the trusteeship of the entity's management.</t>
   </si>
   <si>
-    <t>NotDesignatedAsHedgingInstrumentEconomicHedgesMember, NotDesignatedAsHedgingInstrumentTradingMember</t>
-  </si>
-  <si>
     <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, InvestmentsNetAssetValueMember</t>
   </si>
   <si>
@@ -919,6 +913,21 @@
   </si>
   <si>
     <t>CorporateReconcilingItemsAndEliminationsMember, CorporateAndReconcilingItemsMember, CorporateAndEliminationsMember, EliminationsAndReconcilingItemsMember, OperatingSegmentsAndCorporateNonSegmentMember, OperatingSegmentsExcludingIntersegmentEliminationMember</t>
+  </si>
+  <si>
+    <t>All Taxonomies</t>
+  </si>
+  <si>
+    <t>All to 2016</t>
+  </si>
+  <si>
+    <t>Rule Applies to:</t>
+  </si>
+  <si>
+    <t>NotDesignatedAsHedgingInstrumentEconomicHedgesMember, NotDesignatedAsHedgingInstrumentTradingMember (PRIOR TO 2017)</t>
+  </si>
+  <si>
+    <t>All - except members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis (Not applicable after 2016);  All - except members on: RetirementPlanTypeAxis, RetirementPlanSponsorLocationAxis, RetirementPlanTaxStatusAxis, RetirementPlanFundingStatusAxis, RetirementPlanNameAxis (After 2016)</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1063,6 +1072,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1357,52 +1367,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC101"/>
+  <dimension ref="A1:AD101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="54" customWidth="1"/>
-    <col min="4" max="4" width="47" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="46.85546875" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
-    <col min="9" max="9" width="54.85546875" customWidth="1"/>
+    <col min="1" max="2" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="54" customWidth="1"/>
+    <col min="5" max="5" width="47" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="46.85546875" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" customWidth="1"/>
+    <col min="10" max="10" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" customHeight="1">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -1421,182 +1431,203 @@
       <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
-    </row>
-    <row r="2" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AC1" s="3"/>
+    </row>
+    <row r="2" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>10</v>
+      <c r="B2" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="12"/>
       <c r="G2" s="12"/>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="J2" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>10</v>
+      <c r="B3" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
+      <c r="B4" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>10</v>
+      <c r="B6" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>10</v>
+      <c r="B7" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>10</v>
+      <c r="B8" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -1608,401 +1639,447 @@
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
-    </row>
-    <row r="9" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="U8" s="6"/>
+    </row>
+    <row r="9" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
+      <c r="B9" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="6"/>
+      <c r="I9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>10</v>
+      <c r="B10" s="19" t="s">
+        <v>279</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="6"/>
+      <c r="I10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="6"/>
+      <c r="I11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="6"/>
       <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>10</v>
+      <c r="B12" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="6"/>
+      <c r="I12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="J12" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>10</v>
+      <c r="B13" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="6"/>
+      <c r="I13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>10</v>
+      <c r="B14" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="6"/>
+      <c r="I14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="J14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>273</v>
+      </c>
       <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>10</v>
+      <c r="B15" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="6"/>
+      <c r="I15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="J15" s="6"/>
+      <c r="J15" s="6" t="s">
+        <v>281</v>
+      </c>
       <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:28" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>10</v>
+      <c r="B16" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="G16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="H16" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="I16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>10</v>
+      <c r="B17" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="6"/>
+      <c r="I17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="J17" s="6"/>
+      <c r="J17" s="6" t="s">
+        <v>277</v>
+      </c>
       <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>10</v>
+      <c r="B18" s="19" t="s">
+        <v>278</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6" t="s">
+      <c r="G18" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="6"/>
+      <c r="I19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="6"/>
+      <c r="I20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="F21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="I21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6" t="s">
+      <c r="H22" s="6"/>
+      <c r="I22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="6"/>
+      <c r="I23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -2014,8 +2091,9 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:29" ht="15.75" customHeight="1">
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:30" ht="15.75" customHeight="1">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2045,9 +2123,9 @@
       <c r="AA25" s="4"/>
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
-    </row>
-    <row r="27" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="G27" s="6"/>
+      <c r="AD25" s="4"/>
+    </row>
+    <row r="27" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
@@ -2060,12 +2138,13 @@
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
       <c r="S27" s="6"/>
-    </row>
-    <row r="28" spans="1:29" s="7" customFormat="1" ht="16.5">
+      <c r="T27" s="6"/>
+    </row>
+    <row r="28" spans="1:30" s="7" customFormat="1" ht="16.5">
       <c r="A28" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="13"/>
+        <v>90</v>
+      </c>
+      <c r="B28" s="9"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
@@ -2093,828 +2172,886 @@
       <c r="AA28" s="13"/>
       <c r="AB28" s="13"/>
       <c r="AC28" s="13"/>
-    </row>
-    <row r="29" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD28" s="13"/>
+    </row>
+    <row r="29" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10" t="s">
+    </row>
+    <row r="30" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A30" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A31" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A32" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A33" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A34" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A35" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A36" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A37" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A38" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A39" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A40" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A41" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A42" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A43" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="45" spans="1:6" s="7" customFormat="1" ht="16.5">
+      <c r="A45" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="9"/>
+    </row>
+    <row r="46" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A46" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="E46" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A31" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A32" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A33" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A34" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A35" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A36" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A37" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A38" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A39" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A40" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A41" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A42" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A43" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="45" spans="1:5" s="7" customFormat="1" ht="16.5">
-      <c r="A45" s="9" t="s">
+      <c r="F46" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A47" s="6" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A46" s="10" t="s">
+      <c r="B47" s="6"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A48" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" s="6"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A49" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A50" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A51" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="D51" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A52" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="D52" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A53" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="D53" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A54" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="D54" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A55" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="D55" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="7" customFormat="1" ht="16.5">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+    </row>
+    <row r="57" spans="1:6" s="7" customFormat="1" ht="16.5">
+      <c r="A57" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B57" s="9"/>
+    </row>
+    <row r="58" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A58" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10" t="s">
+    </row>
+    <row r="59" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A59" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A60" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A61" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A62" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A63" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A64" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A65" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A66" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A67" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A68" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A69" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A70" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A71" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A72" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A73" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A74" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A75" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A76" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A77" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A78" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A79" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A80" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="81" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A81" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="82" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A82" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="D82" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="83" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A83" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B83" s="8"/>
+      <c r="D83" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="84" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A84" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B84" s="8"/>
+      <c r="D84" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="85" spans="1:30" s="17" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A85" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="B85" s="16"/>
+      <c r="D85" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" s="18" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="86" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="87" spans="1:30" s="7" customFormat="1" ht="16.5">
+      <c r="A87" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B87" s="9"/>
+    </row>
+    <row r="88" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A88" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="E88" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E46" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A47" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B47" s="15"/>
-      <c r="C47" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A48" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B48" s="15"/>
-      <c r="C48" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A49" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A50" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A51" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A52" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A53" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A54" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A55" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="7" customFormat="1" ht="16.5">
-      <c r="A56" s="9"/>
-    </row>
-    <row r="57" spans="1:5" s="7" customFormat="1" ht="16.5">
-      <c r="A57" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A58" s="10" t="s">
+      <c r="F88" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A59" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A60" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A61" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B61" s="6"/>
-      <c r="C61" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A62" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B62" s="6"/>
-      <c r="C62" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A63" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B63" s="6"/>
-      <c r="C63" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A64" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B64" s="6"/>
-      <c r="C64" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A65" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B65" s="6"/>
-      <c r="C65" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A66" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B66" s="6"/>
-      <c r="C66" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A67" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A68" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A69" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A70" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A71" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A72" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B72" s="6"/>
-      <c r="C72" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A73" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A74" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A75" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="B75" s="6"/>
-      <c r="C75" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A76" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="B76" s="6"/>
-      <c r="C76" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A77" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="B77" s="6"/>
-      <c r="C77" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A78" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="B78" s="6"/>
-      <c r="C78" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A79" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="B79" s="6"/>
-      <c r="C79" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A80" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="B80" s="6"/>
-      <c r="C80" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="81" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A81" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B81" s="6"/>
-      <c r="C81" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="82" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A82" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="83" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A83" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="84" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A84" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="85" spans="1:29" s="17" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A85" s="16" t="s">
-        <v>276</v>
-      </c>
-      <c r="C85" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="D85" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E85" s="18" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="86" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="87" spans="1:29" s="7" customFormat="1" ht="16.5">
-      <c r="A87" s="9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="88" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A88" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B88" s="10"/>
-      <c r="C88" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D88" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E88" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F88" s="6"/>
       <c r="G88" s="6"/>
       <c r="H88" s="6"/>
       <c r="I88" s="6"/>
@@ -2938,22 +3075,23 @@
       <c r="AA88" s="6"/>
       <c r="AB88" s="6"/>
       <c r="AC88" s="6"/>
-    </row>
-    <row r="89" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD88" s="6"/>
+    </row>
+    <row r="89" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A89" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="B89" s="6"/>
-      <c r="C89" s="6" t="s">
+      <c r="E89" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F89" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="D89" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="F89" s="6"/>
       <c r="G89" s="6"/>
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
@@ -2977,22 +3115,23 @@
       <c r="AA89" s="6"/>
       <c r="AB89" s="6"/>
       <c r="AC89" s="6"/>
-    </row>
-    <row r="90" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD89" s="6"/>
+    </row>
+    <row r="90" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A90" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="B90" s="6"/>
-      <c r="C90" s="6" t="s">
+      <c r="E90" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F90" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="D90" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="F90" s="6"/>
       <c r="G90" s="6"/>
       <c r="H90" s="6"/>
       <c r="I90" s="6"/>
@@ -3016,22 +3155,23 @@
       <c r="AA90" s="6"/>
       <c r="AB90" s="6"/>
       <c r="AC90" s="6"/>
-    </row>
-    <row r="91" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD90" s="6"/>
+    </row>
+    <row r="91" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A91" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B91" s="6"/>
-      <c r="C91" s="6" t="s">
+      <c r="E91" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F91" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="D91" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="F91" s="6"/>
       <c r="G91" s="6"/>
       <c r="H91" s="6"/>
       <c r="I91" s="6"/>
@@ -3055,22 +3195,23 @@
       <c r="AA91" s="6"/>
       <c r="AB91" s="6"/>
       <c r="AC91" s="6"/>
-    </row>
-    <row r="92" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD91" s="6"/>
+    </row>
+    <row r="92" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A92" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B92" s="6"/>
-      <c r="C92" s="6" t="s">
+      <c r="E92" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F92" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="D92" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="F92" s="6"/>
       <c r="G92" s="6"/>
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
@@ -3094,22 +3235,23 @@
       <c r="AA92" s="6"/>
       <c r="AB92" s="6"/>
       <c r="AC92" s="6"/>
-    </row>
-    <row r="93" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD92" s="6"/>
+    </row>
+    <row r="93" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A93" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="B93" s="6"/>
-      <c r="C93" s="6" t="s">
+      <c r="E93" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F93" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="D93" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="F93" s="6"/>
       <c r="G93" s="6"/>
       <c r="H93" s="6"/>
       <c r="I93" s="6"/>
@@ -3133,8 +3275,9 @@
       <c r="AA93" s="6"/>
       <c r="AB93" s="6"/>
       <c r="AC93" s="6"/>
-    </row>
-    <row r="94" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD93" s="6"/>
+    </row>
+    <row r="94" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -3164,12 +3307,13 @@
       <c r="AA94" s="6"/>
       <c r="AB94" s="6"/>
       <c r="AC94" s="6"/>
-    </row>
-    <row r="95" spans="1:29" s="7" customFormat="1" ht="16.5">
+      <c r="AD94" s="6"/>
+    </row>
+    <row r="95" spans="1:30" s="7" customFormat="1" ht="16.5">
       <c r="A95" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="B95" s="6"/>
+        <v>259</v>
+      </c>
+      <c r="B95" s="9"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
       <c r="E95" s="6"/>
@@ -3197,22 +3341,23 @@
       <c r="AA95" s="6"/>
       <c r="AB95" s="6"/>
       <c r="AC95" s="6"/>
-    </row>
-    <row r="96" spans="1:29" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD95" s="6"/>
+    </row>
+    <row r="96" spans="1:30" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A96" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F96" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D96" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E96" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F96" s="6"/>
       <c r="G96" s="6"/>
       <c r="H96" s="6"/>
       <c r="I96" s="6"/>
@@ -3236,66 +3381,73 @@
       <c r="AA96" s="6"/>
       <c r="AB96" s="6"/>
       <c r="AC96" s="6"/>
-    </row>
-    <row r="97" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="AD96" s="6"/>
+    </row>
+    <row r="97" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
       <c r="A97" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B97" s="8"/>
+      <c r="D97" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="E97" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="D97" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E97" s="8" t="s">
+    </row>
+    <row r="98" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A98" s="8" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A98" s="8" t="s">
+      <c r="B98" s="8"/>
+      <c r="D98" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="C98" s="6" t="s">
+      <c r="E98" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F98" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="D98" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E98" s="8" t="s">
+    </row>
+    <row r="99" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A99" s="8" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A99" s="8" t="s">
+      <c r="B99" s="8"/>
+      <c r="D99" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="C99" s="6" t="s">
+      <c r="E99" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F99" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="D99" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E99" s="8" t="s">
+    </row>
+    <row r="100" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A100" s="8" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A100" s="8" t="s">
+      <c r="B100" s="8"/>
+      <c r="D100" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="E100" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F100" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="D100" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="101" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:K100"/>
+  <autoFilter ref="A1:L100">
+    <filterColumn colId="1"/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Update DQC_0001 List of Axes (documentation)
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="302">
   <si>
     <t>Rule element ID</t>
   </si>
@@ -287,9 +287,6 @@
     <t>Equity Components [Axis]</t>
   </si>
   <si>
-    <t>WarrantsNotSettleableInCashMember, ContingentConsiderationClassifiedAsEquityMember, EquityIssuedInBusinessCombinationMember, TrustForBenefitOfEmployeesMember</t>
-  </si>
-  <si>
     <t>DQC_0001.76</t>
   </si>
   <si>
@@ -902,9 +899,6 @@
     <t>Customer [Axis]</t>
   </si>
   <si>
-    <t>Release Adopted</t>
-  </si>
-  <si>
     <t>Taxonomy Added</t>
   </si>
   <si>
@@ -921,6 +915,15 @@
   </si>
   <si>
     <t>Hotel [Member]</t>
+  </si>
+  <si>
+    <t>Release Adopted &amp; Updated</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>Before 2018: WarrantsNotSettleableInCashMember, ContingentConsiderationClassifiedAsEquityMember, EquityIssuedInBusinessCombinationMember, TrustForBenefitOfEmployeesMember; Added For 2018: AccumulatedNetGainLossFromCashFlowHedgesIncludingPortionAttributableToNoncontrollingInterestMember, AccumulatedNetGainLossFromDesignatedOrQualifyingCashFlowHedgesMember, AccumulatedNetGainLossFromCashFlowHedgesAttributableToNoncontrollingInterestMember</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1040,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1085,11 +1088,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1178,11 +1205,20 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1483,8 +1519,8 @@
   </sheetPr>
   <dimension ref="A1:AD991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1496,12 +1532,12 @@
     <col min="5" max="5" width="58.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="46.85546875" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" customWidth="1"/>
+    <col min="8" max="8" width="33.7109375" customWidth="1"/>
     <col min="10" max="10" width="54.85546875" customWidth="1"/>
     <col min="11" max="12" width="14.42578125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="6" customFormat="1" ht="28.5">
+    <row r="1" spans="1:29" s="6" customFormat="1" ht="44.25" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1532,11 +1568,11 @@
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="34" t="s">
-        <v>294</v>
-      </c>
-      <c r="L1" s="35" t="s">
-        <v>295</v>
+      <c r="K1" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="L1" s="34" t="s">
+        <v>293</v>
       </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -1583,7 +1619,7 @@
       <c r="J2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="31">
+      <c r="K2" s="36">
         <v>3</v>
       </c>
       <c r="L2" s="32"/>
@@ -1613,7 +1649,7 @@
         <v>21</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="31">
+      <c r="K3" s="37">
         <v>3</v>
       </c>
       <c r="L3" s="32"/>
@@ -1643,7 +1679,7 @@
         <v>15</v>
       </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="31">
+      <c r="K4" s="37">
         <v>3</v>
       </c>
       <c r="L4" s="32"/>
@@ -1677,7 +1713,7 @@
         <v>15</v>
       </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="31">
+      <c r="K5" s="37">
         <v>3</v>
       </c>
       <c r="L5" s="32"/>
@@ -1707,7 +1743,7 @@
         <v>15</v>
       </c>
       <c r="J6" s="10"/>
-      <c r="K6" s="31">
+      <c r="K6" s="37">
         <v>3</v>
       </c>
       <c r="L6" s="32"/>
@@ -1737,8 +1773,8 @@
         <v>15</v>
       </c>
       <c r="J7" s="10"/>
-      <c r="K7" s="31">
-        <v>3</v>
+      <c r="K7" s="38" t="s">
+        <v>300</v>
       </c>
       <c r="L7" s="32"/>
     </row>
@@ -1769,8 +1805,8 @@
         <v>15</v>
       </c>
       <c r="J8" s="10"/>
-      <c r="K8" s="31">
-        <v>3</v>
+      <c r="K8" s="38" t="s">
+        <v>300</v>
       </c>
       <c r="L8" s="32"/>
       <c r="M8" s="10"/>
@@ -1808,7 +1844,7 @@
         <v>15</v>
       </c>
       <c r="J9" s="10"/>
-      <c r="K9" s="31">
+      <c r="K9" s="37">
         <v>3</v>
       </c>
       <c r="L9" s="32"/>
@@ -1838,7 +1874,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="10"/>
-      <c r="K10" s="31">
+      <c r="K10" s="37">
         <v>3</v>
       </c>
       <c r="L10" s="32"/>
@@ -1870,8 +1906,8 @@
       <c r="J11" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="K11" s="31">
-        <v>3</v>
+      <c r="K11" s="38" t="s">
+        <v>300</v>
       </c>
       <c r="L11" s="32"/>
     </row>
@@ -1902,7 +1938,7 @@
       <c r="J12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="K12" s="31">
+      <c r="K12" s="37">
         <v>3</v>
       </c>
       <c r="L12" s="32"/>
@@ -1932,7 +1968,7 @@
         <v>21</v>
       </c>
       <c r="J13" s="10"/>
-      <c r="K13" s="31">
+      <c r="K13" s="37">
         <v>3</v>
       </c>
       <c r="L13" s="32"/>
@@ -1962,7 +1998,7 @@
         <v>21</v>
       </c>
       <c r="J14" s="10"/>
-      <c r="K14" s="31">
+      <c r="K14" s="37">
         <v>3</v>
       </c>
       <c r="L14" s="32"/>
@@ -1994,7 +2030,7 @@
       <c r="J15" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="K15" s="31">
+      <c r="K15" s="37">
         <v>3</v>
       </c>
       <c r="L15" s="32"/>
@@ -2022,14 +2058,14 @@
         <v>71</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="10"/>
-      <c r="K16" s="31">
-        <v>3</v>
+      <c r="K16" s="38" t="s">
+        <v>300</v>
       </c>
       <c r="L16" s="32"/>
     </row>
@@ -2060,8 +2096,8 @@
       <c r="J17" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="K17" s="31">
-        <v>3</v>
+      <c r="K17" s="38" t="s">
+        <v>300</v>
       </c>
       <c r="L17" s="32"/>
     </row>
@@ -2092,7 +2128,7 @@
         <v>15</v>
       </c>
       <c r="J18" s="10"/>
-      <c r="K18" s="31">
+      <c r="K18" s="37">
         <v>3</v>
       </c>
       <c r="L18" s="32"/>
@@ -2122,7 +2158,7 @@
         <v>15</v>
       </c>
       <c r="J19" s="10"/>
-      <c r="K19" s="31">
+      <c r="K19" s="37">
         <v>3</v>
       </c>
       <c r="L19" s="32"/>
@@ -2152,12 +2188,12 @@
         <v>21</v>
       </c>
       <c r="J20" s="10"/>
-      <c r="K20" s="31">
+      <c r="K20" s="37">
         <v>3</v>
       </c>
       <c r="L20" s="32"/>
     </row>
-    <row r="21" spans="1:30" s="24" customFormat="1" ht="72">
+    <row r="21" spans="1:30" s="24" customFormat="1" ht="204">
       <c r="A21" s="29" t="s">
         <v>86</v>
       </c>
@@ -2177,21 +2213,21 @@
         <v>15</v>
       </c>
       <c r="G21" s="30"/>
-      <c r="H21" s="30" t="s">
-        <v>89</v>
+      <c r="H21" s="31" t="s">
+        <v>301</v>
       </c>
       <c r="I21" s="29" t="s">
         <v>15</v>
       </c>
       <c r="J21" s="29"/>
-      <c r="K21" s="31">
-        <v>3</v>
+      <c r="K21" s="38" t="s">
+        <v>300</v>
       </c>
       <c r="L21" s="32"/>
     </row>
     <row r="22" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A22" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>11</v>
@@ -2200,10 +2236,10 @@
         <v>12</v>
       </c>
       <c r="D22" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="29" t="s">
         <v>91</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>92</v>
       </c>
       <c r="F22" s="29" t="s">
         <v>15</v>
@@ -2214,14 +2250,14 @@
         <v>15</v>
       </c>
       <c r="J22" s="29"/>
-      <c r="K22" s="31">
+      <c r="K22" s="37">
         <v>3</v>
       </c>
       <c r="L22" s="32"/>
     </row>
     <row r="23" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A23" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>11</v>
@@ -2230,10 +2266,10 @@
         <v>36</v>
       </c>
       <c r="D23" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="29" t="s">
         <v>94</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>95</v>
       </c>
       <c r="F23" s="29" t="s">
         <v>15</v>
@@ -2244,14 +2280,14 @@
         <v>21</v>
       </c>
       <c r="J23" s="29"/>
-      <c r="K23" s="31">
-        <v>3</v>
+      <c r="K23" s="38" t="s">
+        <v>300</v>
       </c>
       <c r="L23" s="32"/>
     </row>
     <row r="24" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A24" s="31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B24" s="31" t="s">
         <v>11</v>
@@ -2260,10 +2296,10 @@
         <v>12</v>
       </c>
       <c r="D24" s="31" t="s">
+        <v>281</v>
+      </c>
+      <c r="E24" s="31" t="s">
         <v>282</v>
-      </c>
-      <c r="E24" s="31" t="s">
-        <v>283</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>25</v>
@@ -2274,7 +2310,7 @@
         <v>15</v>
       </c>
       <c r="J24" s="31"/>
-      <c r="K24" s="31">
+      <c r="K24" s="37">
         <v>7</v>
       </c>
       <c r="L24" s="32"/>
@@ -2299,7 +2335,7 @@
     </row>
     <row r="25" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A25" s="31" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B25" s="31" t="s">
         <v>11</v>
@@ -2308,10 +2344,10 @@
         <v>12</v>
       </c>
       <c r="D25" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="E25" s="31" t="s">
         <v>285</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>286</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>25</v>
@@ -2322,7 +2358,7 @@
         <v>15</v>
       </c>
       <c r="J25" s="31"/>
-      <c r="K25" s="31">
+      <c r="K25" s="37">
         <v>7</v>
       </c>
       <c r="L25" s="31">
@@ -2349,19 +2385,19 @@
     </row>
     <row r="26" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A26" s="31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B26" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="31" t="s">
+        <v>287</v>
+      </c>
+      <c r="D26" s="33" t="s">
         <v>288</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="E26" s="31" t="s">
         <v>289</v>
-      </c>
-      <c r="E26" s="31" t="s">
-        <v>290</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>25</v>
@@ -2372,7 +2408,7 @@
         <v>15</v>
       </c>
       <c r="J26" s="31"/>
-      <c r="K26" s="31">
+      <c r="K26" s="37">
         <v>7</v>
       </c>
       <c r="L26" s="31">
@@ -2399,19 +2435,19 @@
     </row>
     <row r="27" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A27" s="31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B27" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D27" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="E27" s="31" t="s">
         <v>292</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>293</v>
       </c>
       <c r="F27" s="31" t="s">
         <v>25</v>
@@ -2422,7 +2458,7 @@
         <v>15</v>
       </c>
       <c r="J27" s="31"/>
-      <c r="K27" s="31">
+      <c r="K27" s="37">
         <v>7</v>
       </c>
       <c r="L27" s="32"/>
@@ -2512,7 +2548,7 @@
     </row>
     <row r="32" spans="1:30" s="11" customFormat="1" ht="16.5">
       <c r="A32" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -2546,7 +2582,7 @@
     </row>
     <row r="33" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A33" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -2557,259 +2593,259 @@
         <v>2</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K33" s="32"/>
       <c r="L33" s="32"/>
     </row>
     <row r="34" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A34" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K34" s="32"/>
       <c r="L34" s="32"/>
     </row>
     <row r="35" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A35" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K35" s="32"/>
       <c r="L35" s="32"/>
     </row>
     <row r="36" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A36" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E36" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K36" s="32"/>
       <c r="L36" s="32"/>
     </row>
     <row r="37" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A37" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K37" s="32"/>
       <c r="L37" s="32"/>
     </row>
     <row r="38" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A38" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K38" s="32"/>
       <c r="L38" s="32"/>
     </row>
     <row r="39" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A39" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K39" s="32"/>
       <c r="L39" s="32"/>
     </row>
     <row r="40" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A40" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E40" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K40" s="32"/>
       <c r="L40" s="32"/>
     </row>
     <row r="41" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A41" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K41" s="32"/>
       <c r="L41" s="32"/>
     </row>
     <row r="42" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A42" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E42" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K42" s="32"/>
       <c r="L42" s="32"/>
     </row>
     <row r="43" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A43" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E43" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K43" s="32"/>
       <c r="L43" s="32"/>
     </row>
     <row r="44" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A44" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E44" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K44" s="32"/>
       <c r="L44" s="32"/>
     </row>
     <row r="45" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A45" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E45" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K45" s="32"/>
       <c r="L45" s="32"/>
     </row>
     <row r="46" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A46" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K46" s="32"/>
       <c r="L46" s="32"/>
     </row>
     <row r="47" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A47" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E47" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K47" s="32"/>
       <c r="L47" s="32"/>
@@ -2820,14 +2856,14 @@
     </row>
     <row r="49" spans="1:12" s="11" customFormat="1" ht="16.5">
       <c r="A49" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K49" s="32"/>
       <c r="L49" s="32"/>
     </row>
     <row r="50" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A50" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B50" s="18"/>
       <c r="C50" s="18"/>
@@ -2838,159 +2874,159 @@
         <v>2</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K50" s="32"/>
       <c r="L50" s="32"/>
     </row>
     <row r="51" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A51" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
       <c r="D51" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E51" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="F51" s="10" t="s">
         <v>144</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>145</v>
       </c>
       <c r="K51" s="32"/>
       <c r="L51" s="32"/>
     </row>
     <row r="52" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A52" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
       <c r="D52" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F52" s="10" t="s">
         <v>147</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>148</v>
       </c>
       <c r="K52" s="32"/>
       <c r="L52" s="32"/>
     </row>
     <row r="53" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A53" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
       <c r="D53" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F53" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>151</v>
       </c>
       <c r="K53" s="32"/>
       <c r="L53" s="32"/>
     </row>
     <row r="54" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A54" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F54" s="10" t="s">
         <v>153</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>154</v>
       </c>
       <c r="K54" s="32"/>
       <c r="L54" s="32"/>
     </row>
     <row r="55" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A55" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="D55" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="D55" s="21" t="s">
+      <c r="E55" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F55" s="21" t="s">
         <v>156</v>
-      </c>
-      <c r="E55" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="F55" s="21" t="s">
-        <v>157</v>
       </c>
       <c r="K55" s="32"/>
       <c r="L55" s="32"/>
     </row>
     <row r="56" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A56" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="D56" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="D56" s="21" t="s">
+      <c r="E56" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F56" s="21" t="s">
         <v>159</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="F56" s="21" t="s">
-        <v>160</v>
       </c>
       <c r="K56" s="32"/>
       <c r="L56" s="32"/>
     </row>
     <row r="57" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A57" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="D57" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="D57" s="21" t="s">
+      <c r="E57" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F57" s="21" t="s">
         <v>162</v>
-      </c>
-      <c r="E57" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="F57" s="21" t="s">
-        <v>163</v>
       </c>
       <c r="K57" s="32"/>
       <c r="L57" s="32"/>
     </row>
     <row r="58" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A58" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="D58" s="21" t="s">
+      <c r="E58" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F58" s="21" t="s">
         <v>165</v>
-      </c>
-      <c r="E58" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="F58" s="21" t="s">
-        <v>166</v>
       </c>
       <c r="K58" s="32"/>
       <c r="L58" s="32"/>
     </row>
     <row r="59" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A59" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="D59" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="D59" s="21" t="s">
+      <c r="E59" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F59" s="21" t="s">
         <v>168</v>
-      </c>
-      <c r="E59" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="F59" s="21" t="s">
-        <v>169</v>
       </c>
       <c r="K59" s="32"/>
       <c r="L59" s="32"/>
@@ -3002,14 +3038,14 @@
     </row>
     <row r="61" spans="1:12" s="11" customFormat="1" ht="16.5">
       <c r="A61" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K61" s="32"/>
       <c r="L61" s="32"/>
     </row>
     <row r="62" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A62" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B62" s="18"/>
       <c r="C62" s="18"/>
@@ -3020,495 +3056,495 @@
         <v>2</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K62" s="32"/>
       <c r="L62" s="32"/>
     </row>
     <row r="63" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A63" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E63" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K63" s="32"/>
       <c r="L63" s="32"/>
     </row>
     <row r="64" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A64" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E64" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K64" s="32"/>
       <c r="L64" s="32"/>
     </row>
     <row r="65" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A65" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E65" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K65" s="32"/>
       <c r="L65" s="32"/>
     </row>
     <row r="66" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A66" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E66" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K66" s="32"/>
       <c r="L66" s="32"/>
     </row>
     <row r="67" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A67" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K67" s="32"/>
       <c r="L67" s="32"/>
     </row>
     <row r="68" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A68" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E68" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K68" s="32"/>
       <c r="L68" s="32"/>
     </row>
     <row r="69" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A69" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E69" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K69" s="32"/>
       <c r="L69" s="32"/>
     </row>
     <row r="70" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A70" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E70" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K70" s="32"/>
       <c r="L70" s="32"/>
     </row>
     <row r="71" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A71" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E71" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K71" s="32"/>
       <c r="L71" s="32"/>
     </row>
     <row r="72" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A72" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E72" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K72" s="32"/>
       <c r="L72" s="32"/>
     </row>
     <row r="73" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A73" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
       <c r="D73" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E73" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K73" s="32"/>
       <c r="L73" s="32"/>
     </row>
     <row r="74" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A74" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E74" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K74" s="32"/>
       <c r="L74" s="32"/>
     </row>
     <row r="75" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A75" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E75" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K75" s="32"/>
       <c r="L75" s="32"/>
     </row>
     <row r="76" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A76" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
       <c r="D76" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K76" s="32"/>
       <c r="L76" s="32"/>
     </row>
     <row r="77" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A77" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K77" s="32"/>
       <c r="L77" s="32"/>
     </row>
     <row r="78" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A78" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
       <c r="D78" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F78" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K78" s="32"/>
       <c r="L78" s="32"/>
     </row>
     <row r="79" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A79" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
       <c r="D79" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K79" s="32"/>
       <c r="L79" s="32"/>
     </row>
     <row r="80" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A80" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
       <c r="D80" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E80" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K80" s="32"/>
       <c r="L80" s="32"/>
     </row>
     <row r="81" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A81" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
       <c r="D81" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E81" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K81" s="32"/>
       <c r="L81" s="32"/>
     </row>
     <row r="82" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A82" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
       <c r="D82" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K82" s="32"/>
       <c r="L82" s="32"/>
     </row>
     <row r="83" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A83" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
       <c r="D83" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K83" s="32"/>
       <c r="L83" s="32"/>
     </row>
     <row r="84" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A84" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
       <c r="D84" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E84" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K84" s="32"/>
       <c r="L84" s="32"/>
     </row>
     <row r="85" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A85" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
       <c r="D85" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F85" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K85" s="32"/>
       <c r="L85" s="32"/>
     </row>
     <row r="86" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A86" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="D86" s="21" t="s">
         <v>240</v>
-      </c>
-      <c r="D86" s="21" t="s">
-        <v>241</v>
       </c>
       <c r="E86" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F86" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K86" s="32"/>
       <c r="L86" s="32"/>
     </row>
     <row r="87" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A87" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D87" s="21" t="s">
         <v>243</v>
-      </c>
-      <c r="D87" s="21" t="s">
-        <v>244</v>
       </c>
       <c r="E87" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F87" s="21" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K87" s="32"/>
       <c r="L87" s="32"/>
     </row>
     <row r="88" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A88" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="D88" s="21" t="s">
         <v>246</v>
-      </c>
-      <c r="D88" s="21" t="s">
-        <v>247</v>
       </c>
       <c r="E88" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F88" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K88" s="32"/>
       <c r="L88" s="32"/>
     </row>
     <row r="89" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A89" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="D89" s="21" t="s">
         <v>249</v>
-      </c>
-      <c r="D89" s="21" t="s">
-        <v>250</v>
       </c>
       <c r="E89" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F89" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K89" s="32"/>
       <c r="L89" s="32"/>
     </row>
     <row r="90" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A90" s="22" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E90" s="27" t="s">
         <v>12</v>
@@ -3519,12 +3555,12 @@
     </row>
     <row r="91" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A91" s="26" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B91" s="26"/>
       <c r="C91" s="26"/>
       <c r="D91" s="26" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E91" s="26" t="s">
         <v>12</v>
@@ -3562,14 +3598,14 @@
     </row>
     <row r="93" spans="1:30" s="11" customFormat="1" ht="16.5">
       <c r="A93" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K93" s="32"/>
       <c r="L93" s="32"/>
     </row>
     <row r="94" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A94" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B94" s="18"/>
       <c r="C94" s="18"/>
@@ -3580,7 +3616,7 @@
         <v>2</v>
       </c>
       <c r="F94" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G94" s="10"/>
       <c r="H94" s="10"/>
@@ -3609,18 +3645,18 @@
     </row>
     <row r="95" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A95" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
       <c r="D95" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F95" s="10" t="s">
         <v>254</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F95" s="10" t="s">
-        <v>255</v>
       </c>
       <c r="G95" s="10"/>
       <c r="H95" s="10"/>
@@ -3649,18 +3685,18 @@
     </row>
     <row r="96" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A96" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F96" s="10" t="s">
         <v>257</v>
-      </c>
-      <c r="E96" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F96" s="10" t="s">
-        <v>258</v>
       </c>
       <c r="G96" s="10"/>
       <c r="H96" s="10"/>
@@ -3689,18 +3725,18 @@
     </row>
     <row r="97" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A97" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
       <c r="D97" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F97" s="10" t="s">
         <v>260</v>
-      </c>
-      <c r="E97" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F97" s="10" t="s">
-        <v>261</v>
       </c>
       <c r="G97" s="10"/>
       <c r="H97" s="10"/>
@@ -3729,18 +3765,18 @@
     </row>
     <row r="98" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A98" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
       <c r="D98" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F98" s="10" t="s">
         <v>263</v>
-      </c>
-      <c r="E98" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F98" s="10" t="s">
-        <v>264</v>
       </c>
       <c r="G98" s="10"/>
       <c r="H98" s="10"/>
@@ -3769,18 +3805,18 @@
     </row>
     <row r="99" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A99" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
       <c r="D99" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F99" s="10" t="s">
         <v>266</v>
-      </c>
-      <c r="E99" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F99" s="10" t="s">
-        <v>267</v>
       </c>
       <c r="G99" s="10"/>
       <c r="H99" s="10"/>
@@ -3841,7 +3877,7 @@
     </row>
     <row r="101" spans="1:30" s="11" customFormat="1" ht="16.5">
       <c r="A101" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B101" s="10"/>
       <c r="C101" s="10"/>
@@ -3875,7 +3911,7 @@
     </row>
     <row r="102" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A102" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B102" s="18"/>
       <c r="C102" s="18"/>
@@ -3886,7 +3922,7 @@
         <v>2</v>
       </c>
       <c r="F102" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G102" s="10"/>
       <c r="H102" s="10"/>
@@ -3915,64 +3951,64 @@
     </row>
     <row r="103" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A103" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="D103" s="10" t="s">
         <v>269</v>
-      </c>
-      <c r="D103" s="10" t="s">
-        <v>270</v>
       </c>
       <c r="E103" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F103" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K103" s="32"/>
       <c r="L103" s="32"/>
     </row>
     <row r="104" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A104" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="D104" s="10" t="s">
         <v>272</v>
-      </c>
-      <c r="D104" s="10" t="s">
-        <v>273</v>
       </c>
       <c r="E104" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F104" s="21" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K104" s="32"/>
       <c r="L104" s="32"/>
     </row>
     <row r="105" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A105" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="D105" s="10" t="s">
         <v>275</v>
-      </c>
-      <c r="D105" s="10" t="s">
-        <v>276</v>
       </c>
       <c r="E105" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F105" s="21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K105" s="32"/>
       <c r="L105" s="32"/>
     </row>
     <row r="106" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A106" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="D106" s="21" t="s">
         <v>278</v>
-      </c>
-      <c r="D106" s="21" t="s">
-        <v>279</v>
       </c>
       <c r="E106" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K106" s="32"/>
       <c r="L106" s="32"/>

</xml_diff>

<commit_message>
Additional updates from v7 Public Review (#357)
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -244,686 +244,686 @@
     <t>Consolidation Items [Axis]</t>
   </si>
   <si>
-    <t xml:space="preserve">CorporateReconcilingItemsAndEliminationsMember, CorporateAndReconcilingItemsMember, CorporateAndEliminationsMember, EliminationsAndReconcilingItemsMember, OperatingSegmentsAndCorporateNonSegmentMember
+    <t>DQC_0001.71</t>
+  </si>
+  <si>
+    <t>DefinedBenefitPlanByPlanAssetCategoriesAxis</t>
+  </si>
+  <si>
+    <t>Defined Benefit Plan, Asset Categories [Axis]</t>
+  </si>
+  <si>
+    <t>All - except members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis (Not applicable after 2016);  All - except members on: RetirementPlanTypeAxis, RetirementPlanSponsorLocationAxis, RetirementPlanTaxStatusAxis, RetirementPlanFundingStatusAxis, RetirementPlanNameAxis (After 2016)</t>
+  </si>
+  <si>
+    <t>DQC_0001.72</t>
+  </si>
+  <si>
+    <t>AwardDateAxis</t>
+  </si>
+  <si>
+    <t>Award Date [Axis]</t>
+  </si>
+  <si>
+    <t>DQC_0001.74</t>
+  </si>
+  <si>
+    <t>SubsequentEventTypeAxis</t>
+  </si>
+  <si>
+    <t>Subsequent Event Type [Axis]</t>
+  </si>
+  <si>
+    <t>DQC_0001.75</t>
+  </si>
+  <si>
+    <t>StatementEquityComponentsAxis</t>
+  </si>
+  <si>
+    <t>Equity Components [Axis]</t>
+  </si>
+  <si>
+    <t>DQC_0001.76</t>
+  </si>
+  <si>
+    <t>StatementScenarioAxis</t>
+  </si>
+  <si>
+    <t>Scenario [Axis]</t>
+  </si>
+  <si>
+    <t>DQC_0001.61</t>
+  </si>
+  <si>
+    <t>RangeAxis</t>
+  </si>
+  <si>
+    <t>Range [Axis]</t>
+  </si>
+  <si>
+    <t>Note 1 - Allowable US-GAAP members on the CounterpartyNameAxis</t>
+  </si>
+  <si>
+    <t>Element Name</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>AffiliatedEntityMember</t>
+  </si>
+  <si>
+    <t>Affiliated Entity [Member]</t>
+  </si>
+  <si>
+    <t>An affiliate is a party that, directly or indirectly through one or more intermediaries, controls, is controlled by, or is under common control with the entity.</t>
+  </si>
+  <si>
+    <t>InvestorMember</t>
+  </si>
+  <si>
+    <t>Investor [Member]</t>
+  </si>
+  <si>
+    <t>Business entity or individual that puts money, by purchase or expenditure, in something offering potential profitable returns, such as interest income or appreciation in value.</t>
+  </si>
+  <si>
+    <t>VariableInterestEntityNotPrimaryBeneficiaryMember</t>
+  </si>
+  <si>
+    <t>Variable Interest Entity, Not Primary Beneficiary [Member]</t>
+  </si>
+  <si>
+    <t>Variable Interest Entities (VIE) in which the entity does not have a controlling financial interest (as defined) and of which it is therefore not the primary beneficiary. VIEs of which the entity is not the primary beneficiary because it does not have the power to direct the activities of the VIE that most significantly impact the VIE's economic performance and for which it does not have the obligation to absorb losses of the VIE that could potentially be significant to the VIE or the right to receive benefits from the VIE that could potentially be significant to the VIE are not included in the consolidated financial statements of the entity.</t>
+  </si>
+  <si>
+    <t>ChiefFinancialOfficerMember</t>
+  </si>
+  <si>
+    <t>Chief Financial Officer [Member]</t>
+  </si>
+  <si>
+    <t>Senior executive officer responsible for overseeing the financial activities of the entity.</t>
+  </si>
+  <si>
+    <t>IndividualMember</t>
+  </si>
+  <si>
+    <t>Individual Counterparty [Member]</t>
+  </si>
+  <si>
+    <t>Individual person that is legally permitted to enter into a contract and be sued if that person fails to meet the obligations imposed by a contract.</t>
+  </si>
+  <si>
+    <t>GovernmentMember</t>
+  </si>
+  <si>
+    <t>Government [Member]</t>
+  </si>
+  <si>
+    <t>Organization that is the governing authority of a community.</t>
+  </si>
+  <si>
+    <t>GuarantorSubsidiariesMember</t>
+  </si>
+  <si>
+    <t>Guarantor Subsidiaries [Member]</t>
+  </si>
+  <si>
+    <t>Entity owned or controlled by another entity which has guaranteed the issue of securities by another subsidiary of the parent or has guaranteed the issue of securities by the parent.</t>
+  </si>
+  <si>
+    <t>SubsidiaryIssuerMember</t>
+  </si>
+  <si>
+    <t>Subsidiary Issuer [Member]</t>
+  </si>
+  <si>
+    <t>A company controlled, directly or indirectly, by its parent, which has issued securities and those securities are guaranteed by its parent and another subsidiary of the parent.</t>
+  </si>
+  <si>
+    <t>DirectorMember</t>
+  </si>
+  <si>
+    <t>Director [Member]</t>
+  </si>
+  <si>
+    <t>Person serving on the board of directors (who collectively have responsibility for governing the entity).</t>
+  </si>
+  <si>
+    <t>ChiefExecutiveOfficerMember</t>
+  </si>
+  <si>
+    <t>Chief Executive Officer [Member]</t>
+  </si>
+  <si>
+    <t>Highest ranking executive officer, who has ultimate managerial responsibility for the entity and who reports to the board of directors. In addition, the chief executive officer (CEO) may also be the chairman of the board or president.</t>
+  </si>
+  <si>
+    <t>ChiefOperatingOfficerMember</t>
+  </si>
+  <si>
+    <t>Chief Operating Officer [Member]</t>
+  </si>
+  <si>
+    <t>Senior executive officer responsible for management of day-to-day activities of the entity.</t>
+  </si>
+  <si>
+    <t>GeneralPartnerMember</t>
+  </si>
+  <si>
+    <t>General Partner [Member]</t>
+  </si>
+  <si>
+    <t>Party to a partnership business who has unlimited liability.</t>
+  </si>
+  <si>
+    <t>CorporateJointVentureMember</t>
+  </si>
+  <si>
+    <t>Corporate Joint Venture [Member]</t>
+  </si>
+  <si>
+    <t>Corporation owned and operated by a small group of ventures to accomplish a mutually beneficial venture or project.</t>
+  </si>
+  <si>
+    <t>SubsidiaryOfCommonParentMember</t>
+  </si>
+  <si>
+    <t>Subsidiary of Common Parent [Member]</t>
+  </si>
+  <si>
+    <t>Refers to an entity under the control of the same parent as another entity (that is, a sister company).</t>
+  </si>
+  <si>
+    <t>Note 2 - Allowable extension members on the CurrencyAxis</t>
+  </si>
+  <si>
+    <t>SICAD1Member</t>
+  </si>
+  <si>
+    <t>SICA D1 [Member]</t>
+  </si>
+  <si>
+    <t>extension</t>
+  </si>
+  <si>
+    <t>Venezuelan complementary currency exchange system, Sistema Complementario de Administracion de Divisas 1</t>
+  </si>
+  <si>
+    <t>SICAD2Member</t>
+  </si>
+  <si>
+    <t>SICA D2 [Member]</t>
+  </si>
+  <si>
+    <t>Venezuelan complementary currency exchange system, Sistema Complementario de Administracion de Divisas 2</t>
+  </si>
+  <si>
+    <t>OtherCurrencyMember</t>
+  </si>
+  <si>
+    <t>Other [Member]</t>
+  </si>
+  <si>
+    <t>Represents all other currencies not specifically defined.</t>
+  </si>
+  <si>
+    <t>NonUSDollarMember</t>
+  </si>
+  <si>
+    <t>Non-U.S. Dollar [Member]</t>
+  </si>
+  <si>
+    <t>Represents all other currencies that are not USD.</t>
+  </si>
+  <si>
+    <t>CENCOEXMember</t>
+  </si>
+  <si>
+    <t>CENCOEX [Member]</t>
+  </si>
+  <si>
+    <t>The official Venezuelan exchange rate offered by the National Foreign Trade Center. (CENCOEX)</t>
+  </si>
+  <si>
+    <t>SICADMember</t>
+  </si>
+  <si>
+    <t>SICAD [Member]</t>
+  </si>
+  <si>
+    <t>The Venezuelan exchange rate available to companies importing essential goods (e.g., certain food, medicine, raw materials). Consolidates SICAD 1 and SICAD 2.</t>
+  </si>
+  <si>
+    <t>SIMADIMember</t>
+  </si>
+  <si>
+    <t>SIMADI [Member]</t>
+  </si>
+  <si>
+    <t>The market based Venezuelan Exchange Rate.</t>
+  </si>
+  <si>
+    <t>DIPROMember</t>
+  </si>
+  <si>
+    <t>DIPRO [Member]</t>
+  </si>
+  <si>
+    <t>Venezuelan Exchange Rate that replaced the SICAD on March 10, 2016.  The DIPRO, is used for payments of critical importance such as healthcare.</t>
+  </si>
+  <si>
+    <t>DICOMMember</t>
+  </si>
+  <si>
+    <t>DICON [Member]</t>
+  </si>
+  <si>
+    <t>Venezuelan Exchange Rate that replaced the SIMADI on March 10, 2016.  The DICOM, fluctuates according to market supply and demand.</t>
+  </si>
+  <si>
+    <t>Note 3 - Allowable US-GAAP members on the ProductOrServiceAxis</t>
+  </si>
+  <si>
+    <t>AuctionRateSecuritiesMember</t>
+  </si>
+  <si>
+    <t>Auction Rate Securities [Member]</t>
+  </si>
+  <si>
+    <t>Debt instrument securities (for example, but not limited to, corporate or municipal bonds) that typically have long-term nominal maturities for which the interest rate is reset through an auction process.</t>
+  </si>
+  <si>
+    <t>AutomobileLoanMember</t>
+  </si>
+  <si>
+    <t>Automobile Loan [Member]</t>
+  </si>
+  <si>
+    <t>Loan to finance the purchase of a vehicle.</t>
+  </si>
+  <si>
+    <t>CommercialLoanMember</t>
+  </si>
+  <si>
+    <t>Commercial Loan [Member]</t>
+  </si>
+  <si>
+    <t>A loan, whether secured or unsecured, to a company for purposes such as seasonal working capital needs, inventory financing, equipment purchases and acquisitions.</t>
+  </si>
+  <si>
+    <t>CommercialRealEstateMember</t>
+  </si>
+  <si>
+    <t>Commercial Real Estate [Member]</t>
+  </si>
+  <si>
+    <t>Property that is solely used for business purposes.</t>
+  </si>
+  <si>
+    <t>ConstructionLoansMember</t>
+  </si>
+  <si>
+    <t>Construction Loans [Member]</t>
+  </si>
+  <si>
+    <t>A borrowing arrangement which provides the entity constructing a facility (such as a building and a landfill) with funds to effect construction, generally on a draw down, or as needed, basis.</t>
+  </si>
+  <si>
+    <t>ConsumerLoanMember</t>
+  </si>
+  <si>
+    <t>Consumer Loan [Member]</t>
+  </si>
+  <si>
+    <t>Loan or extension of credit for personal, family, or household use excluding real estate.</t>
+  </si>
+  <si>
+    <t>CrudeOilMember</t>
+  </si>
+  <si>
+    <t>Crude Oil [Member]</t>
+  </si>
+  <si>
+    <t>Unrefined, unprocessed oil, which may be used in a variety of applications, and from which, petroleum-based products are produced.</t>
+  </si>
+  <si>
+    <t>FuelMember</t>
+  </si>
+  <si>
+    <t>Fuel [Member]</t>
+  </si>
+  <si>
+    <t>Represents material used for the production of energy in the form of heat or power. Examples may include, but not be limited to heating, transpiration, etc.</t>
+  </si>
+  <si>
+    <t>GeneralLiabilityMember</t>
+  </si>
+  <si>
+    <t>General Liability [Member]</t>
+  </si>
+  <si>
+    <t>Type of business insurance which provides insurance coverage for a wide variety of liability exposures including, but not limited to, contractual liability, product liability and personal injury liability.</t>
+  </si>
+  <si>
+    <t>HeatingOilMember</t>
+  </si>
+  <si>
+    <t>Heating Oil [Member]</t>
+  </si>
+  <si>
+    <t>Fuel oil used to produce heat in an office, plant, or any other location where temperature is controlled or managed.</t>
+  </si>
+  <si>
+    <t>HomeEquityLoanMember</t>
+  </si>
+  <si>
+    <t>Home Equity Loan [Member]</t>
+  </si>
+  <si>
+    <t>Loan based on the equity of the borrower's residential property in which the borrower receives the loan amount upfront. Excludes home equity lines of credit.</t>
+  </si>
+  <si>
+    <t>HomeEquityMember</t>
+  </si>
+  <si>
+    <t>Home Equity Line of Credit [Member]</t>
+  </si>
+  <si>
+    <t>Revolving, open-end loan extended under a line of credit and secured by the borrower's residential property.</t>
+  </si>
+  <si>
+    <t>LetterOfCreditMember</t>
+  </si>
+  <si>
+    <t>Letter of Credit [Member]</t>
+  </si>
+  <si>
+    <t>A document typically issued by a financial institution which acts as a guarantee of payment to a beneficiary, or as the source of payment for a specific transaction (for example, wiring funds to a foreign exporter if and when specified merchandise is accepted pursuant to the terms of the letter of credit).</t>
+  </si>
+  <si>
+    <t>LineOfCreditMember</t>
+  </si>
+  <si>
+    <t>Line of Credit [Member]</t>
+  </si>
+  <si>
+    <t>A contractual arrangement with a lender under which borrowings can be made up to a specific amount at any point in time, and under which borrowings outstanding may be either short-term or long-term, depending upon the particulars.</t>
+  </si>
+  <si>
+    <t>LoansMember</t>
+  </si>
+  <si>
+    <t>Loans [Member]</t>
+  </si>
+  <si>
+    <t>When a lender gives money or property over other debt securities sold by the issuer. In the event the issuer goes bankrupt, senior debt holders receive priority for [must receive] repayment [prior] relative to junior and unsecured (general) creditors.</t>
+  </si>
+  <si>
+    <t>MortgageLoansOnRealEstateMember</t>
+  </si>
+  <si>
+    <t>Mortgage Loans on Real Estate [Member] (Deprecated 2015-01-31)</t>
+  </si>
+  <si>
+    <t>A loan to finance the purchase of real estate where the lender has a lien on the property as collateral for the loan.</t>
+  </si>
+  <si>
+    <t>NaturalGasLiquidsReservesMember</t>
+  </si>
+  <si>
+    <t>Natural Gas Liquids [Member]</t>
+  </si>
+  <si>
+    <t>Natural gas liquids that include, but are not limited to, ethane, propane, natural gasoline, butane and isobutane.</t>
+  </si>
+  <si>
+    <t>NaturalGasReservesMember</t>
+  </si>
+  <si>
+    <t>Natural Gas [Member]</t>
+  </si>
+  <si>
+    <t>Natural gas composed primarily of methane gas, excluding liquid or condensate natural gas.</t>
+  </si>
+  <si>
+    <t>OilReservesMember</t>
+  </si>
+  <si>
+    <t>Oil [Member]</t>
+  </si>
+  <si>
+    <t>Crude oil, which may also include condensate and natural gas liquids.</t>
+  </si>
+  <si>
+    <t>ProfessionalMalpracticeLiabilityMember</t>
+  </si>
+  <si>
+    <t>Professional Malpractice Liability Insurance [Member]</t>
+  </si>
+  <si>
+    <t>Business insurance coverage for professionals, such as doctors, lawyers, insurance agents, accountants, real estate agents, veterinarians, and others. This liability coverage insures losses for claims arising from mistakes and errors or omissions in the course of professional activities.</t>
+  </si>
+  <si>
+    <t>RealEstateLoanMember</t>
+  </si>
+  <si>
+    <t>Real Estate Loan [Member]</t>
+  </si>
+  <si>
+    <t>Loan to finance the purchase of real estate, including but not limited to, land or building.</t>
+  </si>
+  <si>
+    <t>ResidentialMortgageMember</t>
+  </si>
+  <si>
+    <t>Residential Mortgage [Member]</t>
+  </si>
+  <si>
+    <t>Loan to purchase or refinance residential real estate for example, but not limited to, a home, in which the real estate itself serves as collateral for the loan.</t>
+  </si>
+  <si>
+    <t>SyntheticOilMember</t>
+  </si>
+  <si>
+    <t>Synthetic Oil [Member]</t>
+  </si>
+  <si>
+    <t>Lubricant consisting of chemical compounds that are synthetically made.</t>
+  </si>
+  <si>
+    <t>PublicUtilitiesInventoryWaterMember</t>
+  </si>
+  <si>
+    <t>Water [Member]</t>
+  </si>
+  <si>
+    <t>Clear, colorless, odorless and tasteless liquid essential for most plant and animal life comprised of two parts hydrogen and one part oxygen (H2O).</t>
+  </si>
+  <si>
+    <t>PublicUtilitiesInventoryPropaneMember</t>
+  </si>
+  <si>
+    <t>Propane [Member]</t>
+  </si>
+  <si>
+    <t>Product derived from petroleum during the processing of oil or natural gas which is then used as a heat source or fuel.</t>
+  </si>
+  <si>
+    <t>ResidentialRealEstateMember</t>
+  </si>
+  <si>
+    <t>Residential Real Estate [Member]</t>
+  </si>
+  <si>
+    <t>Property that is used as a home.</t>
+  </si>
+  <si>
+    <t>AutomobilesMember</t>
+  </si>
+  <si>
+    <t>Automobiles [Member]</t>
+  </si>
+  <si>
+    <t>Vehicles that are used primarily for transporting people.</t>
+  </si>
+  <si>
+    <t>Note 4 - Allowable US-GAAP Members on the ConsolidationItemsAxis</t>
+  </si>
+  <si>
+    <t>CorporateReconcilingItemsAndEliminationsMember</t>
+  </si>
+  <si>
+    <t>Eliminations, Corporate and Reconciling Items [Member]</t>
+  </si>
+  <si>
+    <t>Represents the aggregate total of adjustments for non operating corporate items, reconciling items and eliminations.</t>
+  </si>
+  <si>
+    <t>CorporateAndReconcilingItemsMember</t>
+  </si>
+  <si>
+    <t>Corporate and Reconciling Items [Member]</t>
+  </si>
+  <si>
+    <t>Represents the aggregate total of non operating corporate items and reconciling items</t>
+  </si>
+  <si>
+    <t>CorporateAndEliminationsMember</t>
+  </si>
+  <si>
+    <t>Corporate and Eliminations [Member]</t>
+  </si>
+  <si>
+    <t>Represents the aggregate total of non operating corporate items and elimination items</t>
+  </si>
+  <si>
+    <t>EliminationsAndReconcilingItemsMember</t>
+  </si>
+  <si>
+    <t>Eliminations and Reconciling Items [Member]</t>
+  </si>
+  <si>
+    <t>Represents the aggregate total of reconciling items and elimination items</t>
+  </si>
+  <si>
+    <t>OperatingSegmentsAndCorporateNonSegmentMember</t>
+  </si>
+  <si>
+    <t>Operating Segments and Corporate Non Segment [Member]</t>
+  </si>
+  <si>
+    <t>Represents the aggregate total of “Operating Segments” and “Corporate, Non-Segment”, before elimination and reconciliation items.</t>
+  </si>
+  <si>
+    <t>Note 5 - Allowable US-GAAP Members on the StatementEquityComponentsAxis</t>
+  </si>
+  <si>
+    <t>WarrantsNotSettleableInCashMember</t>
+  </si>
+  <si>
+    <t>Warrants Not Settleable in Cash [Member]</t>
+  </si>
+  <si>
+    <t>Warrants not settleable in cash that are classified in shareholders' equity.</t>
+  </si>
+  <si>
+    <t>ContingentConsiderationClassifiedAsEquityMember</t>
+  </si>
+  <si>
+    <t>Contingent Consideration Classified as Equity [Member]</t>
+  </si>
+  <si>
+    <t>Contingent consideration in a business combination that is classified in shareholders' equity.</t>
+  </si>
+  <si>
+    <t>EquityIssuedInBusinessCombinationMember</t>
+  </si>
+  <si>
+    <t>Equity Issued in Business Combination [Member]</t>
+  </si>
+  <si>
+    <t>Equity issued by an entity in a business combination that is classified in shareholders' equity.</t>
+  </si>
+  <si>
+    <t>TrustForBenefitOfEmployeesMember</t>
+  </si>
+  <si>
+    <t>Trust for Benefit of Employees [Member]</t>
+  </si>
+  <si>
+    <t>Trust created by the entity that exists for the benefit of its employees, such as pension and profit-sharing trusts that are managed by or under the trusteeship of the entity's management.</t>
+  </si>
+  <si>
+    <t>DQC_0001.77</t>
+  </si>
+  <si>
+    <t>PreferredUnitsByNameAxis</t>
+  </si>
+  <si>
+    <t>Preferred Units by Name [Axis]</t>
+  </si>
+  <si>
+    <t>DQC_0001.78</t>
+  </si>
+  <si>
+    <t>RetirementPlanNameAxis</t>
+  </si>
+  <si>
+    <t>Retirement Plan Name [Axis]</t>
+  </si>
+  <si>
+    <t>DQC_0001.79</t>
+  </si>
+  <si>
+    <t>srt</t>
+  </si>
+  <si>
+    <t>OwnershipAxis</t>
+  </si>
+  <si>
+    <t>Ownership [Axis]</t>
+  </si>
+  <si>
+    <t>DQC_0001.80</t>
+  </si>
+  <si>
+    <t>MajorCustomersAxis</t>
+  </si>
+  <si>
+    <t>Customer [Axis]</t>
+  </si>
+  <si>
+    <t>Taxonomy Added</t>
+  </si>
+  <si>
+    <t>AuctionRateSecuritiesMember, AutomobileLoanMember, CommercialLoanMember, CommercialRealEstateMember, ConstructionLoansMember, ConsumerLoanMember, CrudeOilMember, FuelMember, GeneralLiabilityMember, HeatingOilMember, HomeEquityLoanMember, HomeEquityMember, LetterOfCreditMember, LineOfCreditMember, LoansMember, MortgageLoansOnRealEstateMember, NaturalGasLiquidsReservesMember, NaturalGasReservesMember, OilReservesMember, ProfessionalMalpracticeLiabilityMember, RealEstateLoanMember, ResidentialMortgageMember, SyntheticOilMember, PublicUtilitiesInventoryWaterMember, PublicUtilitiesInventoryPropaneMember, ResidentialRealEstateMember, RealEstateMember, AutomobilesMember, HotelMember</t>
+  </si>
+  <si>
+    <t>RealEstateMember</t>
+  </si>
+  <si>
+    <t>Real Estate [Member]</t>
+  </si>
+  <si>
+    <t>HotelMember</t>
+  </si>
+  <si>
+    <t>Hotel [Member]</t>
+  </si>
+  <si>
+    <t>Release Adopted &amp; Updated</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>Before 2018: WarrantsNotSettleableInCashMember, ContingentConsiderationClassifiedAsEquityMember, EquityIssuedInBusinessCombinationMember, TrustForBenefitOfEmployeesMember; Added For 2018: AccumulatedNetGainLossFromCashFlowHedgesIncludingPortionAttributableToNoncontrollingInterestMember, AccumulatedNetGainLossFromDesignatedOrQualifyingCashFlowHedgesMember, AccumulatedNetGainLossFromCashFlowHedgesAttributableToNoncontrollingInterestMember</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CorporateReconcilingItemsAndEliminationsMember, CorporateAndReconcilingItemsMember, CorporateAndEliminationsMember, EliminationsAndReconcilingItemsMember, OperatingSegmentsAndCorporateNonSegmentMember, OperatingSegmentsExcludingIntersegmentEliminationMember
 </t>
-  </si>
-  <si>
-    <t>DQC_0001.71</t>
-  </si>
-  <si>
-    <t>DefinedBenefitPlanByPlanAssetCategoriesAxis</t>
-  </si>
-  <si>
-    <t>Defined Benefit Plan, Asset Categories [Axis]</t>
-  </si>
-  <si>
-    <t>All - except members on DefinedBenefitPlansDisclosuresDefinedBenefitPlansAxis (Not applicable after 2016);  All - except members on: RetirementPlanTypeAxis, RetirementPlanSponsorLocationAxis, RetirementPlanTaxStatusAxis, RetirementPlanFundingStatusAxis, RetirementPlanNameAxis (After 2016)</t>
-  </si>
-  <si>
-    <t>DQC_0001.72</t>
-  </si>
-  <si>
-    <t>AwardDateAxis</t>
-  </si>
-  <si>
-    <t>Award Date [Axis]</t>
-  </si>
-  <si>
-    <t>DQC_0001.74</t>
-  </si>
-  <si>
-    <t>SubsequentEventTypeAxis</t>
-  </si>
-  <si>
-    <t>Subsequent Event Type [Axis]</t>
-  </si>
-  <si>
-    <t>DQC_0001.75</t>
-  </si>
-  <si>
-    <t>StatementEquityComponentsAxis</t>
-  </si>
-  <si>
-    <t>Equity Components [Axis]</t>
-  </si>
-  <si>
-    <t>DQC_0001.76</t>
-  </si>
-  <si>
-    <t>StatementScenarioAxis</t>
-  </si>
-  <si>
-    <t>Scenario [Axis]</t>
-  </si>
-  <si>
-    <t>DQC_0001.61</t>
-  </si>
-  <si>
-    <t>RangeAxis</t>
-  </si>
-  <si>
-    <t>Range [Axis]</t>
-  </si>
-  <si>
-    <t>Note 1 - Allowable US-GAAP members on the CounterpartyNameAxis</t>
-  </si>
-  <si>
-    <t>Element Name</t>
-  </si>
-  <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>AffiliatedEntityMember</t>
-  </si>
-  <si>
-    <t>Affiliated Entity [Member]</t>
-  </si>
-  <si>
-    <t>An affiliate is a party that, directly or indirectly through one or more intermediaries, controls, is controlled by, or is under common control with the entity.</t>
-  </si>
-  <si>
-    <t>InvestorMember</t>
-  </si>
-  <si>
-    <t>Investor [Member]</t>
-  </si>
-  <si>
-    <t>Business entity or individual that puts money, by purchase or expenditure, in something offering potential profitable returns, such as interest income or appreciation in value.</t>
-  </si>
-  <si>
-    <t>VariableInterestEntityNotPrimaryBeneficiaryMember</t>
-  </si>
-  <si>
-    <t>Variable Interest Entity, Not Primary Beneficiary [Member]</t>
-  </si>
-  <si>
-    <t>Variable Interest Entities (VIE) in which the entity does not have a controlling financial interest (as defined) and of which it is therefore not the primary beneficiary. VIEs of which the entity is not the primary beneficiary because it does not have the power to direct the activities of the VIE that most significantly impact the VIE's economic performance and for which it does not have the obligation to absorb losses of the VIE that could potentially be significant to the VIE or the right to receive benefits from the VIE that could potentially be significant to the VIE are not included in the consolidated financial statements of the entity.</t>
-  </si>
-  <si>
-    <t>ChiefFinancialOfficerMember</t>
-  </si>
-  <si>
-    <t>Chief Financial Officer [Member]</t>
-  </si>
-  <si>
-    <t>Senior executive officer responsible for overseeing the financial activities of the entity.</t>
-  </si>
-  <si>
-    <t>IndividualMember</t>
-  </si>
-  <si>
-    <t>Individual Counterparty [Member]</t>
-  </si>
-  <si>
-    <t>Individual person that is legally permitted to enter into a contract and be sued if that person fails to meet the obligations imposed by a contract.</t>
-  </si>
-  <si>
-    <t>GovernmentMember</t>
-  </si>
-  <si>
-    <t>Government [Member]</t>
-  </si>
-  <si>
-    <t>Organization that is the governing authority of a community.</t>
-  </si>
-  <si>
-    <t>GuarantorSubsidiariesMember</t>
-  </si>
-  <si>
-    <t>Guarantor Subsidiaries [Member]</t>
-  </si>
-  <si>
-    <t>Entity owned or controlled by another entity which has guaranteed the issue of securities by another subsidiary of the parent or has guaranteed the issue of securities by the parent.</t>
-  </si>
-  <si>
-    <t>SubsidiaryIssuerMember</t>
-  </si>
-  <si>
-    <t>Subsidiary Issuer [Member]</t>
-  </si>
-  <si>
-    <t>A company controlled, directly or indirectly, by its parent, which has issued securities and those securities are guaranteed by its parent and another subsidiary of the parent.</t>
-  </si>
-  <si>
-    <t>DirectorMember</t>
-  </si>
-  <si>
-    <t>Director [Member]</t>
-  </si>
-  <si>
-    <t>Person serving on the board of directors (who collectively have responsibility for governing the entity).</t>
-  </si>
-  <si>
-    <t>ChiefExecutiveOfficerMember</t>
-  </si>
-  <si>
-    <t>Chief Executive Officer [Member]</t>
-  </si>
-  <si>
-    <t>Highest ranking executive officer, who has ultimate managerial responsibility for the entity and who reports to the board of directors. In addition, the chief executive officer (CEO) may also be the chairman of the board or president.</t>
-  </si>
-  <si>
-    <t>ChiefOperatingOfficerMember</t>
-  </si>
-  <si>
-    <t>Chief Operating Officer [Member]</t>
-  </si>
-  <si>
-    <t>Senior executive officer responsible for management of day-to-day activities of the entity.</t>
-  </si>
-  <si>
-    <t>GeneralPartnerMember</t>
-  </si>
-  <si>
-    <t>General Partner [Member]</t>
-  </si>
-  <si>
-    <t>Party to a partnership business who has unlimited liability.</t>
-  </si>
-  <si>
-    <t>CorporateJointVentureMember</t>
-  </si>
-  <si>
-    <t>Corporate Joint Venture [Member]</t>
-  </si>
-  <si>
-    <t>Corporation owned and operated by a small group of ventures to accomplish a mutually beneficial venture or project.</t>
-  </si>
-  <si>
-    <t>SubsidiaryOfCommonParentMember</t>
-  </si>
-  <si>
-    <t>Subsidiary of Common Parent [Member]</t>
-  </si>
-  <si>
-    <t>Refers to an entity under the control of the same parent as another entity (that is, a sister company).</t>
-  </si>
-  <si>
-    <t>Note 2 - Allowable extension members on the CurrencyAxis</t>
-  </si>
-  <si>
-    <t>SICAD1Member</t>
-  </si>
-  <si>
-    <t>SICA D1 [Member]</t>
-  </si>
-  <si>
-    <t>extension</t>
-  </si>
-  <si>
-    <t>Venezuelan complementary currency exchange system, Sistema Complementario de Administracion de Divisas 1</t>
-  </si>
-  <si>
-    <t>SICAD2Member</t>
-  </si>
-  <si>
-    <t>SICA D2 [Member]</t>
-  </si>
-  <si>
-    <t>Venezuelan complementary currency exchange system, Sistema Complementario de Administracion de Divisas 2</t>
-  </si>
-  <si>
-    <t>OtherCurrencyMember</t>
-  </si>
-  <si>
-    <t>Other [Member]</t>
-  </si>
-  <si>
-    <t>Represents all other currencies not specifically defined.</t>
-  </si>
-  <si>
-    <t>NonUSDollarMember</t>
-  </si>
-  <si>
-    <t>Non-U.S. Dollar [Member]</t>
-  </si>
-  <si>
-    <t>Represents all other currencies that are not USD.</t>
-  </si>
-  <si>
-    <t>CENCOEXMember</t>
-  </si>
-  <si>
-    <t>CENCOEX [Member]</t>
-  </si>
-  <si>
-    <t>The official Venezuelan exchange rate offered by the National Foreign Trade Center. (CENCOEX)</t>
-  </si>
-  <si>
-    <t>SICADMember</t>
-  </si>
-  <si>
-    <t>SICAD [Member]</t>
-  </si>
-  <si>
-    <t>The Venezuelan exchange rate available to companies importing essential goods (e.g., certain food, medicine, raw materials). Consolidates SICAD 1 and SICAD 2.</t>
-  </si>
-  <si>
-    <t>SIMADIMember</t>
-  </si>
-  <si>
-    <t>SIMADI [Member]</t>
-  </si>
-  <si>
-    <t>The market based Venezuelan Exchange Rate.</t>
-  </si>
-  <si>
-    <t>DIPROMember</t>
-  </si>
-  <si>
-    <t>DIPRO [Member]</t>
-  </si>
-  <si>
-    <t>Venezuelan Exchange Rate that replaced the SICAD on March 10, 2016.  The DIPRO, is used for payments of critical importance such as healthcare.</t>
-  </si>
-  <si>
-    <t>DICOMMember</t>
-  </si>
-  <si>
-    <t>DICON [Member]</t>
-  </si>
-  <si>
-    <t>Venezuelan Exchange Rate that replaced the SIMADI on March 10, 2016.  The DICOM, fluctuates according to market supply and demand.</t>
-  </si>
-  <si>
-    <t>Note 3 - Allowable US-GAAP members on the ProductOrServiceAxis</t>
-  </si>
-  <si>
-    <t>AuctionRateSecuritiesMember</t>
-  </si>
-  <si>
-    <t>Auction Rate Securities [Member]</t>
-  </si>
-  <si>
-    <t>Debt instrument securities (for example, but not limited to, corporate or municipal bonds) that typically have long-term nominal maturities for which the interest rate is reset through an auction process.</t>
-  </si>
-  <si>
-    <t>AutomobileLoanMember</t>
-  </si>
-  <si>
-    <t>Automobile Loan [Member]</t>
-  </si>
-  <si>
-    <t>Loan to finance the purchase of a vehicle.</t>
-  </si>
-  <si>
-    <t>CommercialLoanMember</t>
-  </si>
-  <si>
-    <t>Commercial Loan [Member]</t>
-  </si>
-  <si>
-    <t>A loan, whether secured or unsecured, to a company for purposes such as seasonal working capital needs, inventory financing, equipment purchases and acquisitions.</t>
-  </si>
-  <si>
-    <t>CommercialRealEstateMember</t>
-  </si>
-  <si>
-    <t>Commercial Real Estate [Member]</t>
-  </si>
-  <si>
-    <t>Property that is solely used for business purposes.</t>
-  </si>
-  <si>
-    <t>ConstructionLoansMember</t>
-  </si>
-  <si>
-    <t>Construction Loans [Member]</t>
-  </si>
-  <si>
-    <t>A borrowing arrangement which provides the entity constructing a facility (such as a building and a landfill) with funds to effect construction, generally on a draw down, or as needed, basis.</t>
-  </si>
-  <si>
-    <t>ConsumerLoanMember</t>
-  </si>
-  <si>
-    <t>Consumer Loan [Member]</t>
-  </si>
-  <si>
-    <t>Loan or extension of credit for personal, family, or household use excluding real estate.</t>
-  </si>
-  <si>
-    <t>CrudeOilMember</t>
-  </si>
-  <si>
-    <t>Crude Oil [Member]</t>
-  </si>
-  <si>
-    <t>Unrefined, unprocessed oil, which may be used in a variety of applications, and from which, petroleum-based products are produced.</t>
-  </si>
-  <si>
-    <t>FuelMember</t>
-  </si>
-  <si>
-    <t>Fuel [Member]</t>
-  </si>
-  <si>
-    <t>Represents material used for the production of energy in the form of heat or power. Examples may include, but not be limited to heating, transpiration, etc.</t>
-  </si>
-  <si>
-    <t>GeneralLiabilityMember</t>
-  </si>
-  <si>
-    <t>General Liability [Member]</t>
-  </si>
-  <si>
-    <t>Type of business insurance which provides insurance coverage for a wide variety of liability exposures including, but not limited to, contractual liability, product liability and personal injury liability.</t>
-  </si>
-  <si>
-    <t>HeatingOilMember</t>
-  </si>
-  <si>
-    <t>Heating Oil [Member]</t>
-  </si>
-  <si>
-    <t>Fuel oil used to produce heat in an office, plant, or any other location where temperature is controlled or managed.</t>
-  </si>
-  <si>
-    <t>HomeEquityLoanMember</t>
-  </si>
-  <si>
-    <t>Home Equity Loan [Member]</t>
-  </si>
-  <si>
-    <t>Loan based on the equity of the borrower's residential property in which the borrower receives the loan amount upfront. Excludes home equity lines of credit.</t>
-  </si>
-  <si>
-    <t>HomeEquityMember</t>
-  </si>
-  <si>
-    <t>Home Equity Line of Credit [Member]</t>
-  </si>
-  <si>
-    <t>Revolving, open-end loan extended under a line of credit and secured by the borrower's residential property.</t>
-  </si>
-  <si>
-    <t>LetterOfCreditMember</t>
-  </si>
-  <si>
-    <t>Letter of Credit [Member]</t>
-  </si>
-  <si>
-    <t>A document typically issued by a financial institution which acts as a guarantee of payment to a beneficiary, or as the source of payment for a specific transaction (for example, wiring funds to a foreign exporter if and when specified merchandise is accepted pursuant to the terms of the letter of credit).</t>
-  </si>
-  <si>
-    <t>LineOfCreditMember</t>
-  </si>
-  <si>
-    <t>Line of Credit [Member]</t>
-  </si>
-  <si>
-    <t>A contractual arrangement with a lender under which borrowings can be made up to a specific amount at any point in time, and under which borrowings outstanding may be either short-term or long-term, depending upon the particulars.</t>
-  </si>
-  <si>
-    <t>LoansMember</t>
-  </si>
-  <si>
-    <t>Loans [Member]</t>
-  </si>
-  <si>
-    <t>When a lender gives money or property over other debt securities sold by the issuer. In the event the issuer goes bankrupt, senior debt holders receive priority for [must receive] repayment [prior] relative to junior and unsecured (general) creditors.</t>
-  </si>
-  <si>
-    <t>MortgageLoansOnRealEstateMember</t>
-  </si>
-  <si>
-    <t>Mortgage Loans on Real Estate [Member] (Deprecated 2015-01-31)</t>
-  </si>
-  <si>
-    <t>A loan to finance the purchase of real estate where the lender has a lien on the property as collateral for the loan.</t>
-  </si>
-  <si>
-    <t>NaturalGasLiquidsReservesMember</t>
-  </si>
-  <si>
-    <t>Natural Gas Liquids [Member]</t>
-  </si>
-  <si>
-    <t>Natural gas liquids that include, but are not limited to, ethane, propane, natural gasoline, butane and isobutane.</t>
-  </si>
-  <si>
-    <t>NaturalGasReservesMember</t>
-  </si>
-  <si>
-    <t>Natural Gas [Member]</t>
-  </si>
-  <si>
-    <t>Natural gas composed primarily of methane gas, excluding liquid or condensate natural gas.</t>
-  </si>
-  <si>
-    <t>OilReservesMember</t>
-  </si>
-  <si>
-    <t>Oil [Member]</t>
-  </si>
-  <si>
-    <t>Crude oil, which may also include condensate and natural gas liquids.</t>
-  </si>
-  <si>
-    <t>ProfessionalMalpracticeLiabilityMember</t>
-  </si>
-  <si>
-    <t>Professional Malpractice Liability Insurance [Member]</t>
-  </si>
-  <si>
-    <t>Business insurance coverage for professionals, such as doctors, lawyers, insurance agents, accountants, real estate agents, veterinarians, and others. This liability coverage insures losses for claims arising from mistakes and errors or omissions in the course of professional activities.</t>
-  </si>
-  <si>
-    <t>RealEstateLoanMember</t>
-  </si>
-  <si>
-    <t>Real Estate Loan [Member]</t>
-  </si>
-  <si>
-    <t>Loan to finance the purchase of real estate, including but not limited to, land or building.</t>
-  </si>
-  <si>
-    <t>ResidentialMortgageMember</t>
-  </si>
-  <si>
-    <t>Residential Mortgage [Member]</t>
-  </si>
-  <si>
-    <t>Loan to purchase or refinance residential real estate for example, but not limited to, a home, in which the real estate itself serves as collateral for the loan.</t>
-  </si>
-  <si>
-    <t>SyntheticOilMember</t>
-  </si>
-  <si>
-    <t>Synthetic Oil [Member]</t>
-  </si>
-  <si>
-    <t>Lubricant consisting of chemical compounds that are synthetically made.</t>
-  </si>
-  <si>
-    <t>PublicUtilitiesInventoryWaterMember</t>
-  </si>
-  <si>
-    <t>Water [Member]</t>
-  </si>
-  <si>
-    <t>Clear, colorless, odorless and tasteless liquid essential for most plant and animal life comprised of two parts hydrogen and one part oxygen (H2O).</t>
-  </si>
-  <si>
-    <t>PublicUtilitiesInventoryPropaneMember</t>
-  </si>
-  <si>
-    <t>Propane [Member]</t>
-  </si>
-  <si>
-    <t>Product derived from petroleum during the processing of oil or natural gas which is then used as a heat source or fuel.</t>
-  </si>
-  <si>
-    <t>ResidentialRealEstateMember</t>
-  </si>
-  <si>
-    <t>Residential Real Estate [Member]</t>
-  </si>
-  <si>
-    <t>Property that is used as a home.</t>
-  </si>
-  <si>
-    <t>AutomobilesMember</t>
-  </si>
-  <si>
-    <t>Automobiles [Member]</t>
-  </si>
-  <si>
-    <t>Vehicles that are used primarily for transporting people.</t>
-  </si>
-  <si>
-    <t>Note 4 - Allowable US-GAAP Members on the ConsolidationItemsAxis</t>
-  </si>
-  <si>
-    <t>CorporateReconcilingItemsAndEliminationsMember</t>
-  </si>
-  <si>
-    <t>Eliminations, Corporate and Reconciling Items [Member]</t>
-  </si>
-  <si>
-    <t>Represents the aggregate total of adjustments for non operating corporate items, reconciling items and eliminations.</t>
-  </si>
-  <si>
-    <t>CorporateAndReconcilingItemsMember</t>
-  </si>
-  <si>
-    <t>Corporate and Reconciling Items [Member]</t>
-  </si>
-  <si>
-    <t>Represents the aggregate total of non operating corporate items and reconciling items</t>
-  </si>
-  <si>
-    <t>CorporateAndEliminationsMember</t>
-  </si>
-  <si>
-    <t>Corporate and Eliminations [Member]</t>
-  </si>
-  <si>
-    <t>Represents the aggregate total of non operating corporate items and elimination items</t>
-  </si>
-  <si>
-    <t>EliminationsAndReconcilingItemsMember</t>
-  </si>
-  <si>
-    <t>Eliminations and Reconciling Items [Member]</t>
-  </si>
-  <si>
-    <t>Represents the aggregate total of reconciling items and elimination items</t>
-  </si>
-  <si>
-    <t>OperatingSegmentsAndCorporateNonSegmentMember</t>
-  </si>
-  <si>
-    <t>Operating Segments and Corporate Non Segment [Member]</t>
-  </si>
-  <si>
-    <t>Represents the aggregate total of “Operating Segments” and “Corporate, Non-Segment”, before elimination and reconciliation items.</t>
-  </si>
-  <si>
-    <t>Note 5 - Allowable US-GAAP Members on the StatementEquityComponentsAxis</t>
-  </si>
-  <si>
-    <t>WarrantsNotSettleableInCashMember</t>
-  </si>
-  <si>
-    <t>Warrants Not Settleable in Cash [Member]</t>
-  </si>
-  <si>
-    <t>Warrants not settleable in cash that are classified in shareholders' equity.</t>
-  </si>
-  <si>
-    <t>ContingentConsiderationClassifiedAsEquityMember</t>
-  </si>
-  <si>
-    <t>Contingent Consideration Classified as Equity [Member]</t>
-  </si>
-  <si>
-    <t>Contingent consideration in a business combination that is classified in shareholders' equity.</t>
-  </si>
-  <si>
-    <t>EquityIssuedInBusinessCombinationMember</t>
-  </si>
-  <si>
-    <t>Equity Issued in Business Combination [Member]</t>
-  </si>
-  <si>
-    <t>Equity issued by an entity in a business combination that is classified in shareholders' equity.</t>
-  </si>
-  <si>
-    <t>TrustForBenefitOfEmployeesMember</t>
-  </si>
-  <si>
-    <t>Trust for Benefit of Employees [Member]</t>
-  </si>
-  <si>
-    <t>Trust created by the entity that exists for the benefit of its employees, such as pension and profit-sharing trusts that are managed by or under the trusteeship of the entity's management.</t>
-  </si>
-  <si>
-    <t>DQC_0001.77</t>
-  </si>
-  <si>
-    <t>PreferredUnitsByNameAxis</t>
-  </si>
-  <si>
-    <t>Preferred Units by Name [Axis]</t>
-  </si>
-  <si>
-    <t>DQC_0001.78</t>
-  </si>
-  <si>
-    <t>RetirementPlanNameAxis</t>
-  </si>
-  <si>
-    <t>Retirement Plan Name [Axis]</t>
-  </si>
-  <si>
-    <t>DQC_0001.79</t>
-  </si>
-  <si>
-    <t>srt</t>
-  </si>
-  <si>
-    <t>OwnershipAxis</t>
-  </si>
-  <si>
-    <t>Ownership [Axis]</t>
-  </si>
-  <si>
-    <t>DQC_0001.80</t>
-  </si>
-  <si>
-    <t>MajorCustomersAxis</t>
-  </si>
-  <si>
-    <t>Customer [Axis]</t>
-  </si>
-  <si>
-    <t>Taxonomy Added</t>
-  </si>
-  <si>
-    <t>AuctionRateSecuritiesMember, AutomobileLoanMember, CommercialLoanMember, CommercialRealEstateMember, ConstructionLoansMember, ConsumerLoanMember, CrudeOilMember, FuelMember, GeneralLiabilityMember, HeatingOilMember, HomeEquityLoanMember, HomeEquityMember, LetterOfCreditMember, LineOfCreditMember, LoansMember, MortgageLoansOnRealEstateMember, NaturalGasLiquidsReservesMember, NaturalGasReservesMember, OilReservesMember, ProfessionalMalpracticeLiabilityMember, RealEstateLoanMember, ResidentialMortgageMember, SyntheticOilMember, PublicUtilitiesInventoryWaterMember, PublicUtilitiesInventoryPropaneMember, ResidentialRealEstateMember, RealEstateMember, AutomobilesMember, HotelMember</t>
-  </si>
-  <si>
-    <t>RealEstateMember</t>
-  </si>
-  <si>
-    <t>Real Estate [Member]</t>
-  </si>
-  <si>
-    <t>HotelMember</t>
-  </si>
-  <si>
-    <t>Hotel [Member]</t>
-  </si>
-  <si>
-    <t>Release Adopted &amp; Updated</t>
-  </si>
-  <si>
-    <t>3,6</t>
-  </si>
-  <si>
-    <t>Before 2018: WarrantsNotSettleableInCashMember, ContingentConsiderationClassifiedAsEquityMember, EquityIssuedInBusinessCombinationMember, TrustForBenefitOfEmployeesMember; Added For 2018: AccumulatedNetGainLossFromCashFlowHedgesIncludingPortionAttributableToNoncontrollingInterestMember, AccumulatedNetGainLossFromDesignatedOrQualifyingCashFlowHedgesMember, AccumulatedNetGainLossFromCashFlowHedgesAttributableToNoncontrollingInterestMember</t>
   </si>
 </sst>
 </file>
@@ -1519,9 +1519,7 @@
   </sheetPr>
   <dimension ref="A1:AD991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -1569,10 +1567,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L1" s="34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -1774,11 +1772,11 @@
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L7" s="32"/>
     </row>
-    <row r="8" spans="1:29" s="11" customFormat="1" ht="180">
+    <row r="8" spans="1:29" s="11" customFormat="1" ht="156">
       <c r="A8" s="12" t="s">
         <v>39</v>
       </c>
@@ -1806,7 +1804,7 @@
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L8" s="32"/>
       <c r="M8" s="10"/>
@@ -1907,7 +1905,7 @@
         <v>53</v>
       </c>
       <c r="K11" s="38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L11" s="32"/>
     </row>
@@ -2058,18 +2056,18 @@
         <v>71</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L16" s="32"/>
     </row>
-    <row r="17" spans="1:30" s="11" customFormat="1" ht="12.75">
+    <row r="17" spans="1:30" s="11" customFormat="1" ht="84">
       <c r="A17" s="12" t="s">
         <v>72</v>
       </c>
@@ -2093,17 +2091,17 @@
       <c r="I17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="10" t="s">
-        <v>75</v>
+      <c r="J17" s="13" t="s">
+        <v>301</v>
       </c>
       <c r="K17" s="38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L17" s="32"/>
     </row>
     <row r="18" spans="1:30" s="11" customFormat="1" ht="96">
       <c r="A18" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>11</v>
@@ -2112,16 +2110,16 @@
         <v>12</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>78</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="10" t="s">
@@ -2135,7 +2133,7 @@
     </row>
     <row r="19" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A19" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>11</v>
@@ -2144,10 +2142,10 @@
         <v>12</v>
       </c>
       <c r="D19" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>82</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>25</v>
@@ -2165,7 +2163,7 @@
     </row>
     <row r="20" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A20" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>11</v>
@@ -2174,10 +2172,10 @@
         <v>12</v>
       </c>
       <c r="D20" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>15</v>
@@ -2195,7 +2193,7 @@
     </row>
     <row r="21" spans="1:30" s="24" customFormat="1" ht="204">
       <c r="A21" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B21" s="29" t="s">
         <v>11</v>
@@ -2204,30 +2202,30 @@
         <v>12</v>
       </c>
       <c r="D21" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="29" t="s">
         <v>87</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>88</v>
       </c>
       <c r="F21" s="29" t="s">
         <v>15</v>
       </c>
       <c r="G21" s="30"/>
       <c r="H21" s="31" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I21" s="29" t="s">
         <v>15</v>
       </c>
       <c r="J21" s="29"/>
       <c r="K21" s="38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L21" s="32"/>
     </row>
     <row r="22" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A22" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>11</v>
@@ -2236,10 +2234,10 @@
         <v>12</v>
       </c>
       <c r="D22" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="29" t="s">
         <v>90</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>91</v>
       </c>
       <c r="F22" s="29" t="s">
         <v>15</v>
@@ -2257,7 +2255,7 @@
     </row>
     <row r="23" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A23" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>11</v>
@@ -2266,10 +2264,10 @@
         <v>36</v>
       </c>
       <c r="D23" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="29" t="s">
         <v>93</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>94</v>
       </c>
       <c r="F23" s="29" t="s">
         <v>15</v>
@@ -2281,13 +2279,13 @@
       </c>
       <c r="J23" s="29"/>
       <c r="K23" s="38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L23" s="32"/>
     </row>
     <row r="24" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A24" s="31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B24" s="31" t="s">
         <v>11</v>
@@ -2296,10 +2294,10 @@
         <v>12</v>
       </c>
       <c r="D24" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="E24" s="31" t="s">
         <v>281</v>
-      </c>
-      <c r="E24" s="31" t="s">
-        <v>282</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>25</v>
@@ -2335,7 +2333,7 @@
     </row>
     <row r="25" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A25" s="31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B25" s="31" t="s">
         <v>11</v>
@@ -2344,10 +2342,10 @@
         <v>12</v>
       </c>
       <c r="D25" s="31" t="s">
+        <v>283</v>
+      </c>
+      <c r="E25" s="31" t="s">
         <v>284</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>285</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>25</v>
@@ -2385,19 +2383,19 @@
     </row>
     <row r="26" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A26" s="31" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B26" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="D26" s="33" t="s">
         <v>287</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="E26" s="31" t="s">
         <v>288</v>
-      </c>
-      <c r="E26" s="31" t="s">
-        <v>289</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>25</v>
@@ -2435,19 +2433,19 @@
     </row>
     <row r="27" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A27" s="31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B27" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D27" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="E27" s="31" t="s">
         <v>291</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>292</v>
       </c>
       <c r="F27" s="31" t="s">
         <v>25</v>
@@ -2548,7 +2546,7 @@
     </row>
     <row r="32" spans="1:30" s="11" customFormat="1" ht="16.5">
       <c r="A32" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -2582,7 +2580,7 @@
     </row>
     <row r="33" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A33" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -2593,259 +2591,259 @@
         <v>2</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K33" s="32"/>
       <c r="L33" s="32"/>
     </row>
     <row r="34" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A34" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K34" s="32"/>
       <c r="L34" s="32"/>
     </row>
     <row r="35" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A35" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K35" s="32"/>
       <c r="L35" s="32"/>
     </row>
     <row r="36" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A36" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E36" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K36" s="32"/>
       <c r="L36" s="32"/>
     </row>
     <row r="37" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A37" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K37" s="32"/>
       <c r="L37" s="32"/>
     </row>
     <row r="38" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A38" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K38" s="32"/>
       <c r="L38" s="32"/>
     </row>
     <row r="39" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A39" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K39" s="32"/>
       <c r="L39" s="32"/>
     </row>
     <row r="40" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A40" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E40" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K40" s="32"/>
       <c r="L40" s="32"/>
     </row>
     <row r="41" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A41" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K41" s="32"/>
       <c r="L41" s="32"/>
     </row>
     <row r="42" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A42" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E42" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K42" s="32"/>
       <c r="L42" s="32"/>
     </row>
     <row r="43" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A43" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E43" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K43" s="32"/>
       <c r="L43" s="32"/>
     </row>
     <row r="44" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A44" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E44" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K44" s="32"/>
       <c r="L44" s="32"/>
     </row>
     <row r="45" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A45" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E45" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K45" s="32"/>
       <c r="L45" s="32"/>
     </row>
     <row r="46" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A46" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K46" s="32"/>
       <c r="L46" s="32"/>
     </row>
     <row r="47" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A47" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E47" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K47" s="32"/>
       <c r="L47" s="32"/>
@@ -2856,14 +2854,14 @@
     </row>
     <row r="49" spans="1:12" s="11" customFormat="1" ht="16.5">
       <c r="A49" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K49" s="32"/>
       <c r="L49" s="32"/>
     </row>
     <row r="50" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A50" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B50" s="18"/>
       <c r="C50" s="18"/>
@@ -2874,159 +2872,159 @@
         <v>2</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K50" s="32"/>
       <c r="L50" s="32"/>
     </row>
     <row r="51" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A51" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
       <c r="D51" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E51" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="F51" s="10" t="s">
         <v>143</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>144</v>
       </c>
       <c r="K51" s="32"/>
       <c r="L51" s="32"/>
     </row>
     <row r="52" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A52" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
       <c r="D52" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F52" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>147</v>
       </c>
       <c r="K52" s="32"/>
       <c r="L52" s="32"/>
     </row>
     <row r="53" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A53" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
       <c r="D53" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F53" s="10" t="s">
         <v>149</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>150</v>
       </c>
       <c r="K53" s="32"/>
       <c r="L53" s="32"/>
     </row>
     <row r="54" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A54" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F54" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>153</v>
       </c>
       <c r="K54" s="32"/>
       <c r="L54" s="32"/>
     </row>
     <row r="55" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A55" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D55" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="D55" s="21" t="s">
+      <c r="E55" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F55" s="21" t="s">
         <v>155</v>
-      </c>
-      <c r="E55" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="F55" s="21" t="s">
-        <v>156</v>
       </c>
       <c r="K55" s="32"/>
       <c r="L55" s="32"/>
     </row>
     <row r="56" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A56" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="D56" s="21" t="s">
+      <c r="E56" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F56" s="21" t="s">
         <v>158</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="F56" s="21" t="s">
-        <v>159</v>
       </c>
       <c r="K56" s="32"/>
       <c r="L56" s="32"/>
     </row>
     <row r="57" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A57" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="D57" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="D57" s="21" t="s">
+      <c r="E57" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F57" s="21" t="s">
         <v>161</v>
-      </c>
-      <c r="E57" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="F57" s="21" t="s">
-        <v>162</v>
       </c>
       <c r="K57" s="32"/>
       <c r="L57" s="32"/>
     </row>
     <row r="58" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A58" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="D58" s="21" t="s">
+      <c r="E58" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F58" s="21" t="s">
         <v>164</v>
-      </c>
-      <c r="E58" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="F58" s="21" t="s">
-        <v>165</v>
       </c>
       <c r="K58" s="32"/>
       <c r="L58" s="32"/>
     </row>
     <row r="59" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A59" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="D59" s="21" t="s">
+      <c r="E59" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F59" s="21" t="s">
         <v>167</v>
-      </c>
-      <c r="E59" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="F59" s="21" t="s">
-        <v>168</v>
       </c>
       <c r="K59" s="32"/>
       <c r="L59" s="32"/>
@@ -3038,14 +3036,14 @@
     </row>
     <row r="61" spans="1:12" s="11" customFormat="1" ht="16.5">
       <c r="A61" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K61" s="32"/>
       <c r="L61" s="32"/>
     </row>
     <row r="62" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A62" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B62" s="18"/>
       <c r="C62" s="18"/>
@@ -3056,495 +3054,495 @@
         <v>2</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K62" s="32"/>
       <c r="L62" s="32"/>
     </row>
     <row r="63" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A63" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E63" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K63" s="32"/>
       <c r="L63" s="32"/>
     </row>
     <row r="64" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A64" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E64" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K64" s="32"/>
       <c r="L64" s="32"/>
     </row>
     <row r="65" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A65" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E65" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K65" s="32"/>
       <c r="L65" s="32"/>
     </row>
     <row r="66" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A66" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E66" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K66" s="32"/>
       <c r="L66" s="32"/>
     </row>
     <row r="67" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A67" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K67" s="32"/>
       <c r="L67" s="32"/>
     </row>
     <row r="68" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A68" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E68" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K68" s="32"/>
       <c r="L68" s="32"/>
     </row>
     <row r="69" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A69" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E69" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K69" s="32"/>
       <c r="L69" s="32"/>
     </row>
     <row r="70" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A70" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E70" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K70" s="32"/>
       <c r="L70" s="32"/>
     </row>
     <row r="71" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A71" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E71" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K71" s="32"/>
       <c r="L71" s="32"/>
     </row>
     <row r="72" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A72" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E72" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K72" s="32"/>
       <c r="L72" s="32"/>
     </row>
     <row r="73" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A73" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
       <c r="D73" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E73" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K73" s="32"/>
       <c r="L73" s="32"/>
     </row>
     <row r="74" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A74" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E74" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K74" s="32"/>
       <c r="L74" s="32"/>
     </row>
     <row r="75" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A75" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E75" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K75" s="32"/>
       <c r="L75" s="32"/>
     </row>
     <row r="76" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A76" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
       <c r="D76" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K76" s="32"/>
       <c r="L76" s="32"/>
     </row>
     <row r="77" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A77" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K77" s="32"/>
       <c r="L77" s="32"/>
     </row>
     <row r="78" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A78" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
       <c r="D78" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F78" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K78" s="32"/>
       <c r="L78" s="32"/>
     </row>
     <row r="79" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A79" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
       <c r="D79" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K79" s="32"/>
       <c r="L79" s="32"/>
     </row>
     <row r="80" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A80" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
       <c r="D80" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E80" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K80" s="32"/>
       <c r="L80" s="32"/>
     </row>
     <row r="81" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A81" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
       <c r="D81" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E81" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K81" s="32"/>
       <c r="L81" s="32"/>
     </row>
     <row r="82" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A82" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
       <c r="D82" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K82" s="32"/>
       <c r="L82" s="32"/>
     </row>
     <row r="83" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A83" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
       <c r="D83" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K83" s="32"/>
       <c r="L83" s="32"/>
     </row>
     <row r="84" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A84" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
       <c r="D84" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E84" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K84" s="32"/>
       <c r="L84" s="32"/>
     </row>
     <row r="85" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A85" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
       <c r="D85" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F85" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K85" s="32"/>
       <c r="L85" s="32"/>
     </row>
     <row r="86" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A86" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="D86" s="21" t="s">
         <v>239</v>
-      </c>
-      <c r="D86" s="21" t="s">
-        <v>240</v>
       </c>
       <c r="E86" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F86" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K86" s="32"/>
       <c r="L86" s="32"/>
     </row>
     <row r="87" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A87" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="D87" s="21" t="s">
         <v>242</v>
-      </c>
-      <c r="D87" s="21" t="s">
-        <v>243</v>
       </c>
       <c r="E87" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F87" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K87" s="32"/>
       <c r="L87" s="32"/>
     </row>
     <row r="88" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A88" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="D88" s="21" t="s">
         <v>245</v>
-      </c>
-      <c r="D88" s="21" t="s">
-        <v>246</v>
       </c>
       <c r="E88" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F88" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K88" s="32"/>
       <c r="L88" s="32"/>
     </row>
     <row r="89" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A89" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="D89" s="21" t="s">
         <v>248</v>
-      </c>
-      <c r="D89" s="21" t="s">
-        <v>249</v>
       </c>
       <c r="E89" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F89" s="21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K89" s="32"/>
       <c r="L89" s="32"/>
     </row>
     <row r="90" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A90" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="D90" s="21" t="s">
         <v>295</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>296</v>
       </c>
       <c r="E90" s="27" t="s">
         <v>12</v>
@@ -3555,12 +3553,12 @@
     </row>
     <row r="91" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A91" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B91" s="26"/>
       <c r="C91" s="26"/>
       <c r="D91" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E91" s="26" t="s">
         <v>12</v>
@@ -3598,14 +3596,14 @@
     </row>
     <row r="93" spans="1:30" s="11" customFormat="1" ht="16.5">
       <c r="A93" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K93" s="32"/>
       <c r="L93" s="32"/>
     </row>
     <row r="94" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A94" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B94" s="18"/>
       <c r="C94" s="18"/>
@@ -3616,7 +3614,7 @@
         <v>2</v>
       </c>
       <c r="F94" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G94" s="10"/>
       <c r="H94" s="10"/>
@@ -3645,18 +3643,18 @@
     </row>
     <row r="95" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A95" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
       <c r="D95" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F95" s="10" t="s">
         <v>253</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F95" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="G95" s="10"/>
       <c r="H95" s="10"/>
@@ -3685,18 +3683,18 @@
     </row>
     <row r="96" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A96" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F96" s="10" t="s">
         <v>256</v>
-      </c>
-      <c r="E96" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F96" s="10" t="s">
-        <v>257</v>
       </c>
       <c r="G96" s="10"/>
       <c r="H96" s="10"/>
@@ -3725,18 +3723,18 @@
     </row>
     <row r="97" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A97" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
       <c r="D97" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F97" s="10" t="s">
         <v>259</v>
-      </c>
-      <c r="E97" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F97" s="10" t="s">
-        <v>260</v>
       </c>
       <c r="G97" s="10"/>
       <c r="H97" s="10"/>
@@ -3765,18 +3763,18 @@
     </row>
     <row r="98" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A98" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
       <c r="D98" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F98" s="10" t="s">
         <v>262</v>
-      </c>
-      <c r="E98" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F98" s="10" t="s">
-        <v>263</v>
       </c>
       <c r="G98" s="10"/>
       <c r="H98" s="10"/>
@@ -3805,18 +3803,18 @@
     </row>
     <row r="99" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A99" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
       <c r="D99" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F99" s="10" t="s">
         <v>265</v>
-      </c>
-      <c r="E99" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F99" s="10" t="s">
-        <v>266</v>
       </c>
       <c r="G99" s="10"/>
       <c r="H99" s="10"/>
@@ -3877,7 +3875,7 @@
     </row>
     <row r="101" spans="1:30" s="11" customFormat="1" ht="16.5">
       <c r="A101" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B101" s="10"/>
       <c r="C101" s="10"/>
@@ -3911,7 +3909,7 @@
     </row>
     <row r="102" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A102" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B102" s="18"/>
       <c r="C102" s="18"/>
@@ -3922,7 +3920,7 @@
         <v>2</v>
       </c>
       <c r="F102" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G102" s="10"/>
       <c r="H102" s="10"/>
@@ -3951,64 +3949,64 @@
     </row>
     <row r="103" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A103" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="D103" s="10" t="s">
         <v>268</v>
-      </c>
-      <c r="D103" s="10" t="s">
-        <v>269</v>
       </c>
       <c r="E103" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F103" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K103" s="32"/>
       <c r="L103" s="32"/>
     </row>
     <row r="104" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A104" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="D104" s="10" t="s">
         <v>271</v>
-      </c>
-      <c r="D104" s="10" t="s">
-        <v>272</v>
       </c>
       <c r="E104" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F104" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K104" s="32"/>
       <c r="L104" s="32"/>
     </row>
     <row r="105" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A105" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="D105" s="10" t="s">
         <v>274</v>
-      </c>
-      <c r="D105" s="10" t="s">
-        <v>275</v>
       </c>
       <c r="E105" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F105" s="21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K105" s="32"/>
       <c r="L105" s="32"/>
     </row>
     <row r="106" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A106" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="D106" s="21" t="s">
         <v>277</v>
-      </c>
-      <c r="D106" s="21" t="s">
-        <v>278</v>
       </c>
       <c r="E106" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K106" s="32"/>
       <c r="L106" s="32"/>

</xml_diff>

<commit_message>
Update documentation dqc_0001 and dqc_0069
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -70,9 +70,6 @@
     <t>Limited</t>
   </si>
   <si>
-    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, InvestmentsNetAssetValueMember</t>
-  </si>
-  <si>
     <t>DQC_0001.52</t>
   </si>
   <si>
@@ -924,6 +921,9 @@
   <si>
     <t xml:space="preserve">CorporateReconcilingItemsAndEliminationsMember, CorporateAndReconcilingItemsMember, CorporateAndEliminationsMember, EliminationsAndReconcilingItemsMember, OperatingSegmentsAndCorporateNonSegmentMember, OperatingSegmentsExcludingIntersegmentEliminationMember
 </t>
+  </si>
+  <si>
+    <t>FairValueInputsLevel1AndLevel2Member, FairValueInputsLevel2AndLevel3Member, FairValueInputsLevel12And3Member, FairValueInputsLevel1AndLevel3Member, FairValueMeasuredAtNetAssetValuePerShareMember</t>
   </si>
 </sst>
 </file>
@@ -1519,7 +1519,9 @@
   </sheetPr>
   <dimension ref="A1:AD991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -1567,10 +1569,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L1" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -1615,7 +1617,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>17</v>
+        <v>301</v>
       </c>
       <c r="K2" s="36">
         <v>3</v>
@@ -1624,7 +1626,7 @@
     </row>
     <row r="3" spans="1:29" s="11" customFormat="1" ht="12.75">
       <c r="A3" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
@@ -1633,10 +1635,10 @@
         <v>12</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>20</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>15</v>
@@ -1644,7 +1646,7 @@
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="37">
@@ -1654,7 +1656,7 @@
     </row>
     <row r="4" spans="1:29" s="11" customFormat="1" ht="12.75">
       <c r="A4" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>11</v>
@@ -1663,13 +1665,13 @@
         <v>12</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
@@ -1684,28 +1686,28 @@
     </row>
     <row r="5" spans="1:29" s="11" customFormat="1" ht="60">
       <c r="A5" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>30</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>31</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>15</v>
@@ -1718,7 +1720,7 @@
     </row>
     <row r="6" spans="1:29" s="11" customFormat="1" ht="12.75">
       <c r="A6" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>11</v>
@@ -1727,13 +1729,13 @@
         <v>12</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="F6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
@@ -1748,22 +1750,22 @@
     </row>
     <row r="7" spans="1:29" s="11" customFormat="1" ht="12.75">
       <c r="A7" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="F7" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -1772,39 +1774,39 @@
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L7" s="32"/>
     </row>
     <row r="8" spans="1:29" s="11" customFormat="1" ht="156">
       <c r="A8" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="F8" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>15</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L8" s="32"/>
       <c r="M8" s="10"/>
@@ -1819,7 +1821,7 @@
     </row>
     <row r="9" spans="1:29" s="11" customFormat="1" ht="12.75">
       <c r="A9" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>11</v>
@@ -1828,13 +1830,13 @@
         <v>12</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>45</v>
-      </c>
       <c r="F9" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
@@ -1849,22 +1851,22 @@
     </row>
     <row r="10" spans="1:29" s="11" customFormat="1" ht="12.75">
       <c r="A10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="F10" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
@@ -1879,19 +1881,19 @@
     </row>
     <row r="11" spans="1:29" s="11" customFormat="1" ht="12.75">
       <c r="A11" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>15</v>
@@ -1902,16 +1904,16 @@
         <v>16</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K11" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L11" s="32"/>
     </row>
     <row r="12" spans="1:29" s="11" customFormat="1" ht="12.75">
       <c r="A12" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>11</v>
@@ -1920,10 +1922,10 @@
         <v>12</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>15</v>
@@ -1934,7 +1936,7 @@
         <v>16</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K12" s="37">
         <v>3</v>
@@ -1943,7 +1945,7 @@
     </row>
     <row r="13" spans="1:29" s="11" customFormat="1" ht="12.75">
       <c r="A13" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -1952,10 +1954,10 @@
         <v>12</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>60</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>15</v>
@@ -1963,7 +1965,7 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="37">
@@ -1973,7 +1975,7 @@
     </row>
     <row r="14" spans="1:29" s="11" customFormat="1" ht="12.75">
       <c r="A14" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>11</v>
@@ -1982,10 +1984,10 @@
         <v>12</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>15</v>
@@ -1993,7 +1995,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="37">
@@ -2003,7 +2005,7 @@
     </row>
     <row r="15" spans="1:29" s="11" customFormat="1" ht="12.75">
       <c r="A15" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>11</v>
@@ -2012,10 +2014,10 @@
         <v>12</v>
       </c>
       <c r="D15" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>66</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>15</v>
@@ -2026,7 +2028,7 @@
         <v>16</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K15" s="37">
         <v>3</v>
@@ -2035,53 +2037,53 @@
     </row>
     <row r="16" spans="1:29" s="11" customFormat="1" ht="312.75" thickBot="1">
       <c r="A16" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>70</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L16" s="32"/>
     </row>
     <row r="17" spans="1:30" s="11" customFormat="1" ht="84">
       <c r="A17" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>74</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>15</v>
@@ -2092,16 +2094,16 @@
         <v>16</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K17" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L17" s="32"/>
     </row>
     <row r="18" spans="1:30" s="11" customFormat="1" ht="96">
       <c r="A18" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>11</v>
@@ -2110,16 +2112,16 @@
         <v>12</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="10" t="s">
@@ -2133,7 +2135,7 @@
     </row>
     <row r="19" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A19" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>11</v>
@@ -2142,13 +2144,13 @@
         <v>12</v>
       </c>
       <c r="D19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>81</v>
-      </c>
       <c r="F19" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
@@ -2163,7 +2165,7 @@
     </row>
     <row r="20" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A20" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>11</v>
@@ -2172,10 +2174,10 @@
         <v>12</v>
       </c>
       <c r="D20" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>15</v>
@@ -2183,7 +2185,7 @@
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="37">
@@ -2193,7 +2195,7 @@
     </row>
     <row r="21" spans="1:30" s="24" customFormat="1" ht="204">
       <c r="A21" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="29" t="s">
         <v>11</v>
@@ -2202,30 +2204,30 @@
         <v>12</v>
       </c>
       <c r="D21" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="29" t="s">
         <v>86</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>87</v>
       </c>
       <c r="F21" s="29" t="s">
         <v>15</v>
       </c>
       <c r="G21" s="30"/>
       <c r="H21" s="31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I21" s="29" t="s">
         <v>15</v>
       </c>
       <c r="J21" s="29"/>
       <c r="K21" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L21" s="32"/>
     </row>
     <row r="22" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A22" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>11</v>
@@ -2234,10 +2236,10 @@
         <v>12</v>
       </c>
       <c r="D22" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="29" t="s">
         <v>89</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>90</v>
       </c>
       <c r="F22" s="29" t="s">
         <v>15</v>
@@ -2255,19 +2257,19 @@
     </row>
     <row r="23" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A23" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B23" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="29" t="s">
         <v>92</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>93</v>
       </c>
       <c r="F23" s="29" t="s">
         <v>15</v>
@@ -2275,17 +2277,17 @@
       <c r="G23" s="30"/>
       <c r="H23" s="30"/>
       <c r="I23" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J23" s="29"/>
       <c r="K23" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L23" s="32"/>
     </row>
     <row r="24" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A24" s="31" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B24" s="31" t="s">
         <v>11</v>
@@ -2294,13 +2296,13 @@
         <v>12</v>
       </c>
       <c r="D24" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="E24" s="31" t="s">
         <v>280</v>
       </c>
-      <c r="E24" s="31" t="s">
-        <v>281</v>
-      </c>
       <c r="F24" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -2333,7 +2335,7 @@
     </row>
     <row r="25" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A25" s="31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B25" s="31" t="s">
         <v>11</v>
@@ -2342,13 +2344,13 @@
         <v>12</v>
       </c>
       <c r="D25" s="31" t="s">
+        <v>282</v>
+      </c>
+      <c r="E25" s="31" t="s">
         <v>283</v>
       </c>
-      <c r="E25" s="31" t="s">
-        <v>284</v>
-      </c>
       <c r="F25" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
@@ -2383,22 +2385,22 @@
     </row>
     <row r="26" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A26" s="31" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B26" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="D26" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="E26" s="31" t="s">
         <v>287</v>
       </c>
-      <c r="E26" s="31" t="s">
-        <v>288</v>
-      </c>
       <c r="F26" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26" s="31"/>
       <c r="H26" s="31"/>
@@ -2433,22 +2435,22 @@
     </row>
     <row r="27" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A27" s="31" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B27" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D27" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="E27" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="E27" s="31" t="s">
-        <v>291</v>
-      </c>
       <c r="F27" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
@@ -2546,7 +2548,7 @@
     </row>
     <row r="32" spans="1:30" s="11" customFormat="1" ht="16.5">
       <c r="A32" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
@@ -2580,7 +2582,7 @@
     </row>
     <row r="33" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A33" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -2591,259 +2593,259 @@
         <v>2</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K33" s="32"/>
       <c r="L33" s="32"/>
     </row>
     <row r="34" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A34" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K34" s="32"/>
       <c r="L34" s="32"/>
     </row>
     <row r="35" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A35" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K35" s="32"/>
       <c r="L35" s="32"/>
     </row>
     <row r="36" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A36" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E36" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K36" s="32"/>
       <c r="L36" s="32"/>
     </row>
     <row r="37" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A37" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E37" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K37" s="32"/>
       <c r="L37" s="32"/>
     </row>
     <row r="38" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A38" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K38" s="32"/>
       <c r="L38" s="32"/>
     </row>
     <row r="39" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A39" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K39" s="32"/>
       <c r="L39" s="32"/>
     </row>
     <row r="40" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A40" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E40" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K40" s="32"/>
       <c r="L40" s="32"/>
     </row>
     <row r="41" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A41" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K41" s="32"/>
       <c r="L41" s="32"/>
     </row>
     <row r="42" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A42" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E42" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K42" s="32"/>
       <c r="L42" s="32"/>
     </row>
     <row r="43" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A43" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E43" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K43" s="32"/>
       <c r="L43" s="32"/>
     </row>
     <row r="44" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A44" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E44" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K44" s="32"/>
       <c r="L44" s="32"/>
     </row>
     <row r="45" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A45" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E45" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K45" s="32"/>
       <c r="L45" s="32"/>
     </row>
     <row r="46" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A46" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K46" s="32"/>
       <c r="L46" s="32"/>
     </row>
     <row r="47" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A47" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E47" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K47" s="32"/>
       <c r="L47" s="32"/>
@@ -2854,14 +2856,14 @@
     </row>
     <row r="49" spans="1:12" s="11" customFormat="1" ht="16.5">
       <c r="A49" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K49" s="32"/>
       <c r="L49" s="32"/>
     </row>
     <row r="50" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A50" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B50" s="18"/>
       <c r="C50" s="18"/>
@@ -2872,159 +2874,159 @@
         <v>2</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K50" s="32"/>
       <c r="L50" s="32"/>
     </row>
     <row r="51" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A51" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
       <c r="D51" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E51" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="F51" s="10" t="s">
         <v>142</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>143</v>
       </c>
       <c r="K51" s="32"/>
       <c r="L51" s="32"/>
     </row>
     <row r="52" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A52" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
       <c r="D52" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F52" s="10" t="s">
         <v>145</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>146</v>
       </c>
       <c r="K52" s="32"/>
       <c r="L52" s="32"/>
     </row>
     <row r="53" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A53" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
       <c r="D53" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F53" s="10" t="s">
         <v>148</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>149</v>
       </c>
       <c r="K53" s="32"/>
       <c r="L53" s="32"/>
     </row>
     <row r="54" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A54" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F54" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>152</v>
       </c>
       <c r="K54" s="32"/>
       <c r="L54" s="32"/>
     </row>
     <row r="55" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A55" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D55" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="D55" s="21" t="s">
+      <c r="E55" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F55" s="21" t="s">
         <v>154</v>
-      </c>
-      <c r="E55" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="F55" s="21" t="s">
-        <v>155</v>
       </c>
       <c r="K55" s="32"/>
       <c r="L55" s="32"/>
     </row>
     <row r="56" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A56" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="D56" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="D56" s="21" t="s">
+      <c r="E56" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F56" s="21" t="s">
         <v>157</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="F56" s="21" t="s">
-        <v>158</v>
       </c>
       <c r="K56" s="32"/>
       <c r="L56" s="32"/>
     </row>
     <row r="57" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A57" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="D57" s="21" t="s">
+      <c r="E57" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F57" s="21" t="s">
         <v>160</v>
-      </c>
-      <c r="E57" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="F57" s="21" t="s">
-        <v>161</v>
       </c>
       <c r="K57" s="32"/>
       <c r="L57" s="32"/>
     </row>
     <row r="58" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A58" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="D58" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="D58" s="21" t="s">
+      <c r="E58" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F58" s="21" t="s">
         <v>163</v>
-      </c>
-      <c r="E58" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="F58" s="21" t="s">
-        <v>164</v>
       </c>
       <c r="K58" s="32"/>
       <c r="L58" s="32"/>
     </row>
     <row r="59" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A59" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D59" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="D59" s="21" t="s">
+      <c r="E59" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F59" s="21" t="s">
         <v>166</v>
-      </c>
-      <c r="E59" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="F59" s="21" t="s">
-        <v>167</v>
       </c>
       <c r="K59" s="32"/>
       <c r="L59" s="32"/>
@@ -3036,14 +3038,14 @@
     </row>
     <row r="61" spans="1:12" s="11" customFormat="1" ht="16.5">
       <c r="A61" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K61" s="32"/>
       <c r="L61" s="32"/>
     </row>
     <row r="62" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A62" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B62" s="18"/>
       <c r="C62" s="18"/>
@@ -3054,495 +3056,495 @@
         <v>2</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K62" s="32"/>
       <c r="L62" s="32"/>
     </row>
     <row r="63" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A63" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E63" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K63" s="32"/>
       <c r="L63" s="32"/>
     </row>
     <row r="64" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A64" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E64" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K64" s="32"/>
       <c r="L64" s="32"/>
     </row>
     <row r="65" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A65" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E65" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K65" s="32"/>
       <c r="L65" s="32"/>
     </row>
     <row r="66" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A66" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E66" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K66" s="32"/>
       <c r="L66" s="32"/>
     </row>
     <row r="67" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A67" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
       <c r="D67" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K67" s="32"/>
       <c r="L67" s="32"/>
     </row>
     <row r="68" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A68" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E68" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K68" s="32"/>
       <c r="L68" s="32"/>
     </row>
     <row r="69" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A69" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E69" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K69" s="32"/>
       <c r="L69" s="32"/>
     </row>
     <row r="70" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A70" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E70" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K70" s="32"/>
       <c r="L70" s="32"/>
     </row>
     <row r="71" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A71" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E71" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K71" s="32"/>
       <c r="L71" s="32"/>
     </row>
     <row r="72" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A72" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E72" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K72" s="32"/>
       <c r="L72" s="32"/>
     </row>
     <row r="73" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A73" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
       <c r="D73" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E73" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K73" s="32"/>
       <c r="L73" s="32"/>
     </row>
     <row r="74" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A74" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E74" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K74" s="32"/>
       <c r="L74" s="32"/>
     </row>
     <row r="75" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A75" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E75" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K75" s="32"/>
       <c r="L75" s="32"/>
     </row>
     <row r="76" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A76" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B76" s="10"/>
       <c r="C76" s="10"/>
       <c r="D76" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K76" s="32"/>
       <c r="L76" s="32"/>
     </row>
     <row r="77" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A77" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K77" s="32"/>
       <c r="L77" s="32"/>
     </row>
     <row r="78" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A78" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B78" s="10"/>
       <c r="C78" s="10"/>
       <c r="D78" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F78" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K78" s="32"/>
       <c r="L78" s="32"/>
     </row>
     <row r="79" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A79" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B79" s="10"/>
       <c r="C79" s="10"/>
       <c r="D79" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K79" s="32"/>
       <c r="L79" s="32"/>
     </row>
     <row r="80" spans="1:12" s="11" customFormat="1" ht="12.75">
       <c r="A80" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B80" s="10"/>
       <c r="C80" s="10"/>
       <c r="D80" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E80" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K80" s="32"/>
       <c r="L80" s="32"/>
     </row>
     <row r="81" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A81" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B81" s="10"/>
       <c r="C81" s="10"/>
       <c r="D81" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E81" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K81" s="32"/>
       <c r="L81" s="32"/>
     </row>
     <row r="82" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A82" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
       <c r="D82" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K82" s="32"/>
       <c r="L82" s="32"/>
     </row>
     <row r="83" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A83" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
       <c r="D83" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K83" s="32"/>
       <c r="L83" s="32"/>
     </row>
     <row r="84" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A84" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
       <c r="D84" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E84" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K84" s="32"/>
       <c r="L84" s="32"/>
     </row>
     <row r="85" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A85" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
       <c r="D85" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F85" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K85" s="32"/>
       <c r="L85" s="32"/>
     </row>
     <row r="86" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A86" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="D86" s="21" t="s">
         <v>238</v>
-      </c>
-      <c r="D86" s="21" t="s">
-        <v>239</v>
       </c>
       <c r="E86" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F86" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K86" s="32"/>
       <c r="L86" s="32"/>
     </row>
     <row r="87" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A87" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="D87" s="21" t="s">
         <v>241</v>
-      </c>
-      <c r="D87" s="21" t="s">
-        <v>242</v>
       </c>
       <c r="E87" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F87" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K87" s="32"/>
       <c r="L87" s="32"/>
     </row>
     <row r="88" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A88" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="D88" s="21" t="s">
         <v>244</v>
-      </c>
-      <c r="D88" s="21" t="s">
-        <v>245</v>
       </c>
       <c r="E88" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F88" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K88" s="32"/>
       <c r="L88" s="32"/>
     </row>
     <row r="89" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A89" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="D89" s="21" t="s">
         <v>247</v>
-      </c>
-      <c r="D89" s="21" t="s">
-        <v>248</v>
       </c>
       <c r="E89" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F89" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K89" s="32"/>
       <c r="L89" s="32"/>
     </row>
     <row r="90" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A90" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="D90" s="21" t="s">
         <v>294</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>295</v>
       </c>
       <c r="E90" s="27" t="s">
         <v>12</v>
@@ -3553,12 +3555,12 @@
     </row>
     <row r="91" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A91" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B91" s="26"/>
       <c r="C91" s="26"/>
       <c r="D91" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E91" s="26" t="s">
         <v>12</v>
@@ -3596,14 +3598,14 @@
     </row>
     <row r="93" spans="1:30" s="11" customFormat="1" ht="16.5">
       <c r="A93" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K93" s="32"/>
       <c r="L93" s="32"/>
     </row>
     <row r="94" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A94" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B94" s="18"/>
       <c r="C94" s="18"/>
@@ -3614,7 +3616,7 @@
         <v>2</v>
       </c>
       <c r="F94" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G94" s="10"/>
       <c r="H94" s="10"/>
@@ -3643,18 +3645,18 @@
     </row>
     <row r="95" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A95" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
       <c r="D95" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F95" s="10" t="s">
         <v>252</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F95" s="10" t="s">
-        <v>253</v>
       </c>
       <c r="G95" s="10"/>
       <c r="H95" s="10"/>
@@ -3683,18 +3685,18 @@
     </row>
     <row r="96" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A96" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F96" s="10" t="s">
         <v>255</v>
-      </c>
-      <c r="E96" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F96" s="10" t="s">
-        <v>256</v>
       </c>
       <c r="G96" s="10"/>
       <c r="H96" s="10"/>
@@ -3723,18 +3725,18 @@
     </row>
     <row r="97" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A97" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
       <c r="D97" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F97" s="10" t="s">
         <v>258</v>
-      </c>
-      <c r="E97" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F97" s="10" t="s">
-        <v>259</v>
       </c>
       <c r="G97" s="10"/>
       <c r="H97" s="10"/>
@@ -3763,18 +3765,18 @@
     </row>
     <row r="98" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A98" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
       <c r="D98" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F98" s="10" t="s">
         <v>261</v>
-      </c>
-      <c r="E98" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F98" s="10" t="s">
-        <v>262</v>
       </c>
       <c r="G98" s="10"/>
       <c r="H98" s="10"/>
@@ -3803,18 +3805,18 @@
     </row>
     <row r="99" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A99" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
       <c r="D99" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F99" s="10" t="s">
         <v>264</v>
-      </c>
-      <c r="E99" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F99" s="10" t="s">
-        <v>265</v>
       </c>
       <c r="G99" s="10"/>
       <c r="H99" s="10"/>
@@ -3875,7 +3877,7 @@
     </row>
     <row r="101" spans="1:30" s="11" customFormat="1" ht="16.5">
       <c r="A101" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B101" s="10"/>
       <c r="C101" s="10"/>
@@ -3909,7 +3911,7 @@
     </row>
     <row r="102" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A102" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B102" s="18"/>
       <c r="C102" s="18"/>
@@ -3920,7 +3922,7 @@
         <v>2</v>
       </c>
       <c r="F102" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G102" s="10"/>
       <c r="H102" s="10"/>
@@ -3949,64 +3951,64 @@
     </row>
     <row r="103" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A103" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="D103" s="10" t="s">
         <v>267</v>
-      </c>
-      <c r="D103" s="10" t="s">
-        <v>268</v>
       </c>
       <c r="E103" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F103" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K103" s="32"/>
       <c r="L103" s="32"/>
     </row>
     <row r="104" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A104" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="D104" s="10" t="s">
         <v>270</v>
-      </c>
-      <c r="D104" s="10" t="s">
-        <v>271</v>
       </c>
       <c r="E104" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F104" s="21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K104" s="32"/>
       <c r="L104" s="32"/>
     </row>
     <row r="105" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A105" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="D105" s="10" t="s">
         <v>273</v>
-      </c>
-      <c r="D105" s="10" t="s">
-        <v>274</v>
       </c>
       <c r="E105" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F105" s="21" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K105" s="32"/>
       <c r="L105" s="32"/>
     </row>
     <row r="106" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A106" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="D106" s="21" t="s">
         <v>276</v>
-      </c>
-      <c r="D106" s="21" t="s">
-        <v>277</v>
       </c>
       <c r="E106" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K106" s="32"/>
       <c r="L106" s="32"/>

</xml_diff>

<commit_message>
Update dqc_0001 list of axes
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -1519,7 +1519,9 @@
   </sheetPr>
   <dimension ref="A1:AD991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100:XFD100"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
fix dqc_0001 list of axes - excel
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="305">
   <si>
     <t>Rule element ID</t>
   </si>
@@ -767,9 +767,6 @@
   </si>
   <si>
     <t>Vehicles that are used primarily for transporting people.</t>
-  </si>
-  <si>
-    <t>Note 4 - Allowable US-GAAP Members on the ConsolidationItemsAxis</t>
   </si>
   <si>
     <t>CorporateReconcilingItemsAndEliminationsMember</t>
@@ -924,6 +921,18 @@
   <si>
     <t xml:space="preserve">CorporateReconcilingItemsAndEliminationsMember, CorporateAndReconcilingItemsMember, CorporateAndEliminationsMember, EliminationsAndReconcilingItemsMember, OperatingSegmentsAndCorporateNonSegmentMember, OperatingSegmentsExcludingIntersegmentEliminationMember
 </t>
+  </si>
+  <si>
+    <t>OperatingSegmentsExcludingIntersegmentEliminationMember</t>
+  </si>
+  <si>
+    <t>Operating Segments Excluding Intersegment Elimination [Member]</t>
+  </si>
+  <si>
+    <t>Represents the aggregate total of “Operating Segments” before intersegment eliminations.</t>
+  </si>
+  <si>
+    <t>Note 4 - Allowable extensions on the ConsolidationItemsAxis</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1220,6 +1229,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1517,11 +1528,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD991"/>
+  <dimension ref="A1:AD992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100:XFD100"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -1569,10 +1578,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L1" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -1774,7 +1783,7 @@
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L7" s="32"/>
     </row>
@@ -1806,7 +1815,7 @@
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L8" s="32"/>
       <c r="M8" s="10"/>
@@ -1907,7 +1916,7 @@
         <v>53</v>
       </c>
       <c r="K11" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L11" s="32"/>
     </row>
@@ -2058,14 +2067,14 @@
         <v>71</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L16" s="32"/>
     </row>
@@ -2094,10 +2103,10 @@
         <v>16</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K17" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L17" s="32"/>
     </row>
@@ -2214,14 +2223,14 @@
       </c>
       <c r="G21" s="30"/>
       <c r="H21" s="31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I21" s="29" t="s">
         <v>15</v>
       </c>
       <c r="J21" s="29"/>
       <c r="K21" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L21" s="32"/>
     </row>
@@ -2281,13 +2290,13 @@
       </c>
       <c r="J23" s="29"/>
       <c r="K23" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L23" s="32"/>
     </row>
     <row r="24" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A24" s="31" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B24" s="31" t="s">
         <v>11</v>
@@ -2296,10 +2305,10 @@
         <v>12</v>
       </c>
       <c r="D24" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="E24" s="31" t="s">
         <v>280</v>
-      </c>
-      <c r="E24" s="31" t="s">
-        <v>281</v>
       </c>
       <c r="F24" s="31" t="s">
         <v>25</v>
@@ -2335,7 +2344,7 @@
     </row>
     <row r="25" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A25" s="31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B25" s="31" t="s">
         <v>11</v>
@@ -2344,10 +2353,10 @@
         <v>12</v>
       </c>
       <c r="D25" s="31" t="s">
+        <v>282</v>
+      </c>
+      <c r="E25" s="31" t="s">
         <v>283</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>284</v>
       </c>
       <c r="F25" s="31" t="s">
         <v>25</v>
@@ -2385,19 +2394,19 @@
     </row>
     <row r="26" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A26" s="31" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B26" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="D26" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="E26" s="31" t="s">
         <v>287</v>
-      </c>
-      <c r="E26" s="31" t="s">
-        <v>288</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>25</v>
@@ -2435,19 +2444,19 @@
     </row>
     <row r="27" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A27" s="31" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B27" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D27" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="E27" s="31" t="s">
         <v>290</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>291</v>
       </c>
       <c r="F27" s="31" t="s">
         <v>25</v>
@@ -3541,10 +3550,10 @@
     </row>
     <row r="90" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A90" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="D90" s="21" t="s">
         <v>294</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>295</v>
       </c>
       <c r="E90" s="27" t="s">
         <v>12</v>
@@ -3555,12 +3564,12 @@
     </row>
     <row r="91" spans="1:30" s="24" customFormat="1" ht="12.75">
       <c r="A91" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B91" s="26"/>
       <c r="C91" s="26"/>
       <c r="D91" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E91" s="26" t="s">
         <v>12</v>
@@ -3598,7 +3607,7 @@
     </row>
     <row r="93" spans="1:30" s="11" customFormat="1" ht="16.5">
       <c r="A93" s="16" t="s">
-        <v>250</v>
+        <v>304</v>
       </c>
       <c r="K93" s="32"/>
       <c r="L93" s="32"/>
@@ -3645,18 +3654,18 @@
     </row>
     <row r="95" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A95" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
       <c r="D95" s="10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E95" s="10" t="s">
         <v>142</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G95" s="10"/>
       <c r="H95" s="10"/>
@@ -3685,18 +3694,18 @@
     </row>
     <row r="96" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A96" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>142</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G96" s="10"/>
       <c r="H96" s="10"/>
@@ -3725,18 +3734,18 @@
     </row>
     <row r="97" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A97" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
       <c r="D97" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E97" s="10" t="s">
         <v>142</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G97" s="10"/>
       <c r="H97" s="10"/>
@@ -3765,18 +3774,18 @@
     </row>
     <row r="98" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A98" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
       <c r="D98" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E98" s="10" t="s">
         <v>142</v>
       </c>
       <c r="F98" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G98" s="10"/>
       <c r="H98" s="10"/>
@@ -3805,18 +3814,18 @@
     </row>
     <row r="99" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A99" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
       <c r="D99" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E99" s="10" t="s">
         <v>142</v>
       </c>
       <c r="F99" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G99" s="10"/>
       <c r="H99" s="10"/>
@@ -3843,87 +3852,60 @@
       <c r="AC99" s="10"/>
       <c r="AD99" s="10"/>
     </row>
-    <row r="100" spans="1:30" s="11" customFormat="1" ht="12.75">
-      <c r="A100" s="10"/>
-      <c r="B100" s="10"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
-      <c r="E100" s="10"/>
-      <c r="F100" s="10"/>
-      <c r="G100" s="10"/>
-      <c r="H100" s="10"/>
-      <c r="I100" s="10"/>
-      <c r="J100" s="10"/>
-      <c r="K100" s="32"/>
-      <c r="L100" s="32"/>
-      <c r="M100" s="10"/>
-      <c r="N100" s="10"/>
-      <c r="O100" s="10"/>
-      <c r="P100" s="10"/>
-      <c r="Q100" s="10"/>
-      <c r="R100" s="10"/>
-      <c r="S100" s="10"/>
-      <c r="T100" s="10"/>
-      <c r="U100" s="10"/>
-      <c r="V100" s="10"/>
-      <c r="W100" s="10"/>
-      <c r="X100" s="10"/>
-      <c r="Y100" s="10"/>
-      <c r="Z100" s="10"/>
-      <c r="AA100" s="10"/>
-      <c r="AB100" s="10"/>
-      <c r="AC100" s="10"/>
-      <c r="AD100" s="10"/>
-    </row>
-    <row r="101" spans="1:30" s="11" customFormat="1" ht="16.5">
-      <c r="A101" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="B101" s="10"/>
-      <c r="C101" s="10"/>
-      <c r="D101" s="10"/>
-      <c r="E101" s="10"/>
-      <c r="F101" s="10"/>
-      <c r="G101" s="10"/>
-      <c r="H101" s="10"/>
-      <c r="I101" s="10"/>
-      <c r="J101" s="10"/>
+    <row r="100" spans="1:30" s="11" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A100" s="39" t="s">
+        <v>301</v>
+      </c>
+      <c r="B100" s="26"/>
+      <c r="C100" s="26"/>
+      <c r="D100" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="E100" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="F100" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="G100" s="26"/>
+      <c r="H100" s="26"/>
+      <c r="I100" s="26"/>
+      <c r="J100" s="26"/>
+      <c r="K100" s="26"/>
+      <c r="L100" s="26"/>
+      <c r="M100" s="26"/>
+      <c r="N100" s="26"/>
+      <c r="O100" s="26"/>
+      <c r="P100" s="26"/>
+      <c r="Q100" s="26"/>
+      <c r="R100" s="26"/>
+      <c r="S100" s="26"/>
+      <c r="T100" s="26"/>
+      <c r="U100" s="26"/>
+      <c r="V100" s="26"/>
+      <c r="W100" s="26"/>
+      <c r="X100" s="26"/>
+      <c r="Y100" s="26"/>
+      <c r="Z100" s="26"/>
+      <c r="AA100" s="26"/>
+      <c r="AB100" s="26"/>
+      <c r="AC100" s="26"/>
+      <c r="AD100" s="26"/>
+    </row>
+    <row r="101" spans="1:30" s="24" customFormat="1" ht="16.5">
+      <c r="A101" s="25"/>
       <c r="K101" s="32"/>
       <c r="L101" s="32"/>
-      <c r="M101" s="10"/>
-      <c r="N101" s="10"/>
-      <c r="O101" s="10"/>
-      <c r="P101" s="10"/>
-      <c r="Q101" s="10"/>
-      <c r="R101" s="10"/>
-      <c r="S101" s="10"/>
-      <c r="T101" s="10"/>
-      <c r="U101" s="10"/>
-      <c r="V101" s="10"/>
-      <c r="W101" s="10"/>
-      <c r="X101" s="10"/>
-      <c r="Y101" s="10"/>
-      <c r="Z101" s="10"/>
-      <c r="AA101" s="10"/>
-      <c r="AB101" s="10"/>
-      <c r="AC101" s="10"/>
-      <c r="AD101" s="10"/>
-    </row>
-    <row r="102" spans="1:30" s="11" customFormat="1" ht="12.75">
-      <c r="A102" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="B102" s="18"/>
-      <c r="C102" s="18"/>
-      <c r="D102" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E102" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F102" s="18" t="s">
-        <v>96</v>
-      </c>
+    </row>
+    <row r="102" spans="1:30" s="11" customFormat="1" ht="16.5">
+      <c r="A102" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B102" s="10"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="10"/>
+      <c r="E102" s="10"/>
+      <c r="F102" s="10"/>
       <c r="G102" s="10"/>
       <c r="H102" s="10"/>
       <c r="I102" s="10"/>
@@ -3950,94 +3932,130 @@
       <c r="AD102" s="10"/>
     </row>
     <row r="103" spans="1:30" s="11" customFormat="1" ht="12.75">
-      <c r="A103" s="21" t="s">
-        <v>267</v>
-      </c>
-      <c r="D103" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="E103" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F103" s="21" t="s">
-        <v>269</v>
-      </c>
+      <c r="A103" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E103" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F103" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G103" s="10"/>
+      <c r="H103" s="10"/>
+      <c r="I103" s="10"/>
+      <c r="J103" s="10"/>
       <c r="K103" s="32"/>
       <c r="L103" s="32"/>
+      <c r="M103" s="10"/>
+      <c r="N103" s="10"/>
+      <c r="O103" s="10"/>
+      <c r="P103" s="10"/>
+      <c r="Q103" s="10"/>
+      <c r="R103" s="10"/>
+      <c r="S103" s="10"/>
+      <c r="T103" s="10"/>
+      <c r="U103" s="10"/>
+      <c r="V103" s="10"/>
+      <c r="W103" s="10"/>
+      <c r="X103" s="10"/>
+      <c r="Y103" s="10"/>
+      <c r="Z103" s="10"/>
+      <c r="AA103" s="10"/>
+      <c r="AB103" s="10"/>
+      <c r="AC103" s="10"/>
+      <c r="AD103" s="10"/>
     </row>
     <row r="104" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A104" s="21" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D104" s="10" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E104" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F104" s="21" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="K104" s="32"/>
       <c r="L104" s="32"/>
     </row>
     <row r="105" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A105" s="21" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D105" s="10" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E105" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F105" s="21" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="K105" s="32"/>
       <c r="L105" s="32"/>
     </row>
     <row r="106" spans="1:30" s="11" customFormat="1" ht="12.75">
       <c r="A106" s="21" t="s">
-        <v>276</v>
-      </c>
-      <c r="D106" s="21" t="s">
-        <v>277</v>
+        <v>272</v>
+      </c>
+      <c r="D106" s="10" t="s">
+        <v>273</v>
       </c>
       <c r="E106" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="K106" s="32"/>
       <c r="L106" s="32"/>
     </row>
-    <row r="107" spans="1:30" s="11" customFormat="1" ht="15.75" customHeight="1">
+    <row r="107" spans="1:30" s="11" customFormat="1" ht="12.75">
+      <c r="A107" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="D107" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="E107" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F107" s="21" t="s">
+        <v>277</v>
+      </c>
       <c r="K107" s="32"/>
       <c r="L107" s="32"/>
     </row>
-    <row r="108" spans="1:30" s="11" customFormat="1" ht="16.5">
-      <c r="A108" s="16"/>
-      <c r="B108" s="10"/>
-      <c r="C108" s="10"/>
-      <c r="D108" s="10"/>
-      <c r="E108" s="10"/>
-      <c r="F108" s="10"/>
+    <row r="108" spans="1:30" s="11" customFormat="1" ht="15.75" customHeight="1">
       <c r="K108" s="32"/>
       <c r="L108" s="32"/>
     </row>
-    <row r="109" spans="1:30" s="1" customFormat="1" ht="12.75">
-      <c r="A109" s="2"/>
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
+    <row r="109" spans="1:30" s="11" customFormat="1" ht="16.5">
+      <c r="A109" s="16"/>
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="10"/>
       <c r="K109" s="32"/>
       <c r="L109" s="32"/>
     </row>
-    <row r="110" spans="1:30" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="110" spans="1:30" s="1" customFormat="1" ht="12.75">
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
       <c r="K110" s="32"/>
       <c r="L110" s="32"/>
     </row>
@@ -4045,7 +4063,7 @@
       <c r="K111" s="32"/>
       <c r="L111" s="32"/>
     </row>
-    <row r="112" spans="1:30" ht="15.75" customHeight="1">
+    <row r="112" spans="1:30" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="K112" s="32"/>
       <c r="L112" s="32"/>
     </row>
@@ -7564,6 +7582,10 @@
     <row r="991" spans="11:12" ht="15.75" customHeight="1">
       <c r="K991" s="32"/>
       <c r="L991" s="32"/>
+    </row>
+    <row r="992" spans="11:12" ht="15.75" customHeight="1">
+      <c r="K992" s="32"/>
+      <c r="L992" s="32"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1"/>

</xml_diff>

<commit_message>
Update dqc_0001 documentation for StatementEquityComponentsAxis changes
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -296,9 +296,6 @@
     <t>Equity Components [Axis]</t>
   </si>
   <si>
-    <t>Before 2018: WarrantsNotSettleableInCashMember, ContingentConsiderationClassifiedAsEquityMember, EquityIssuedInBusinessCombinationMember, TrustForBenefitOfEmployeesMember; Added For 2018: AccumulatedNetGainLossFromCashFlowHedgesIncludingPortionAttributableToNoncontrollingInterestMember, AccumulatedNetGainLossFromDesignatedOrQualifyingCashFlowHedgesMember, AccumulatedNetGainLossFromCashFlowHedgesAttributableToNoncontrollingInterestMember</t>
-  </si>
-  <si>
     <t>DQC_0001.76</t>
   </si>
   <si>
@@ -939,6 +936,9 @@
   </si>
   <si>
     <t>Trust created by the entity that exists for the benefit of its employees, such as pension and profit-sharing trusts that are managed by or under the trusteeship of the entity's management.</t>
+  </si>
+  <si>
+    <t>Removed for 2020: all except TrustForBenefitOfEmployeesMember; Removed for 2019: WarrantsNotSettleableInCashMember, ContingentConsiderationClassifiedAsEquityMember, EquityIssuedInBusinessCombinationMember; Added for 2019: AociGainLossDebtSecuritiesAvailableForSaleWithAllowanceForCreditLossParentMember, AociGainLossDebtSecuritiesAvailableForSaleWithAllowanceForCreditLossIncludingNoncontrollingInterestMember, AociGainLossDebtSecuritiesAvailableForSaleWithAllowanceForCreditLossNoncontrollingInterestMember, AociGainLossDebtSecuritiesAvailableForSaleWithoutAllowanceForCreditLossParentMember, AociGainLossDebtSecuritiesAvailableForSaleWithoutAllowanceForCreditLossNoncontrollingInterestMember, AociGainLossDebtSecuritiesAvailableForSaleWithoutAllowanceForCreditLossIncludingNoncontrollingInterestMember; Added For 2018: AccumulatedNetGainLossFromCashFlowHedgesIncludingPortionAttributableToNoncontrollingInterestMember, AccumulatedNetGainLossFromDesignatedOrQualifyingCashFlowHedgesMember, AccumulatedNetGainLossFromCashFlowHedgesAttributableToNoncontrollingInterestMember; Before 2018: WarrantsNotSettleableInCashMember, ContingentConsiderationClassifiedAsEquityMember, EquityIssuedInBusinessCombinationMember, TrustForBenefitOfEmployeesMember</t>
   </si>
 </sst>
 </file>
@@ -1416,9 +1416,7 @@
   </sheetPr>
   <dimension ref="A1:AD111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -2050,7 +2048,7 @@
         <v>17</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>93</v>
+        <v>307</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>17</v>
@@ -2061,7 +2059,7 @@
     </row>
     <row r="22" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A22" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>13</v>
@@ -2070,10 +2068,10 @@
         <v>14</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>17</v>
@@ -2087,7 +2085,7 @@
     </row>
     <row r="23" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A23" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>13</v>
@@ -2096,10 +2094,10 @@
         <v>38</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>17</v>
@@ -2113,7 +2111,7 @@
     </row>
     <row r="24" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A24" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>13</v>
@@ -2122,10 +2120,10 @@
         <v>14</v>
       </c>
       <c r="D24" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>102</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>27</v>
@@ -2139,7 +2137,7 @@
     </row>
     <row r="25" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A25" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>13</v>
@@ -2148,10 +2146,10 @@
         <v>14</v>
       </c>
       <c r="D25" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>27</v>
@@ -2168,19 +2166,19 @@
     </row>
     <row r="26" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A26" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>27</v>
@@ -2197,19 +2195,19 @@
     </row>
     <row r="27" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A27" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>27</v>
@@ -2223,7 +2221,7 @@
     </row>
     <row r="28" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A28" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>13</v>
@@ -2232,10 +2230,10 @@
         <v>14</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>115</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>17</v>
@@ -2299,7 +2297,7 @@
     </row>
     <row r="33" spans="1:30" s="20" customFormat="1" ht="16.5">
       <c r="A33" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
@@ -2333,7 +2331,7 @@
     </row>
     <row r="34" spans="1:30" s="5" customFormat="1" ht="15">
       <c r="A34" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -2344,214 +2342,214 @@
         <v>2</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A35" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="E35" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A36" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="E36" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A37" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="E37" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A38" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="E38" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A39" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="E39" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A40" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E40" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A41" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="E41" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A42" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="E42" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>141</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A43" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="E43" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A44" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="E44" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A45" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="E45" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A46" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="E46" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A47" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="E47" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A48" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="E48" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="8" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="50" spans="1:6" s="18" customFormat="1" ht="16.5">
       <c r="A50" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="5" customFormat="1" ht="15">
       <c r="A51" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -2562,150 +2560,150 @@
         <v>2</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A52" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
       <c r="D52" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="F52" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A53" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
       <c r="D53" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F53" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A54" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
       <c r="D54" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F54" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A55" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="E55" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F55" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A56" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D56" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="D56" s="22" t="s">
+      <c r="E56" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F56" s="22" t="s">
         <v>176</v>
-      </c>
-      <c r="E56" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F56" s="22" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A57" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D57" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="E57" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F57" s="22" t="s">
         <v>179</v>
-      </c>
-      <c r="E57" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F57" s="22" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A58" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D58" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="E58" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F58" s="22" t="s">
         <v>182</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F58" s="22" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A59" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="D59" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="E59" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F59" s="22" t="s">
         <v>185</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F59" s="22" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A60" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D60" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="E60" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F60" s="22" t="s">
         <v>188</v>
-      </c>
-      <c r="E60" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F60" s="22" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="8" customFormat="1" ht="12"/>
     <row r="62" spans="1:6" s="18" customFormat="1" ht="16.5">
       <c r="A62" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="5" customFormat="1" ht="15">
       <c r="A63" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -2716,393 +2714,393 @@
         <v>2</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A64" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D64" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="E64" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" s="8" t="s">
         <v>192</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A65" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D65" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="E65" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" s="8" t="s">
         <v>195</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A66" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D66" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="E66" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="8" t="s">
         <v>198</v>
-      </c>
-      <c r="E66" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A67" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D67" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="E67" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="8" t="s">
         <v>201</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A68" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D68" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="D68" s="8" t="s">
+      <c r="E68" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" s="8" t="s">
         <v>204</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A69" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D69" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="E69" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A70" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D70" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="E70" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" s="8" t="s">
         <v>210</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F70" s="8" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A71" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D71" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="E71" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="8" t="s">
         <v>213</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F71" s="8" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A72" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D72" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="E72" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="E72" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F72" s="8" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A73" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D73" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="E73" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F73" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="E73" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A74" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="D74" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="E74" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="E74" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F74" s="8" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A75" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D75" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="E75" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F75" s="8" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A76" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D76" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="E76" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" s="8" t="s">
         <v>228</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F76" s="8" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A77" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="D77" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="E77" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F77" s="8" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A78" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="D78" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="E78" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" s="8" t="s">
         <v>234</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A79" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D79" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="D79" s="8" t="s">
+      <c r="E79" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" s="8" t="s">
         <v>237</v>
-      </c>
-      <c r="E79" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F79" s="8" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A80" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D80" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="E80" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F80" s="8" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A81" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D81" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="E81" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="E81" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F81" s="8" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A82" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D82" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="E82" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="8" t="s">
         <v>246</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F82" s="8" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A83" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D83" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="E83" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" s="8" t="s">
         <v>249</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A84" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D84" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="D84" s="8" t="s">
+      <c r="E84" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="8" t="s">
         <v>252</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F84" s="8" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A85" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="D85" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="D85" s="8" t="s">
+      <c r="E85" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="8" t="s">
         <v>255</v>
-      </c>
-      <c r="E85" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F85" s="8" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A86" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D86" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="D86" s="8" t="s">
+      <c r="E86" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="8" t="s">
         <v>258</v>
-      </c>
-      <c r="E86" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A87" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="D87" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="D87" s="22" t="s">
+      <c r="E87" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F87" s="22" t="s">
         <v>261</v>
-      </c>
-      <c r="E87" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F87" s="22" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A88" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="D88" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="D88" s="22" t="s">
+      <c r="E88" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88" s="22" t="s">
         <v>264</v>
-      </c>
-      <c r="E88" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F88" s="22" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A89" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="D89" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="D89" s="22" t="s">
+      <c r="E89" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F89" s="22" t="s">
         <v>267</v>
-      </c>
-      <c r="E89" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F89" s="22" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="90" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A90" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="D90" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="D90" s="22" t="s">
+      <c r="E90" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F90" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="E90" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F90" s="22" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A91" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="D91" s="22" t="s">
         <v>272</v>
-      </c>
-      <c r="D91" s="22" t="s">
-        <v>273</v>
       </c>
       <c r="E91" s="22" t="s">
         <v>14</v>
@@ -3110,10 +3108,10 @@
     </row>
     <row r="92" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A92" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D92" s="8" t="s">
         <v>274</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>275</v>
       </c>
       <c r="E92" s="22" t="s">
         <v>14</v>
@@ -3122,12 +3120,12 @@
     <row r="93" spans="1:6" s="8" customFormat="1" ht="12"/>
     <row r="94" spans="1:6" s="18" customFormat="1" ht="16.5">
       <c r="A94" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="95" spans="1:6" s="5" customFormat="1" ht="15">
       <c r="A95" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B95" s="17"/>
       <c r="C95" s="17"/>
@@ -3138,102 +3136,102 @@
         <v>2</v>
       </c>
       <c r="F95" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="96" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A96" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D96" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="D96" s="8" t="s">
+      <c r="E96" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F96" s="8" t="s">
         <v>278</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F96" s="8" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A97" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D97" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="D97" s="8" t="s">
+      <c r="E97" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F97" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F97" s="8" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A98" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="D98" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="D98" s="8" t="s">
+      <c r="E98" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F98" s="8" t="s">
         <v>284</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F98" s="8" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="99" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A99" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D99" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="D99" s="8" t="s">
+      <c r="E99" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F99" s="8" t="s">
         <v>287</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F99" s="8" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="100" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A100" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D100" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="D100" s="8" t="s">
+      <c r="E100" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F100" s="8" t="s">
         <v>290</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F100" s="8" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="101" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A101" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="D101" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="D101" s="8" t="s">
+      <c r="E101" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F101" s="8" t="s">
         <v>293</v>
-      </c>
-      <c r="E101" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F101" s="8" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="102" spans="1:6" s="8" customFormat="1" ht="12"/>
     <row r="103" spans="1:6" s="18" customFormat="1" ht="16.5">
       <c r="A103" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="104" spans="1:6" s="5" customFormat="1" ht="15">
       <c r="A104" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B104" s="17"/>
       <c r="C104" s="17"/>
@@ -3244,63 +3242,63 @@
         <v>2</v>
       </c>
       <c r="F104" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="105" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A105" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="D105" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="D105" s="8" t="s">
+      <c r="E105" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F105" s="22" t="s">
         <v>297</v>
-      </c>
-      <c r="E105" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F105" s="22" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A106" s="22" t="s">
+        <v>298</v>
+      </c>
+      <c r="D106" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="D106" s="8" t="s">
+      <c r="E106" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F106" s="22" t="s">
         <v>300</v>
-      </c>
-      <c r="E106" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F106" s="22" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="107" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A107" s="22" t="s">
+        <v>301</v>
+      </c>
+      <c r="D107" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="D107" s="8" t="s">
+      <c r="E107" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F107" s="22" t="s">
         <v>303</v>
-      </c>
-      <c r="E107" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F107" s="22" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="108" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A108" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="D108" s="22" t="s">
         <v>305</v>
       </c>
-      <c r="D108" s="22" t="s">
+      <c r="E108" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" s="22" t="s">
         <v>306</v>
-      </c>
-      <c r="E108" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F108" s="22" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="16.5">

</xml_diff>

<commit_message>
Update xule for multi-inline filing processing (#477)
* Update dqc_0001 documentation for StatementEquityComponentsAxis changes

* Update xule multi-inline filings

* Update .gitignore for vscode
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
+++ b/docs/DQC_US_0001/DQC_0001_ListOfAxes.xlsx
@@ -296,9 +296,6 @@
     <t>Equity Components [Axis]</t>
   </si>
   <si>
-    <t>Before 2018: WarrantsNotSettleableInCashMember, ContingentConsiderationClassifiedAsEquityMember, EquityIssuedInBusinessCombinationMember, TrustForBenefitOfEmployeesMember; Added For 2018: AccumulatedNetGainLossFromCashFlowHedgesIncludingPortionAttributableToNoncontrollingInterestMember, AccumulatedNetGainLossFromDesignatedOrQualifyingCashFlowHedgesMember, AccumulatedNetGainLossFromCashFlowHedgesAttributableToNoncontrollingInterestMember</t>
-  </si>
-  <si>
     <t>DQC_0001.76</t>
   </si>
   <si>
@@ -939,6 +936,9 @@
   </si>
   <si>
     <t>Trust created by the entity that exists for the benefit of its employees, such as pension and profit-sharing trusts that are managed by or under the trusteeship of the entity's management.</t>
+  </si>
+  <si>
+    <t>Removed for 2020: all except TrustForBenefitOfEmployeesMember; Removed for 2019: WarrantsNotSettleableInCashMember, ContingentConsiderationClassifiedAsEquityMember, EquityIssuedInBusinessCombinationMember; Added for 2019: AociGainLossDebtSecuritiesAvailableForSaleWithAllowanceForCreditLossParentMember, AociGainLossDebtSecuritiesAvailableForSaleWithAllowanceForCreditLossIncludingNoncontrollingInterestMember, AociGainLossDebtSecuritiesAvailableForSaleWithAllowanceForCreditLossNoncontrollingInterestMember, AociGainLossDebtSecuritiesAvailableForSaleWithoutAllowanceForCreditLossParentMember, AociGainLossDebtSecuritiesAvailableForSaleWithoutAllowanceForCreditLossNoncontrollingInterestMember, AociGainLossDebtSecuritiesAvailableForSaleWithoutAllowanceForCreditLossIncludingNoncontrollingInterestMember; Added For 2018: AccumulatedNetGainLossFromCashFlowHedgesIncludingPortionAttributableToNoncontrollingInterestMember, AccumulatedNetGainLossFromDesignatedOrQualifyingCashFlowHedgesMember, AccumulatedNetGainLossFromCashFlowHedgesAttributableToNoncontrollingInterestMember; Before 2018: WarrantsNotSettleableInCashMember, ContingentConsiderationClassifiedAsEquityMember, EquityIssuedInBusinessCombinationMember, TrustForBenefitOfEmployeesMember</t>
   </si>
 </sst>
 </file>
@@ -1416,9 +1416,7 @@
   </sheetPr>
   <dimension ref="A1:AD111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -2050,7 +2048,7 @@
         <v>17</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>93</v>
+        <v>307</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>17</v>
@@ -2061,7 +2059,7 @@
     </row>
     <row r="22" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A22" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>13</v>
@@ -2070,10 +2068,10 @@
         <v>14</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>17</v>
@@ -2087,7 +2085,7 @@
     </row>
     <row r="23" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A23" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>13</v>
@@ -2096,10 +2094,10 @@
         <v>38</v>
       </c>
       <c r="D23" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>17</v>
@@ -2113,7 +2111,7 @@
     </row>
     <row r="24" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A24" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>13</v>
@@ -2122,10 +2120,10 @@
         <v>14</v>
       </c>
       <c r="D24" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>102</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>27</v>
@@ -2139,7 +2137,7 @@
     </row>
     <row r="25" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A25" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>13</v>
@@ -2148,10 +2146,10 @@
         <v>14</v>
       </c>
       <c r="D25" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>27</v>
@@ -2168,19 +2166,19 @@
     </row>
     <row r="26" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A26" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>27</v>
@@ -2197,19 +2195,19 @@
     </row>
     <row r="27" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A27" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>27</v>
@@ -2223,7 +2221,7 @@
     </row>
     <row r="28" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A28" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>13</v>
@@ -2232,10 +2230,10 @@
         <v>14</v>
       </c>
       <c r="D28" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>115</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>17</v>
@@ -2299,7 +2297,7 @@
     </row>
     <row r="33" spans="1:30" s="20" customFormat="1" ht="16.5">
       <c r="A33" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
@@ -2333,7 +2331,7 @@
     </row>
     <row r="34" spans="1:30" s="5" customFormat="1" ht="15">
       <c r="A34" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -2344,214 +2342,214 @@
         <v>2</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A35" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="E35" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A36" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="E36" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A37" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="E37" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A38" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="E38" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A39" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="E39" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A40" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E40" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A41" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="E41" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A42" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="E42" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>141</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A43" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="E43" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A44" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="E44" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A45" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="E45" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A46" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="E46" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A47" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="E47" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:30" s="8" customFormat="1" ht="12">
       <c r="A48" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="E48" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="8" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="50" spans="1:6" s="18" customFormat="1" ht="16.5">
       <c r="A50" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="5" customFormat="1" ht="15">
       <c r="A51" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -2562,150 +2560,150 @@
         <v>2</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A52" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
       <c r="D52" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="F52" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A53" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
       <c r="D53" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F53" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A54" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
       <c r="D54" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F54" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A55" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="E55" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F55" s="8" t="s">
         <v>173</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A56" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D56" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="D56" s="22" t="s">
+      <c r="E56" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F56" s="22" t="s">
         <v>176</v>
-      </c>
-      <c r="E56" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F56" s="22" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A57" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="D57" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="E57" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F57" s="22" t="s">
         <v>179</v>
-      </c>
-      <c r="E57" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F57" s="22" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A58" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D58" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="D58" s="22" t="s">
+      <c r="E58" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F58" s="22" t="s">
         <v>182</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F58" s="22" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A59" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="D59" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="E59" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F59" s="22" t="s">
         <v>185</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F59" s="22" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A60" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D60" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="E60" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F60" s="22" t="s">
         <v>188</v>
-      </c>
-      <c r="E60" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F60" s="22" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="8" customFormat="1" ht="12"/>
     <row r="62" spans="1:6" s="18" customFormat="1" ht="16.5">
       <c r="A62" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="5" customFormat="1" ht="15">
       <c r="A63" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -2716,393 +2714,393 @@
         <v>2</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A64" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D64" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="E64" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" s="8" t="s">
         <v>192</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A65" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D65" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="E65" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" s="8" t="s">
         <v>195</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="66" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A66" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D66" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="E66" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="8" t="s">
         <v>198</v>
-      </c>
-      <c r="E66" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A67" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D67" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="D67" s="8" t="s">
+      <c r="E67" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="8" t="s">
         <v>201</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A68" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D68" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="D68" s="8" t="s">
+      <c r="E68" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" s="8" t="s">
         <v>204</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A69" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D69" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="E69" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="70" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A70" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D70" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="D70" s="8" t="s">
+      <c r="E70" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" s="8" t="s">
         <v>210</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F70" s="8" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A71" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D71" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="E71" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="8" t="s">
         <v>213</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F71" s="8" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A72" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D72" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="E72" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="E72" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F72" s="8" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A73" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D73" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="E73" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F73" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="E73" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="74" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A74" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="D74" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="D74" s="8" t="s">
+      <c r="E74" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="E74" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F74" s="8" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A75" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D75" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="D75" s="8" t="s">
+      <c r="E75" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F75" s="8" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="76" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A76" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D76" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="E76" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" s="8" t="s">
         <v>228</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F76" s="8" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="77" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A77" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="D77" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="D77" s="8" t="s">
+      <c r="E77" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F77" s="8" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A78" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="D78" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="D78" s="8" t="s">
+      <c r="E78" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" s="8" t="s">
         <v>234</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="79" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A79" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D79" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="D79" s="8" t="s">
+      <c r="E79" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" s="8" t="s">
         <v>237</v>
-      </c>
-      <c r="E79" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F79" s="8" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="80" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A80" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D80" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="E80" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F80" s="8" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A81" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D81" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="D81" s="8" t="s">
+      <c r="E81" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="E81" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F81" s="8" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A82" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D82" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="D82" s="8" t="s">
+      <c r="E82" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="8" t="s">
         <v>246</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F82" s="8" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A83" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D83" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="E83" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" s="8" t="s">
         <v>249</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="84" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A84" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D84" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="D84" s="8" t="s">
+      <c r="E84" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="8" t="s">
         <v>252</v>
-      </c>
-      <c r="E84" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F84" s="8" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A85" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="D85" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="D85" s="8" t="s">
+      <c r="E85" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="8" t="s">
         <v>255</v>
-      </c>
-      <c r="E85" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F85" s="8" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="86" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A86" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D86" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="D86" s="8" t="s">
+      <c r="E86" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="8" t="s">
         <v>258</v>
-      </c>
-      <c r="E86" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A87" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="D87" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="D87" s="22" t="s">
+      <c r="E87" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F87" s="22" t="s">
         <v>261</v>
-      </c>
-      <c r="E87" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F87" s="22" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="88" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A88" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="D88" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="D88" s="22" t="s">
+      <c r="E88" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88" s="22" t="s">
         <v>264</v>
-      </c>
-      <c r="E88" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F88" s="22" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="89" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A89" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="D89" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="D89" s="22" t="s">
+      <c r="E89" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F89" s="22" t="s">
         <v>267</v>
-      </c>
-      <c r="E89" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F89" s="22" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="90" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A90" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="D90" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="D90" s="22" t="s">
+      <c r="E90" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F90" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="E90" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F90" s="22" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="91" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A91" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="D91" s="22" t="s">
         <v>272</v>
-      </c>
-      <c r="D91" s="22" t="s">
-        <v>273</v>
       </c>
       <c r="E91" s="22" t="s">
         <v>14</v>
@@ -3110,10 +3108,10 @@
     </row>
     <row r="92" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A92" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D92" s="8" t="s">
         <v>274</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>275</v>
       </c>
       <c r="E92" s="22" t="s">
         <v>14</v>
@@ -3122,12 +3120,12 @@
     <row r="93" spans="1:6" s="8" customFormat="1" ht="12"/>
     <row r="94" spans="1:6" s="18" customFormat="1" ht="16.5">
       <c r="A94" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="95" spans="1:6" s="5" customFormat="1" ht="15">
       <c r="A95" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B95" s="17"/>
       <c r="C95" s="17"/>
@@ -3138,102 +3136,102 @@
         <v>2</v>
       </c>
       <c r="F95" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="96" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A96" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D96" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="D96" s="8" t="s">
+      <c r="E96" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F96" s="8" t="s">
         <v>278</v>
-      </c>
-      <c r="E96" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F96" s="8" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A97" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D97" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="D97" s="8" t="s">
+      <c r="E97" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F97" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="E97" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F97" s="8" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="98" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A98" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="D98" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="D98" s="8" t="s">
+      <c r="E98" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F98" s="8" t="s">
         <v>284</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F98" s="8" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="99" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A99" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D99" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="D99" s="8" t="s">
+      <c r="E99" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F99" s="8" t="s">
         <v>287</v>
-      </c>
-      <c r="E99" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F99" s="8" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="100" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A100" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D100" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="D100" s="8" t="s">
+      <c r="E100" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F100" s="8" t="s">
         <v>290</v>
-      </c>
-      <c r="E100" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F100" s="8" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="101" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A101" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="D101" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="D101" s="8" t="s">
+      <c r="E101" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F101" s="8" t="s">
         <v>293</v>
-      </c>
-      <c r="E101" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F101" s="8" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="102" spans="1:6" s="8" customFormat="1" ht="12"/>
     <row r="103" spans="1:6" s="18" customFormat="1" ht="16.5">
       <c r="A103" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="104" spans="1:6" s="5" customFormat="1" ht="15">
       <c r="A104" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B104" s="17"/>
       <c r="C104" s="17"/>
@@ -3244,63 +3242,63 @@
         <v>2</v>
       </c>
       <c r="F104" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="105" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A105" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="D105" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="D105" s="8" t="s">
+      <c r="E105" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F105" s="22" t="s">
         <v>297</v>
-      </c>
-      <c r="E105" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F105" s="22" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A106" s="22" t="s">
+        <v>298</v>
+      </c>
+      <c r="D106" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="D106" s="8" t="s">
+      <c r="E106" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F106" s="22" t="s">
         <v>300</v>
-      </c>
-      <c r="E106" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F106" s="22" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="107" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A107" s="22" t="s">
+        <v>301</v>
+      </c>
+      <c r="D107" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="D107" s="8" t="s">
+      <c r="E107" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F107" s="22" t="s">
         <v>303</v>
-      </c>
-      <c r="E107" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F107" s="22" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="108" spans="1:6" s="8" customFormat="1" ht="12">
       <c r="A108" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="D108" s="22" t="s">
         <v>305</v>
       </c>
-      <c r="D108" s="22" t="s">
+      <c r="E108" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" s="22" t="s">
         <v>306</v>
-      </c>
-      <c r="E108" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F108" s="22" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="16.5">

</xml_diff>